<commit_message>
Changes to asset model loader
</commit_message>
<xml_diff>
--- a/data/inputs/Asset Model - Demo.xlsx
+++ b/data/inputs/Asset Model - Demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtreseder\OneDrive - KPMG\Documents\3. Client\Essential Energy\Probability of Failure Model\pof\data\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1280" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{C1C2E50E-1E74-411E-9EEE-558607B14A1C}"/>
+  <xr:revisionPtr revIDLastSave="1295" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{DDC26A5F-EB1F-4CE9-904B-45CFD087DA60}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="315">
   <si>
     <t>component</t>
   </si>
@@ -987,6 +987,9 @@
   </si>
   <si>
     <t>upper</t>
+  </si>
+  <si>
+    <t>replacement_failed</t>
   </si>
 </sst>
 </file>
@@ -1353,7 +1356,28 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{FE42BDC6-EBD5-43A7-A342-17D1DCC45724}"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2243,7 +2267,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="O13:O15 O17:O18">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2711,10 +2735,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA0734F-FFBE-4DAF-BDE5-A12359370A0D}">
-  <dimension ref="A1:BB33"/>
+  <dimension ref="A1:BB35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AN25" sqref="AN25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3149,7 +3173,9 @@
       <c r="AR5" s="18"/>
       <c r="AS5" s="50"/>
       <c r="AT5" s="18"/>
-      <c r="AU5" s="18"/>
+      <c r="AU5" s="18" t="b">
+        <v>1</v>
+      </c>
       <c r="AV5" s="18"/>
       <c r="AW5" s="50"/>
       <c r="AX5" s="18"/>
@@ -3282,10 +3308,18 @@
         <v>0</v>
       </c>
       <c r="AW7" s="50"/>
-      <c r="AX7" s="18"/>
-      <c r="AY7" s="18"/>
-      <c r="AZ7" s="18"/>
-      <c r="BA7" s="18"/>
+      <c r="AX7" s="18" t="s">
+        <v>291</v>
+      </c>
+      <c r="AY7" s="18">
+        <v>0</v>
+      </c>
+      <c r="AZ7" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="BA7" s="18" t="s">
+        <v>20</v>
+      </c>
       <c r="BB7" s="47"/>
     </row>
     <row r="8" spans="1:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -3518,205 +3552,216 @@
       <c r="AW14" s="50"/>
       <c r="BB14" s="47"/>
     </row>
-    <row r="15" spans="1:54" s="56" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
+      <c r="E15" s="56"/>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
       <c r="I15" s="15"/>
-      <c r="AI15" s="57"/>
-      <c r="AJ15" s="57"/>
-      <c r="AK15" s="57"/>
-      <c r="AL15" s="57"/>
-      <c r="AM15" s="57"/>
-      <c r="AN15" s="57"/>
-      <c r="AO15" s="57"/>
-      <c r="AQ15" s="58"/>
-      <c r="AR15" s="58"/>
-      <c r="AS15" s="58"/>
-      <c r="AT15" s="57"/>
-      <c r="AU15" s="57"/>
-      <c r="AV15" s="57"/>
-      <c r="AW15" s="57"/>
+      <c r="J15" s="56"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="56"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="56"/>
+      <c r="AI15" s="50"/>
+      <c r="AJ15" s="50"/>
+      <c r="AK15" s="50"/>
+      <c r="AL15" s="50"/>
+      <c r="AM15" s="50"/>
+      <c r="AN15" s="50"/>
+      <c r="AO15" s="50"/>
+      <c r="AQ15" s="53"/>
+      <c r="AR15" s="53"/>
+      <c r="AS15" s="53"/>
+      <c r="AT15" s="50"/>
+      <c r="AU15" s="50"/>
+      <c r="AV15" s="50"/>
+      <c r="AW15" s="50"/>
     </row>
     <row r="16" spans="1:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E16" s="56"/>
       <c r="J16" s="56"/>
-      <c r="K16" s="15" t="s">
-        <v>82</v>
-      </c>
       <c r="R16" s="56"/>
       <c r="T16" s="56"/>
       <c r="U16" s="15" t="s">
-        <v>71</v>
+        <v>314</v>
       </c>
       <c r="V16" s="15">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="W16" s="15">
-        <v>50</v>
+        <v>7000</v>
       </c>
       <c r="X16" s="15" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="Y16" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="Z16" s="15" t="s">
-        <v>310</v>
-      </c>
-      <c r="AB16" s="15">
+        <v>311</v>
+      </c>
+      <c r="AA16" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="AD16" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="50"/>
+      <c r="AJ16" s="16"/>
+      <c r="AK16" s="16"/>
+      <c r="AL16" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM16" s="16"/>
+      <c r="AN16" s="16"/>
+      <c r="AO16" s="50"/>
+      <c r="AQ16" s="19"/>
+      <c r="AR16" s="19"/>
+      <c r="AS16" s="53"/>
+      <c r="AT16" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AU16" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV16" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW16" s="50"/>
+      <c r="AX16" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="AY16" s="15">
+        <v>1</v>
+      </c>
+      <c r="AZ16" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="BA16" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="AC16" s="15">
-        <v>5</v>
-      </c>
-      <c r="AE16" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="AF16" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="AG16" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="AH16" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="AI16" s="50"/>
-      <c r="AJ16" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="AK16" s="18"/>
-      <c r="AL16" s="18"/>
-      <c r="AM16" s="18"/>
-      <c r="AN16" s="18"/>
-      <c r="AO16" s="50"/>
-      <c r="AQ16" s="18"/>
-      <c r="AR16" s="18"/>
-      <c r="AS16" s="50"/>
-      <c r="AT16" s="16"/>
-      <c r="AU16" s="18"/>
-      <c r="AV16" s="18"/>
-      <c r="AW16" s="50"/>
-      <c r="AX16" s="18"/>
-      <c r="AY16" s="18"/>
-      <c r="AZ16" s="18"/>
-      <c r="BA16" s="18"/>
       <c r="BB16" s="47"/>
     </row>
-    <row r="17" spans="3:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E17" s="56"/>
-      <c r="J17" s="56"/>
-      <c r="R17" s="56"/>
-      <c r="T17" s="56"/>
-      <c r="U17" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="V17" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="W17" s="15">
-        <v>100</v>
-      </c>
-      <c r="X17" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y17" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z17" s="15" t="s">
-        <v>311</v>
-      </c>
-      <c r="AI17" s="50"/>
-      <c r="AJ17" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="AK17" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="AL17" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM17" s="16"/>
-      <c r="AN17" s="16"/>
-      <c r="AO17" s="50"/>
-      <c r="AP17" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="AQ17" s="19">
-        <v>50</v>
-      </c>
-      <c r="AR17" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="AS17" s="53"/>
-      <c r="AT17" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="AU17" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="AV17" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="AW17" s="50"/>
-      <c r="AX17" s="18"/>
-      <c r="AY17" s="18"/>
-      <c r="AZ17" s="18"/>
-      <c r="BA17" s="18"/>
-      <c r="BB17" s="47"/>
-    </row>
-    <row r="18" spans="3:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:54" s="56" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="AI17" s="57"/>
+      <c r="AJ17" s="57"/>
+      <c r="AK17" s="57"/>
+      <c r="AL17" s="57"/>
+      <c r="AM17" s="57"/>
+      <c r="AN17" s="57"/>
+      <c r="AO17" s="57"/>
+      <c r="AQ17" s="58"/>
+      <c r="AR17" s="58"/>
+      <c r="AS17" s="58"/>
+      <c r="AT17" s="57"/>
+      <c r="AU17" s="57"/>
+      <c r="AV17" s="57"/>
+      <c r="AW17" s="57"/>
+    </row>
+    <row r="18" spans="1:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E18" s="56"/>
       <c r="J18" s="56"/>
+      <c r="K18" s="15" t="s">
+        <v>82</v>
+      </c>
       <c r="R18" s="56"/>
       <c r="T18" s="56"/>
+      <c r="U18" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="V18" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="W18" s="15">
+        <v>50</v>
+      </c>
+      <c r="X18" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y18" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z18" s="15" t="s">
+        <v>310</v>
+      </c>
+      <c r="AB18" s="15">
+        <v>20</v>
+      </c>
+      <c r="AC18" s="15">
+        <v>5</v>
+      </c>
+      <c r="AE18" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF18" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG18" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH18" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="AI18" s="50"/>
-      <c r="AJ18" s="16"/>
-      <c r="AK18" s="16"/>
-      <c r="AL18" s="16"/>
-      <c r="AM18" s="16"/>
-      <c r="AN18" s="16"/>
+      <c r="AJ18" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK18" s="18"/>
+      <c r="AL18" s="18"/>
+      <c r="AM18" s="18"/>
+      <c r="AN18" s="18"/>
       <c r="AO18" s="50"/>
-      <c r="AP18" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="AQ18" s="19">
-        <v>50</v>
-      </c>
-      <c r="AR18" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="AS18" s="53"/>
+      <c r="AQ18" s="18"/>
+      <c r="AR18" s="18"/>
+      <c r="AS18" s="50"/>
       <c r="AT18" s="16"/>
-      <c r="AU18" s="16"/>
-      <c r="AV18" s="16"/>
+      <c r="AU18" s="18"/>
+      <c r="AV18" s="18"/>
       <c r="AW18" s="50"/>
+      <c r="AX18" s="18"/>
+      <c r="AY18" s="18"/>
+      <c r="AZ18" s="18"/>
+      <c r="BA18" s="18"/>
       <c r="BB18" s="47"/>
     </row>
-    <row r="19" spans="3:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E19" s="56"/>
       <c r="J19" s="56"/>
       <c r="R19" s="56"/>
       <c r="T19" s="56"/>
       <c r="U19" s="15" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="V19" s="15">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="W19" s="15">
-        <v>3500</v>
+        <v>100</v>
       </c>
       <c r="X19" s="15" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="Y19" s="15" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="Z19" s="15" t="s">
         <v>311</v>
@@ -3738,10 +3783,10 @@
         <v>21</v>
       </c>
       <c r="AQ19" s="19">
-        <v>0</v>
-      </c>
-      <c r="AR19" s="19">
         <v>50</v>
+      </c>
+      <c r="AR19" s="19" t="s">
+        <v>79</v>
       </c>
       <c r="AS19" s="53"/>
       <c r="AT19" s="16" t="b">
@@ -3754,23 +3799,32 @@
         <v>0</v>
       </c>
       <c r="AW19" s="50"/>
+      <c r="AX19" s="18"/>
+      <c r="AY19" s="18"/>
+      <c r="AZ19" s="18"/>
+      <c r="BA19" s="18"/>
       <c r="BB19" s="47"/>
     </row>
-    <row r="20" spans="3:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E20" s="56"/>
       <c r="J20" s="56"/>
       <c r="R20" s="56"/>
       <c r="T20" s="56"/>
-      <c r="AI20" s="47"/>
-      <c r="AO20" s="47"/>
+      <c r="AI20" s="50"/>
+      <c r="AJ20" s="16"/>
+      <c r="AK20" s="16"/>
+      <c r="AL20" s="16"/>
+      <c r="AM20" s="16"/>
+      <c r="AN20" s="16"/>
+      <c r="AO20" s="50"/>
       <c r="AP20" s="15" t="s">
         <v>45</v>
       </c>
       <c r="AQ20" s="19">
-        <v>0</v>
-      </c>
-      <c r="AR20" s="19">
         <v>50</v>
+      </c>
+      <c r="AR20" s="19" t="s">
+        <v>79</v>
       </c>
       <c r="AS20" s="53"/>
       <c r="AT20" s="16"/>
@@ -3779,216 +3833,198 @@
       <c r="AW20" s="50"/>
       <c r="BB20" s="47"/>
     </row>
-    <row r="21" spans="3:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21" s="60"/>
-      <c r="F21"/>
-      <c r="G21"/>
-      <c r="H21"/>
-      <c r="I21"/>
-      <c r="J21" s="60"/>
-      <c r="K21"/>
-      <c r="L21"/>
-      <c r="M21"/>
-      <c r="N21"/>
-      <c r="O21"/>
-      <c r="P21"/>
-      <c r="Q21"/>
-      <c r="R21" s="60"/>
-      <c r="S21"/>
-      <c r="T21" s="60"/>
-      <c r="U21"/>
-      <c r="V21"/>
-      <c r="W21"/>
-      <c r="X21"/>
-      <c r="Y21"/>
-      <c r="Z21"/>
-      <c r="AA21"/>
-      <c r="AB21"/>
-      <c r="AC21"/>
-      <c r="AD21"/>
-      <c r="AE21"/>
-      <c r="AF21"/>
-      <c r="AG21"/>
-      <c r="AH21"/>
-      <c r="AI21" s="51"/>
-      <c r="AJ21" s="17"/>
-      <c r="AK21" s="17"/>
-      <c r="AL21" s="17"/>
-      <c r="AM21" s="17"/>
-      <c r="AN21" s="17"/>
-      <c r="AO21" s="51"/>
+    <row r="21" spans="1:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="56"/>
+      <c r="J21" s="56"/>
+      <c r="R21" s="56"/>
+      <c r="T21" s="56"/>
+      <c r="U21" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="V21" s="15">
+        <v>1</v>
+      </c>
+      <c r="W21" s="15">
+        <v>3500</v>
+      </c>
+      <c r="X21" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y21" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z21" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="AI21" s="50"/>
+      <c r="AJ21" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK21" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL21" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM21" s="16"/>
+      <c r="AN21" s="16"/>
+      <c r="AO21" s="50"/>
       <c r="AP21" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="AQ21" s="19">
+        <v>0</v>
+      </c>
+      <c r="AR21" s="19">
+        <v>50</v>
+      </c>
+      <c r="AS21" s="53"/>
+      <c r="AT21" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AU21" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV21" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW21" s="50"/>
+      <c r="BB21" s="47"/>
+    </row>
+    <row r="22" spans="1:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E22" s="56"/>
+      <c r="J22" s="56"/>
+      <c r="R22" s="56"/>
+      <c r="T22" s="56"/>
+      <c r="AI22" s="47"/>
+      <c r="AO22" s="47"/>
+      <c r="AP22" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="AQ22" s="19">
+        <v>0</v>
+      </c>
+      <c r="AR22" s="19">
+        <v>50</v>
+      </c>
+      <c r="AS22" s="53"/>
+      <c r="AT22" s="16"/>
+      <c r="AU22" s="16"/>
+      <c r="AV22" s="16"/>
+      <c r="AW22" s="50"/>
+      <c r="BB22" s="47"/>
+    </row>
+    <row r="23" spans="1:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23" s="60"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23" s="60"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+      <c r="P23"/>
+      <c r="Q23"/>
+      <c r="R23" s="60"/>
+      <c r="S23"/>
+      <c r="T23" s="60"/>
+      <c r="U23"/>
+      <c r="V23"/>
+      <c r="W23"/>
+      <c r="X23"/>
+      <c r="Y23"/>
+      <c r="Z23"/>
+      <c r="AA23"/>
+      <c r="AB23"/>
+      <c r="AC23"/>
+      <c r="AD23"/>
+      <c r="AE23"/>
+      <c r="AF23"/>
+      <c r="AG23"/>
+      <c r="AH23"/>
+      <c r="AI23" s="51"/>
+      <c r="AJ23" s="17"/>
+      <c r="AK23" s="17"/>
+      <c r="AL23" s="17"/>
+      <c r="AM23" s="17"/>
+      <c r="AN23" s="17"/>
+      <c r="AO23" s="51"/>
+      <c r="AP23" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="AQ21" s="20">
-        <v>0</v>
-      </c>
-      <c r="AR21" s="20">
+      <c r="AQ23" s="20">
+        <v>0</v>
+      </c>
+      <c r="AR23" s="20">
         <v>3</v>
       </c>
-      <c r="AS21" s="54"/>
-      <c r="AT21" s="17"/>
-      <c r="AU21" s="17"/>
-      <c r="AV21" s="17"/>
-      <c r="AW21" s="51"/>
-      <c r="AX21"/>
-      <c r="AY21"/>
-      <c r="AZ21"/>
-      <c r="BA21"/>
-      <c r="BB21" s="47"/>
-    </row>
-    <row r="22" spans="3:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22" s="60"/>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22"/>
-      <c r="I22"/>
-      <c r="J22" s="60"/>
-      <c r="K22"/>
-      <c r="L22"/>
-      <c r="M22"/>
-      <c r="N22"/>
-      <c r="O22"/>
-      <c r="P22"/>
-      <c r="Q22"/>
-      <c r="R22" s="60"/>
-      <c r="S22"/>
-      <c r="T22" s="60"/>
-      <c r="U22" s="15" t="s">
+      <c r="AS23" s="54"/>
+      <c r="AT23" s="17"/>
+      <c r="AU23" s="17"/>
+      <c r="AV23" s="17"/>
+      <c r="AW23" s="51"/>
+      <c r="AX23"/>
+      <c r="AY23"/>
+      <c r="AZ23"/>
+      <c r="BA23"/>
+      <c r="BB23" s="47"/>
+    </row>
+    <row r="24" spans="1:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24" s="60"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24" s="60"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+      <c r="R24" s="60"/>
+      <c r="S24"/>
+      <c r="T24" s="60"/>
+      <c r="U24" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="V22" s="15">
+      <c r="V24" s="15">
         <v>1</v>
       </c>
-      <c r="W22" s="15">
+      <c r="W24" s="15">
         <v>7000</v>
-      </c>
-      <c r="X22" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y22" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z22" s="15" t="s">
-        <v>311</v>
-      </c>
-      <c r="AI22" s="47"/>
-      <c r="AL22" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="AO22" s="47"/>
-      <c r="AS22" s="47"/>
-      <c r="AW22" s="47"/>
-      <c r="AX22"/>
-      <c r="AY22"/>
-      <c r="AZ22"/>
-      <c r="BA22"/>
-      <c r="BB22" s="47"/>
-    </row>
-    <row r="23" spans="3:54" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E23" s="56"/>
-      <c r="J23" s="56"/>
-      <c r="R23" s="56"/>
-      <c r="T23" s="56"/>
-      <c r="AI23" s="50"/>
-      <c r="AJ23" s="16"/>
-      <c r="AK23" s="16"/>
-      <c r="AL23" s="16"/>
-      <c r="AM23" s="16"/>
-      <c r="AN23" s="16"/>
-      <c r="AO23" s="50"/>
-      <c r="AQ23" s="19"/>
-      <c r="AR23" s="19"/>
-      <c r="AS23" s="53"/>
-      <c r="AT23" s="16"/>
-      <c r="AU23" s="16"/>
-      <c r="AV23" s="16"/>
-      <c r="AW23" s="50"/>
-      <c r="BB23" s="47"/>
-    </row>
-    <row r="24" spans="3:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E24" s="56"/>
-      <c r="J24" s="56"/>
-      <c r="R24" s="56"/>
-      <c r="T24" s="56"/>
-      <c r="U24" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="V24" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="W24" s="15">
-        <v>50</v>
       </c>
       <c r="X24" s="15" t="s">
         <v>20</v>
       </c>
       <c r="Y24" s="15" t="s">
-        <v>270</v>
+        <v>73</v>
       </c>
       <c r="Z24" s="15" t="s">
         <v>311</v>
       </c>
-      <c r="AD24" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE24" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF24" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="AG24" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="AH24" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="AI24" s="50"/>
-      <c r="AJ24" s="16" t="b">
+      <c r="AI24" s="47"/>
+      <c r="AL24" s="15" t="b">
         <v>1</v>
       </c>
-      <c r="AK24" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="AL24" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM24" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN24" s="16"/>
-      <c r="AO24" s="50"/>
-      <c r="AP24" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="AQ24" s="19">
-        <v>50</v>
-      </c>
-      <c r="AR24" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="AS24" s="53"/>
-      <c r="AT24" s="16"/>
-      <c r="AU24" s="16"/>
-      <c r="AV24" s="16"/>
-      <c r="AW24" s="50"/>
-      <c r="AX24" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="AY24" s="15">
-        <v>50</v>
-      </c>
-      <c r="AZ24" s="16" t="s">
-        <v>271</v>
-      </c>
+      <c r="AO24" s="47"/>
+      <c r="AS24" s="47"/>
+      <c r="AW24" s="47"/>
+      <c r="AX24"/>
+      <c r="AY24"/>
+      <c r="AZ24"/>
+      <c r="BA24"/>
       <c r="BB24" s="47"/>
     </row>
-    <row r="25" spans="3:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:54" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E25" s="56"/>
       <c r="J25" s="56"/>
       <c r="R25" s="56"/>
@@ -4000,55 +4036,95 @@
       <c r="AM25" s="16"/>
       <c r="AN25" s="16"/>
       <c r="AO25" s="50"/>
-      <c r="AP25" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="AQ25" s="19">
-        <v>170</v>
-      </c>
-      <c r="AR25" s="19" t="s">
-        <v>79</v>
-      </c>
+      <c r="AQ25" s="19"/>
+      <c r="AR25" s="19"/>
       <c r="AS25" s="53"/>
       <c r="AT25" s="16"/>
       <c r="AU25" s="16"/>
       <c r="AV25" s="16"/>
       <c r="AW25" s="50"/>
-      <c r="AX25" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AY25" s="15">
+      <c r="BB25" s="47"/>
+    </row>
+    <row r="26" spans="1:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E26" s="56"/>
+      <c r="J26" s="56"/>
+      <c r="R26" s="56"/>
+      <c r="T26" s="56"/>
+      <c r="U26" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="V26" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="W26" s="15">
         <v>50</v>
       </c>
-      <c r="AZ25" s="16" t="s">
+      <c r="X26" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y26" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="Z26" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="AD26" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="AF26" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="AG26" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH26" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="AI26" s="50"/>
+      <c r="AJ26" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK26" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL26" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM26" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN26" s="16"/>
+      <c r="AO26" s="50"/>
+      <c r="AP26" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="AQ26" s="19">
+        <v>50</v>
+      </c>
+      <c r="AR26" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="AS26" s="53"/>
+      <c r="AT26" s="16"/>
+      <c r="AU26" s="16"/>
+      <c r="AV26" s="16"/>
+      <c r="AW26" s="50"/>
+      <c r="AX26" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="AY26" s="15">
+        <v>50</v>
+      </c>
+      <c r="AZ26" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="BB25" s="47"/>
-    </row>
-    <row r="26" spans="3:54" s="65" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="AI26" s="66"/>
-      <c r="AJ26" s="66"/>
-      <c r="AK26" s="66"/>
-      <c r="AL26" s="66"/>
-      <c r="AM26" s="66"/>
-      <c r="AN26" s="66"/>
-      <c r="AO26" s="66"/>
-      <c r="AQ26" s="67"/>
-      <c r="AR26" s="67"/>
-      <c r="AS26" s="67"/>
-      <c r="AT26" s="66"/>
-      <c r="AU26" s="66"/>
-      <c r="AV26" s="66"/>
-      <c r="AW26" s="66"/>
-    </row>
-    <row r="27" spans="3:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D27" s="15" t="s">
-        <v>305</v>
-      </c>
+      <c r="BB26" s="47"/>
+    </row>
+    <row r="27" spans="1:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E27" s="56"/>
-      <c r="F27" s="15" t="s">
-        <v>306</v>
-      </c>
       <c r="J27" s="56"/>
       <c r="R27" s="56"/>
       <c r="T27" s="56"/>
@@ -4059,93 +4135,167 @@
       <c r="AM27" s="16"/>
       <c r="AN27" s="16"/>
       <c r="AO27" s="50"/>
-      <c r="AQ27" s="19"/>
-      <c r="AR27" s="19"/>
+      <c r="AP27" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="AQ27" s="19">
+        <v>170</v>
+      </c>
+      <c r="AR27" s="19" t="s">
+        <v>79</v>
+      </c>
       <c r="AS27" s="53"/>
       <c r="AT27" s="16"/>
       <c r="AU27" s="16"/>
       <c r="AV27" s="16"/>
       <c r="AW27" s="50"/>
+      <c r="AX27" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY27" s="15">
+        <v>50</v>
+      </c>
+      <c r="AZ27" s="16" t="s">
+        <v>271</v>
+      </c>
       <c r="BB27" s="47"/>
     </row>
-    <row r="28" spans="3:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E28" s="56"/>
-      <c r="F28" s="15" t="s">
+    <row r="28" spans="1:54" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI28" s="66"/>
+      <c r="AJ28" s="66"/>
+      <c r="AK28" s="66"/>
+      <c r="AL28" s="66"/>
+      <c r="AM28" s="66"/>
+      <c r="AN28" s="66"/>
+      <c r="AO28" s="66"/>
+      <c r="AQ28" s="67"/>
+      <c r="AR28" s="67"/>
+      <c r="AS28" s="67"/>
+      <c r="AT28" s="66"/>
+      <c r="AU28" s="66"/>
+      <c r="AV28" s="66"/>
+      <c r="AW28" s="66"/>
+    </row>
+    <row r="29" spans="1:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="E29" s="56"/>
+      <c r="F29" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="J29" s="56"/>
+      <c r="R29" s="56"/>
+      <c r="T29" s="56"/>
+      <c r="AI29" s="50"/>
+      <c r="AJ29" s="16"/>
+      <c r="AK29" s="16"/>
+      <c r="AL29" s="16"/>
+      <c r="AM29" s="16"/>
+      <c r="AN29" s="16"/>
+      <c r="AO29" s="50"/>
+      <c r="AQ29" s="19"/>
+      <c r="AR29" s="19"/>
+      <c r="AS29" s="53"/>
+      <c r="AT29" s="16"/>
+      <c r="AU29" s="16"/>
+      <c r="AV29" s="16"/>
+      <c r="AW29" s="50"/>
+      <c r="BB29" s="47"/>
+    </row>
+    <row r="30" spans="1:54" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E30" s="56"/>
+      <c r="F30" s="15" t="s">
         <v>307</v>
       </c>
-      <c r="J28" s="56"/>
-      <c r="R28" s="56"/>
-      <c r="T28" s="56"/>
-      <c r="AI28" s="50"/>
-      <c r="AJ28" s="16"/>
-      <c r="AK28" s="16"/>
-      <c r="AL28" s="16"/>
-      <c r="AM28" s="16"/>
-      <c r="AN28" s="16"/>
-      <c r="AO28" s="50"/>
-      <c r="AQ28" s="19"/>
-      <c r="AR28" s="19"/>
-      <c r="AS28" s="53"/>
-      <c r="AT28" s="16"/>
-      <c r="AU28" s="16"/>
-      <c r="AV28" s="16"/>
-      <c r="AW28" s="50"/>
-      <c r="BB28" s="47"/>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="59"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="59"/>
+      <c r="J30" s="56"/>
+      <c r="R30" s="56"/>
+      <c r="T30" s="56"/>
+      <c r="AI30" s="50"/>
+      <c r="AJ30" s="16"/>
+      <c r="AK30" s="16"/>
+      <c r="AL30" s="16"/>
+      <c r="AM30" s="16"/>
+      <c r="AN30" s="16"/>
+      <c r="AO30" s="50"/>
+      <c r="AQ30" s="19"/>
+      <c r="AR30" s="19"/>
+      <c r="AS30" s="53"/>
+      <c r="AT30" s="16"/>
+      <c r="AU30" s="16"/>
+      <c r="AV30" s="16"/>
+      <c r="AW30" s="50"/>
+      <c r="BB30" s="47"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="59"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="AX10:XFD11 AP12 BB16:XFD22 V29:V30 S5:U5 AJ5:XFD9 AJ13:XFD15 AJ17:BA18 AJ22:BA22 AJ19:AO19 AJ10:AO10 B6:B25 W28:Z28 X29:Z30 V13:X15 Z13:AH15 V5:AH10 V17:X19 Z17:AH19 AA16:AE16 Y13:Y19 AJ23:XFD30 AA22:AI30 V22:Z27 C11:T11 B5:Q5 C22:U25 C6:U10 B26:U30 C13:U19 C20:T20">
+  <conditionalFormatting sqref="AX10:XFD11 AP12 BB18:XFD24 V31:V32 S5:U5 AJ5:XFD9 AJ13:XFD14 AJ19:BA20 AJ24:BA24 AJ21:AO21 AJ10:AO10 B6:B14 W30:Z30 X31:Z32 V5:AH10 V19:X21 Z19:AH21 AA18:AE18 AJ25:XFD32 AA24:AI32 V24:Z29 C11:T11 B5:Q5 C24:U27 C6:U10 B28:U32 C13:AH14 C22:T22 C17:U21 Y17:Y21 Z17:AH17 V17:X17 B17:B27 AJ17:XFD17">
+    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AP10:AW11">
+    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AX21:BA22 AP23 V18:W18 AJ18:BA18">
+    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AP21:AW22">
     <cfRule type="cellIs" dxfId="16" priority="9" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AP10:AW11">
+  <conditionalFormatting sqref="AE18">
     <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AX19:BA20 AP21 V16:W16 AJ16:BA16">
+  <conditionalFormatting sqref="AF18:AH18">
     <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AP19:AW20">
+  <conditionalFormatting sqref="X18:Z18">
     <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE16">
+  <conditionalFormatting sqref="AI13:AI14 AI19:AI21 AI5:AI10 AI17">
     <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF16:AH16">
+  <conditionalFormatting sqref="AI18">
     <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X16:Z16">
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+  <conditionalFormatting sqref="AX16:XFD16 AJ15:XFD15 AJ16:AO16 B15:AH16">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI13:AI15 AI17:AI19 AI5:AI10">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+  <conditionalFormatting sqref="AP16:AW16">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI16">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+  <conditionalFormatting sqref="AI15:AI16">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6010,37 +6160,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AE9:XFD10 W11 AI15:XFD21 F29:XFD29 E9:V9 N30:XFD31 M29:M31 E22:XFD28 E18:V18 E21:AH21 E16:AH17 E30:E31 G30:L31 E12:XFD14 E4:XFD8 A10:B10 A21:C31 A12:C18 A4:C9 A19:B19">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W9:AD10">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE18:AH19 W20 E15:F15 Q15:AH15 H15:M15">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W18:AD19">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M15">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15:P15">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
ModelLoader: fixed task issue
</commit_message>
<xml_diff>
--- a/data/inputs/Asset Model - Demo.xlsx
+++ b/data/inputs/Asset Model - Demo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23308"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -4007,8 +4007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA0734F-FFBE-4DAF-BDE5-A12359370A0D}">
   <dimension ref="A1:BB84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U38" sqref="U38"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>

</xml_diff>

<commit_message>
Updates - Everything working
</commit_message>
<xml_diff>
--- a/data/inputs/Asset Model - Demo.xlsx
+++ b/data/inputs/Asset Model - Demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtreseder\OneDrive - KPMG\Documents\3. Client\Essential Energy\Probability of Failure Model\pof\data\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1661" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1DA7D12E-0385-4804-A9DD-D616FE6A2368}"/>
+  <xr:revisionPtr revIDLastSave="1664" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{99608332-D90C-4D24-845F-E9A2028A70F5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,7 +78,7 @@
     20mm of wallthickness loss not detectable</t>
       </text>
     </comment>
-    <comment ref="H7" authorId="2" shapeId="0" xr:uid="{3FC98A93-1BD2-46CA-8439-5A569DD9E38A}">
+    <comment ref="H6" authorId="2" shapeId="0" xr:uid="{3FC98A93-1BD2-46CA-8439-5A569DD9E38A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="331">
   <si>
     <t>Cause</t>
   </si>
@@ -449,6 +449,12 @@
     <t>ssf_calc</t>
   </si>
   <si>
+    <t>actual_safety_factor</t>
+  </si>
+  <si>
+    <t>dsf_calc</t>
+  </si>
+  <si>
     <t>termite_powder</t>
   </si>
   <si>
@@ -473,12 +479,6 @@
     <t>reduction_factor</t>
   </si>
   <si>
-    <t>actual_safety_factor</t>
-  </si>
-  <si>
-    <t>dsf_calc</t>
-  </si>
-  <si>
     <t>lightning_damage</t>
   </si>
   <si>
@@ -488,6 +488,9 @@
     <t>fire_damage</t>
   </si>
   <si>
+    <t>impact_damage</t>
+  </si>
+  <si>
     <t>CAT3/4 replacement</t>
   </si>
   <si>
@@ -497,9 +500,6 @@
     <t>as_good_as_new</t>
   </si>
   <si>
-    <t>impact_damage</t>
-  </si>
-  <si>
     <t>lean_angle</t>
   </si>
   <si>
@@ -516,9 +516,6 @@
   </si>
   <si>
     <t>lightning</t>
-  </si>
-  <si>
-    <t>lightning_strike</t>
   </si>
   <si>
     <t>assisted_failures</t>
@@ -1279,7 +1276,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1397,6 +1394,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6E0B4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1425,7 +1428,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1611,6 +1614,7 @@
     <xf numFmtId="0" fontId="9" fillId="20" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -3063,7 +3067,7 @@
   <threadedComment ref="AU5" dT="2020-09-09T03:27:17.71" personId="{382B0E3D-8CF3-4AD9-8A08-175DF2A62319}" id="{C397EB22-6AC0-4AF2-9D5D-CDA1CF4C3832}">
     <text>20mm of wallthickness loss not detectable</text>
   </threadedComment>
-  <threadedComment ref="H7" dT="2020-09-09T03:31:13.87" personId="{382B0E3D-8CF3-4AD9-8A08-175DF2A62319}" id="{3FC98A93-1BD2-46CA-8439-5A569DD9E38A}">
+  <threadedComment ref="H6" dT="2020-09-09T03:31:13.87" personId="{382B0E3D-8CF3-4AD9-8A08-175DF2A62319}" id="{3FC98A93-1BD2-46CA-8439-5A569DD9E38A}">
     <text>250 mm</text>
   </threadedComment>
   <threadedComment ref="AU8" dT="2020-09-09T03:33:43.87" personId="{382B0E3D-8CF3-4AD9-8A08-175DF2A62319}" id="{214FAD6C-C7E5-485F-8706-D09B002BBC46}">
@@ -3154,134 +3158,134 @@
   <sheetData>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
+        <v>262</v>
+      </c>
+      <c r="F3" t="s">
         <v>263</v>
-      </c>
-      <c r="F3" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" t="s">
+        <v>264</v>
+      </c>
+      <c r="F5" t="s">
         <v>265</v>
-      </c>
-      <c r="F5" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
+        <v>266</v>
+      </c>
+      <c r="N6" t="s">
         <v>267</v>
-      </c>
-      <c r="N6" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:19">
       <c r="O12" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Q12" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="S12" s="1" t="s">
         <v>271</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:19">
       <c r="F13" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="O13" t="s">
         <v>273</v>
       </c>
-      <c r="O13" t="s">
+      <c r="Q13" t="s">
+        <v>171</v>
+      </c>
+      <c r="S13" t="s">
         <v>274</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>172</v>
-      </c>
-      <c r="S13" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:19">
       <c r="F14" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="O14" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q14" t="s">
         <v>276</v>
       </c>
-      <c r="O14" t="s">
-        <v>169</v>
-      </c>
-      <c r="Q14" t="s">
+      <c r="S14" t="s">
         <v>277</v>
-      </c>
-      <c r="S14" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="15" spans="1:19">
       <c r="F15" t="s">
+        <v>278</v>
+      </c>
+      <c r="J15" t="s">
         <v>279</v>
       </c>
-      <c r="J15" t="s">
+      <c r="O15" t="s">
         <v>280</v>
       </c>
-      <c r="O15" t="s">
+      <c r="Q15" t="s">
         <v>281</v>
       </c>
-      <c r="Q15" t="s">
-        <v>282</v>
-      </c>
       <c r="S15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:19">
       <c r="F16" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>104</v>
+      </c>
+      <c r="S16" t="s">
         <v>283</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>103</v>
-      </c>
-      <c r="S16" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="17" spans="1:19">
       <c r="F17" t="s">
+        <v>284</v>
+      </c>
+      <c r="O17" t="s">
         <v>285</v>
       </c>
-      <c r="O17" t="s">
+      <c r="Q17" t="s">
         <v>286</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="18" spans="1:19">
       <c r="O18" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="20" spans="1:19">
       <c r="F20" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="27" spans="1:19">
       <c r="A27" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="31" spans="1:19">
       <c r="D31" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E31" t="s">
         <v>6</v>
@@ -3290,44 +3294,44 @@
         <v>80</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="S31" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:19">
       <c r="A32" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J32" t="s">
         <v>24</v>
       </c>
       <c r="R32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="S32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="2:19">
       <c r="B33" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K33" t="s">
         <v>51</v>
       </c>
       <c r="R33" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="S33">
         <v>0</v>
@@ -3335,13 +3339,13 @@
     </row>
     <row r="34" spans="2:19">
       <c r="C34" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K34" t="s">
         <v>54</v>
       </c>
       <c r="R34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="S34">
         <v>0.5</v>
@@ -3349,19 +3353,19 @@
     </row>
     <row r="35" spans="2:19">
       <c r="C35" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D35" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G35" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L35" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="R35" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="S35">
         <v>1</v>
@@ -3369,13 +3373,13 @@
     </row>
     <row r="36" spans="2:19">
       <c r="D36" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L36" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="R36" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="S36">
         <v>1</v>
@@ -3391,10 +3395,10 @@
     </row>
     <row r="38" spans="2:19">
       <c r="C38" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K38" t="s">
         <v>2</v>
@@ -3402,13 +3406,13 @@
     </row>
     <row r="39" spans="2:19">
       <c r="C39" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E39" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J39" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="2:19">
@@ -3428,29 +3432,29 @@
     </row>
     <row r="52" spans="1:12">
       <c r="H52" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="I53" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="54" spans="1:12">
       <c r="E54" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F54">
         <v>4</v>
@@ -3484,76 +3488,76 @@
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="59" spans="1:12">
       <c r="F59" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="60" spans="1:12">
       <c r="B60" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E60" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="61" spans="1:12">
       <c r="E61" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="62" spans="1:12">
       <c r="E62" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="B65" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="B68" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B69">
         <v>4</v>
       </c>
       <c r="C69" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B70">
         <v>250</v>
       </c>
       <c r="C70" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B71">
         <v>12.5</v>
       </c>
       <c r="C71" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -3585,48 +3589,48 @@
   <sheetData>
     <row r="2" spans="1:19">
       <c r="A2" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:19">
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>314</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="B4" t="s">
+        <v>315</v>
+      </c>
+      <c r="I4" t="s">
+        <v>313</v>
+      </c>
+      <c r="J4" t="s">
+        <v>314</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="I4" t="s">
-        <v>314</v>
-      </c>
-      <c r="J4" t="s">
-        <v>315</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" t="s">
         <v>317</v>
       </c>
-      <c r="R4" t="s">
-        <v>318</v>
-      </c>
       <c r="S4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="B5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I5" s="3">
         <v>14</v>
@@ -3636,18 +3640,18 @@
       </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="R5" s="41" t="s">
         <v>320</v>
       </c>
-      <c r="R5" s="41" t="s">
+      <c r="S5" t="s">
         <v>321</v>
-      </c>
-      <c r="S5" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="6" spans="1:19">
       <c r="H6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I6">
         <f>I5/4</f>
@@ -3659,51 +3663,51 @@
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="R6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="S6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="P7" s="1"/>
       <c r="Q7" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="R7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="S7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="8" spans="1:19">
       <c r="H8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I8" s="5">
         <v>320</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="R8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="S8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I9" s="5">
         <v>100</v>
@@ -3711,7 +3715,7 @@
     </row>
     <row r="10" spans="1:19">
       <c r="H10" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I10" s="5">
         <v>10</v>
@@ -3719,12 +3723,12 @@
     </row>
     <row r="11" spans="1:19">
       <c r="B11" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="12" spans="1:19">
       <c r="B12" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I12" s="9">
         <v>3.7</v>
@@ -3736,20 +3740,20 @@
     </row>
     <row r="16" spans="1:19">
       <c r="J16" t="s">
+        <v>328</v>
+      </c>
+      <c r="M16" t="s">
         <v>329</v>
-      </c>
-      <c r="M16" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="19" spans="10:10">
       <c r="J19" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="1048576" spans="15:15">
       <c r="O1048576" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -4028,8 +4032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA0734F-FFBE-4DAF-BDE5-A12359370A0D}">
   <dimension ref="A1:BG84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>
@@ -4523,10 +4527,18 @@
     </row>
     <row r="6" spans="1:59" s="15" customFormat="1">
       <c r="E6" s="56"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6" s="42"/>
-      <c r="I6"/>
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H6" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
       <c r="J6" s="56"/>
       <c r="R6" s="59"/>
       <c r="S6" s="15" t="s">
@@ -4586,16 +4598,16 @@
       <c r="D7" s="15"/>
       <c r="E7" s="56"/>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="G7" t="s">
-        <v>78</v>
-      </c>
-      <c r="H7" s="42" t="s">
-        <v>79</v>
+        <v>87</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="56"/>
       <c r="K7" s="15"/>
@@ -4650,13 +4662,13 @@
     <row r="8" spans="1:59" s="15" customFormat="1">
       <c r="E8" s="56"/>
       <c r="F8" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G8" t="s">
-        <v>87</v>
-      </c>
-      <c r="H8">
-        <v>4</v>
+        <v>89</v>
+      </c>
+      <c r="H8" s="42" t="s">
+        <v>79</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -4665,7 +4677,7 @@
       <c r="R8" s="56"/>
       <c r="Y8" s="56"/>
       <c r="Z8" s="15" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="AA8" s="42">
         <v>0.9</v>
@@ -4677,16 +4689,16 @@
         <v>2</v>
       </c>
       <c r="AD8" s="15" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="AE8" s="15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AF8" s="15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AI8" s="15" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="AN8" s="50"/>
       <c r="AO8" s="16" t="b">
@@ -4708,7 +4720,7 @@
         <v>50</v>
       </c>
       <c r="AW8" s="98" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AX8" s="53"/>
       <c r="AY8" s="16" t="b">
@@ -4722,13 +4734,13 @@
       </c>
       <c r="BB8" s="50"/>
       <c r="BC8" s="95" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BD8" s="97">
         <v>0</v>
       </c>
       <c r="BE8" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BF8" s="18" t="s">
         <v>2</v>
@@ -4737,17 +4749,17 @@
     </row>
     <row r="9" spans="1:59" s="15" customFormat="1">
       <c r="E9" s="56"/>
-      <c r="F9" t="s">
-        <v>96</v>
-      </c>
-      <c r="G9" t="s">
-        <v>97</v>
-      </c>
-      <c r="H9" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
+      <c r="F9" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="H9" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="J9" s="56"/>
       <c r="R9" s="56"/>
@@ -4766,7 +4778,7 @@
         <v>50</v>
       </c>
       <c r="AW9" s="98" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AX9" s="53"/>
       <c r="AY9" s="16"/>
@@ -4784,7 +4796,7 @@
       <c r="D10" s="15"/>
       <c r="E10" s="56"/>
       <c r="F10" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G10" s="15" t="s">
         <v>99</v>
@@ -4848,7 +4860,7 @@
     <row r="11" spans="1:59" s="15" customFormat="1">
       <c r="E11" s="56"/>
       <c r="F11" s="15" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G11" s="15" t="s">
         <v>99</v>
@@ -4863,7 +4875,7 @@
       <c r="R11" s="56"/>
       <c r="Y11" s="56"/>
       <c r="Z11" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AA11" s="15">
         <v>1</v>
@@ -4875,13 +4887,13 @@
         <v>2</v>
       </c>
       <c r="AD11" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AE11" s="15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AF11" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AI11" s="15" t="s">
         <v>6</v>
@@ -4920,13 +4932,13 @@
       </c>
       <c r="BB11" s="50"/>
       <c r="BC11" s="80" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BD11" s="19">
         <v>1</v>
       </c>
       <c r="BE11" s="15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BF11" s="15" t="s">
         <v>2</v>
@@ -4936,7 +4948,7 @@
     <row r="12" spans="1:59" s="15" customFormat="1">
       <c r="E12" s="56"/>
       <c r="F12" s="15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G12" s="15" t="s">
         <v>99</v>
@@ -4973,18 +4985,6 @@
     <row r="13" spans="1:59">
       <c r="A13" s="15"/>
       <c r="B13" s="15"/>
-      <c r="F13" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="H13" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I13" s="15" t="b">
-        <v>0</v>
-      </c>
       <c r="AU13" s="86"/>
       <c r="AV13" s="84"/>
       <c r="AW13" s="84"/>
@@ -5067,13 +5067,13 @@
         <v>2</v>
       </c>
       <c r="AD15" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AE15" s="15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AF15" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AI15" s="15" t="s">
         <v>6</v>
@@ -5102,13 +5102,13 @@
       </c>
       <c r="BB15" s="50"/>
       <c r="BC15" s="80" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BD15" s="19">
         <v>1</v>
       </c>
       <c r="BE15" s="15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BF15" s="15" t="s">
         <v>2</v>
@@ -5278,7 +5278,7 @@
       <c r="R19" s="56"/>
       <c r="Y19" s="56"/>
       <c r="Z19" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AA19" s="15">
         <v>1</v>
@@ -5290,13 +5290,13 @@
         <v>2</v>
       </c>
       <c r="AD19" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AE19" s="15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AF19" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AI19" s="15" t="s">
         <v>6</v>
@@ -5335,13 +5335,13 @@
       </c>
       <c r="BB19" s="50"/>
       <c r="BC19" s="80" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BD19" s="19">
         <v>1</v>
       </c>
       <c r="BE19" s="15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BF19" s="15" t="s">
         <v>2</v>
@@ -5534,13 +5534,13 @@
         <v>2</v>
       </c>
       <c r="AD23" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AE23" s="15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AF23" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AI23" s="15" t="s">
         <v>6</v>
@@ -5569,13 +5569,13 @@
       </c>
       <c r="BB23" s="50"/>
       <c r="BC23" s="80" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BD23" s="19">
         <v>1</v>
       </c>
       <c r="BE23" s="15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BF23" s="15" t="s">
         <v>2</v>
@@ -5760,10 +5760,10 @@
         <v>2</v>
       </c>
       <c r="AD27" s="15" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="AE27" s="15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AF27" s="15" t="s">
         <v>82</v>
@@ -5788,7 +5788,7 @@
         <v>50</v>
       </c>
       <c r="AW27" s="75" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AX27" s="53"/>
       <c r="AY27" s="16" t="b">
@@ -5827,7 +5827,7 @@
         <v>50</v>
       </c>
       <c r="AW28" s="75" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AX28" s="53"/>
       <c r="AY28" s="16"/>
@@ -5886,7 +5886,7 @@
       <c r="R30" s="56"/>
       <c r="Y30" s="56"/>
       <c r="Z30" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AA30" s="15">
         <v>1</v>
@@ -5898,13 +5898,13 @@
         <v>2</v>
       </c>
       <c r="AD30" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AE30" s="15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AF30" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AI30" s="15" t="s">
         <v>6</v>
@@ -5943,13 +5943,13 @@
       </c>
       <c r="BB30" s="50"/>
       <c r="BC30" s="80" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BD30" s="19">
         <v>1</v>
       </c>
       <c r="BE30" s="15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BF30" s="15" t="s">
         <v>2</v>
@@ -6142,13 +6142,13 @@
         <v>2</v>
       </c>
       <c r="AD34" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AE34" s="15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AF34" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AI34" s="15" t="s">
         <v>6</v>
@@ -6177,13 +6177,13 @@
       </c>
       <c r="BB34" s="50"/>
       <c r="BC34" s="80" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BD34" s="19">
         <v>1</v>
       </c>
       <c r="BE34" s="15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BF34" s="15" t="s">
         <v>2</v>
@@ -6242,8 +6242,8 @@
         <v>1</v>
       </c>
       <c r="R36" s="56"/>
-      <c r="S36" s="41" t="s">
-        <v>111</v>
+      <c r="S36" s="99" t="s">
+        <v>98</v>
       </c>
       <c r="T36" s="41"/>
       <c r="U36" s="41"/>
@@ -6273,7 +6273,7 @@
         <v>82</v>
       </c>
       <c r="AJ36" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AN36" s="50"/>
       <c r="AO36" s="18" t="b">
@@ -6285,7 +6285,7 @@
       <c r="AS36" s="18"/>
       <c r="AT36" s="50"/>
       <c r="AU36" s="88" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AV36" s="19" t="b">
         <v>1</v>
@@ -6393,7 +6393,7 @@
       <c r="AS38" s="18"/>
       <c r="AT38" s="50"/>
       <c r="AU38" s="88" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AV38" s="19" t="b">
         <v>1</v>
@@ -6489,13 +6489,13 @@
         <v>2</v>
       </c>
       <c r="AD40" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AE40" s="15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AF40" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AI40" s="15" t="s">
         <v>6</v>
@@ -6524,13 +6524,13 @@
       </c>
       <c r="BB40" s="50"/>
       <c r="BC40" s="80" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BD40" s="19">
         <v>1</v>
       </c>
       <c r="BE40" s="15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BF40" s="15" t="s">
         <v>2</v>
@@ -6615,7 +6615,7 @@
         <v>82</v>
       </c>
       <c r="AJ42" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AN42" s="50"/>
       <c r="AO42" s="18" t="b">
@@ -6699,7 +6699,7 @@
       <c r="R44" s="56"/>
       <c r="Y44" s="56"/>
       <c r="Z44" s="45" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AA44" s="15">
         <v>1</v>
@@ -6711,13 +6711,13 @@
         <v>2</v>
       </c>
       <c r="AD44" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AE44" s="15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AF44" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AI44" s="15" t="s">
         <v>6</v>
@@ -6756,13 +6756,13 @@
       </c>
       <c r="BB44" s="50"/>
       <c r="BC44" s="80" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BD44" s="19">
         <v>1</v>
       </c>
       <c r="BE44" s="15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BF44" s="15" t="s">
         <v>2</v>
@@ -6955,13 +6955,13 @@
         <v>2</v>
       </c>
       <c r="AD48" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AE48" s="15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AF48" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AI48" s="15" t="s">
         <v>6</v>
@@ -6990,13 +6990,13 @@
       </c>
       <c r="BB48" s="50"/>
       <c r="BC48" s="80" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BD48" s="19">
         <v>1</v>
       </c>
       <c r="BE48" s="15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BF48" s="15" t="s">
         <v>2</v>
@@ -7034,7 +7034,7 @@
       <c r="E50" s="56"/>
       <c r="J50" s="56"/>
       <c r="K50" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L50" s="41">
         <v>50</v>
@@ -7056,7 +7056,7 @@
       </c>
       <c r="R50" s="56"/>
       <c r="S50" s="15" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="Y50" s="56"/>
       <c r="Z50" s="15" t="s">
@@ -7081,7 +7081,7 @@
         <v>82</v>
       </c>
       <c r="AJ50" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AN50" s="50"/>
       <c r="AO50" s="18" t="b">
@@ -7193,13 +7193,13 @@
         <v>2</v>
       </c>
       <c r="AD52" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AE52" s="15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AF52" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AI52" s="15" t="s">
         <v>6</v>
@@ -7228,13 +7228,13 @@
       </c>
       <c r="BB52" s="50"/>
       <c r="BC52" s="80" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BD52" s="19">
         <v>1</v>
       </c>
       <c r="BE52" s="15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BF52" s="15" t="s">
         <v>2</v>
@@ -7272,7 +7272,7 @@
       <c r="E54" s="56"/>
       <c r="J54" s="56"/>
       <c r="K54" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L54" s="41">
         <v>50</v>
@@ -7401,7 +7401,7 @@
       <c r="R56" s="56"/>
       <c r="Y56" s="56"/>
       <c r="Z56" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AA56" s="15">
         <v>1</v>
@@ -7413,13 +7413,13 @@
         <v>2</v>
       </c>
       <c r="AD56" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AE56" s="15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AF56" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AI56" s="15" t="s">
         <v>6</v>
@@ -7458,13 +7458,13 @@
       </c>
       <c r="BB56" s="50"/>
       <c r="BC56" s="80" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BD56" s="19">
         <v>1</v>
       </c>
       <c r="BE56" s="15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BF56" s="15" t="s">
         <v>2</v>
@@ -7657,13 +7657,13 @@
         <v>2</v>
       </c>
       <c r="AD60" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AE60" s="15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AF60" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AI60" s="15" t="s">
         <v>6</v>
@@ -7692,13 +7692,13 @@
       </c>
       <c r="BB60" s="50"/>
       <c r="BC60" s="80" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BD60" s="19">
         <v>1</v>
       </c>
       <c r="BE60" s="15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BF60" s="15" t="s">
         <v>2</v>
@@ -7727,11 +7727,11 @@
     <row r="62" spans="1:59" s="15" customFormat="1">
       <c r="C62" s="41"/>
       <c r="D62" s="41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E62" s="56"/>
       <c r="F62" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G62" t="s">
         <v>99</v>
@@ -7744,7 +7744,7 @@
       </c>
       <c r="J62" s="56"/>
       <c r="K62" s="42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L62" s="41">
         <v>50</v>
@@ -7899,7 +7899,7 @@
       <c r="R64" s="56"/>
       <c r="Y64" s="56"/>
       <c r="Z64" s="45" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AA64" s="15">
         <v>1</v>
@@ -7911,13 +7911,13 @@
         <v>2</v>
       </c>
       <c r="AD64" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AE64" s="15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AF64" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AI64" s="15" t="s">
         <v>6</v>
@@ -7956,13 +7956,13 @@
       </c>
       <c r="BB64" s="50"/>
       <c r="BC64" s="80" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BD64" s="19">
         <v>1</v>
       </c>
       <c r="BE64" s="15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BF64" s="15" t="s">
         <v>2</v>
@@ -8087,13 +8087,13 @@
         <v>69</v>
       </c>
       <c r="AD68" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AE68" s="15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AF68" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AI68" s="15" t="s">
         <v>6</v>
@@ -8122,13 +8122,13 @@
       </c>
       <c r="BB68" s="50"/>
       <c r="BC68" s="80" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BD68" s="19">
         <v>1</v>
       </c>
       <c r="BE68" s="15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BF68" s="15" t="s">
         <v>2</v>
@@ -8157,11 +8157,11 @@
     <row r="70" spans="1:59" s="15" customFormat="1">
       <c r="C70" s="41"/>
       <c r="D70" s="41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E70" s="56"/>
       <c r="F70" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G70" t="s">
         <v>99</v>
@@ -8174,7 +8174,7 @@
       </c>
       <c r="J70" s="56"/>
       <c r="K70" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L70" s="41">
         <v>50</v>
@@ -8331,7 +8331,7 @@
       <c r="R72" s="56"/>
       <c r="Y72" s="56"/>
       <c r="Z72" s="45" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AA72" s="15">
         <v>1</v>
@@ -8343,13 +8343,13 @@
         <v>2</v>
       </c>
       <c r="AD72" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AE72" s="15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AF72" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AI72" s="15" t="s">
         <v>6</v>
@@ -8388,13 +8388,13 @@
       </c>
       <c r="BB72" s="50"/>
       <c r="BC72" s="80" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BD72" s="19">
         <v>1</v>
       </c>
       <c r="BE72" s="15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BF72" s="15" t="s">
         <v>2</v>
@@ -8507,7 +8507,7 @@
       <c r="R76" s="56"/>
       <c r="Y76" s="56"/>
       <c r="Z76" s="45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AA76" s="15">
         <v>1</v>
@@ -8519,13 +8519,13 @@
         <v>69</v>
       </c>
       <c r="AD76" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AE76" s="15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AF76" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AI76" s="15" t="s">
         <v>6</v>
@@ -8554,13 +8554,13 @@
       </c>
       <c r="BB76" s="50"/>
       <c r="BC76" s="80" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BD76" s="19">
         <v>1</v>
       </c>
       <c r="BE76" s="15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BF76" s="15" t="s">
         <v>2</v>
@@ -8588,17 +8588,17 @@
     </row>
     <row r="78" spans="1:59" s="15" customFormat="1">
       <c r="D78" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E78" s="56"/>
       <c r="F78" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J78" s="56"/>
       <c r="R78" s="56"/>
       <c r="Y78" s="56"/>
       <c r="Z78" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AA78" s="15">
         <v>0.9</v>
@@ -8610,16 +8610,16 @@
         <v>2</v>
       </c>
       <c r="AD78" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AE78" s="15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AI78" s="15" t="s">
         <v>6</v>
       </c>
       <c r="AJ78" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AK78" s="15" t="s">
         <v>85</v>
@@ -8652,7 +8652,7 @@
         <v>50</v>
       </c>
       <c r="AW78" s="19" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AX78" s="53"/>
       <c r="AY78" s="16"/>
@@ -8666,14 +8666,14 @@
         <v>50</v>
       </c>
       <c r="BE78" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="BG78" s="47"/>
     </row>
     <row r="79" spans="1:59" s="15" customFormat="1">
       <c r="E79" s="56"/>
       <c r="F79" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J79" s="56"/>
       <c r="R79" s="56"/>
@@ -8692,7 +8692,7 @@
         <v>170</v>
       </c>
       <c r="AW79" s="19" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AX79" s="53"/>
       <c r="AY79" s="16"/>
@@ -8706,7 +8706,7 @@
         <v>50</v>
       </c>
       <c r="BE79" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="BG79" s="47"/>
     </row>
@@ -8722,7 +8722,7 @@
       <c r="J84" s="59"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="BC11:XFD12 AU13 AO5:XFD6 AO11:AT11 B7:B13 AF17:AJ17 C12:Y12 AD16:AD17 AE16:AM16 AA16:AC16 AO16:XFD16 C10:Y10 BG10:XFD10 C8:AM9 AO8:XFD9 BG7:XFD7 AC80:XFD81 BG78:XFD79 B80:AA81 B78:Y79 B77:XFD77 I23:Y23 I35:XFD35 C23:E23 F22:H23 B35:H39 B71:B74 C71:I72 C11:AM11 AG36:BB36 C7:R7 Y7 BG17:XFD23 B16:B23 C18:E20 I18:Y20 F17:H19 BG36:XFD40 B40:Y40 I36:K36 I37:Y39 BG50:XFD52 B52:Y52 F13:I13 C16:Z17 R36:AE36 B5:Q6 S5:AM6">
+  <conditionalFormatting sqref="BC11:XFD12 AU13 AO5:XFD6 AO11:AT11 B7:B13 AF17:AJ17 AD16:AD17 AE16:AM16 AA16:AC16 AO16:XFD16 BG10:XFD10 AO8:XFD9 BG7:XFD7 AC80:XFD81 BG78:XFD79 B80:AA81 B78:Y79 B77:XFD77 I23:Y23 I35:XFD35 C23:E23 F22:H23 B35:H39 B71:B74 C71:I72 AG36:BB36 Y7 BG17:XFD23 B16:B23 C18:E20 I18:Y20 F17:H19 BG36:XFD40 B40:Y40 I36:K36 I37:Y39 BG50:XFD52 B52:Y52 C16:Z17 B5:Q6 S5:AM6 R36:AE36 J12:Y12 J10:Y10 J8:AM9 J11:AM11 C7:E12 J7:R7 F6:I12">
     <cfRule type="cellIs" dxfId="164" priority="181" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
@@ -9531,39 +9531,39 @@
     <row r="2" spans="1:20">
       <c r="J2" s="1"/>
       <c r="Q2" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="R2" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="R2" s="27" t="s">
+      <c r="S2" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="S2" s="27" t="s">
+      <c r="T2" s="27" t="s">
         <v>131</v>
-      </c>
-      <c r="T2" s="27" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" t="s">
         <v>133</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>134</v>
-      </c>
-      <c r="D3" t="s">
-        <v>135</v>
       </c>
       <c r="Q3" s="28"/>
     </row>
     <row r="4" spans="1:20">
       <c r="B4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="Q4" s="29" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="R4" s="29"/>
       <c r="S4" s="29"/>
@@ -9571,7 +9571,7 @@
     </row>
     <row r="5" spans="1:20">
       <c r="B5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q5" s="29"/>
       <c r="R5" s="30" t="s">
@@ -9582,7 +9582,7 @@
     </row>
     <row r="6" spans="1:20">
       <c r="B6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q6" s="31"/>
       <c r="R6" s="31"/>
@@ -9593,72 +9593,72 @@
     </row>
     <row r="7" spans="1:20">
       <c r="B7" t="s">
+        <v>138</v>
+      </c>
+      <c r="T7" t="s">
         <v>139</v>
-      </c>
-      <c r="T7" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="T8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="T9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="T10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="T11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="Q12" s="31"/>
       <c r="R12" s="31"/>
       <c r="S12" s="31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="T12" s="31"/>
     </row>
     <row r="13" spans="1:20">
       <c r="T13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="Q14" s="31"/>
       <c r="R14" s="31"/>
       <c r="S14" s="31" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T14" s="31"/>
     </row>
     <row r="15" spans="1:20">
       <c r="T15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="T16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="17:20">
       <c r="T17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="17:20">
       <c r="Q18" s="29"/>
       <c r="R18" s="30" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="S18" s="29"/>
       <c r="T18" s="29"/>
@@ -9667,85 +9667,85 @@
       <c r="Q19" s="31"/>
       <c r="R19" s="31"/>
       <c r="S19" s="31" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="T19" s="31"/>
     </row>
     <row r="20" spans="17:20">
       <c r="T20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="17:20">
       <c r="Q21" s="28"/>
       <c r="S21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="17:20">
       <c r="Q22" s="28"/>
       <c r="T22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="17:20">
       <c r="Q23" s="28"/>
       <c r="S23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="17:20">
       <c r="Q24" s="28"/>
       <c r="T24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="17:20">
       <c r="Q25" s="28"/>
       <c r="T25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="17:20">
       <c r="Q26" s="28"/>
       <c r="S26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="17:20">
       <c r="Q27" s="28"/>
       <c r="S27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="17:20">
       <c r="Q28" s="28"/>
       <c r="T28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="17:20">
       <c r="Q29" s="28"/>
       <c r="S29" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="17:20">
       <c r="Q30" s="28"/>
       <c r="T30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="17:20">
       <c r="Q31" s="28"/>
       <c r="T31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="17:20">
       <c r="Q32" s="29"/>
       <c r="R32" s="30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="S32" s="29"/>
       <c r="T32" s="29"/>
@@ -9754,34 +9754,34 @@
       <c r="Q33" s="31"/>
       <c r="R33" s="31"/>
       <c r="S33" s="31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="T33" s="31"/>
     </row>
     <row r="34" spans="17:20">
       <c r="Q34" s="28"/>
       <c r="T34" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="35" spans="17:20">
       <c r="Q35" s="31"/>
       <c r="R35" s="31"/>
       <c r="S35" s="31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="T35" s="31"/>
     </row>
     <row r="36" spans="17:20">
       <c r="Q36" s="28"/>
       <c r="T36" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="37" spans="17:20">
       <c r="Q37" s="29"/>
       <c r="R37" s="30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S37" s="29"/>
       <c r="T37" s="29"/>
@@ -9790,28 +9790,28 @@
       <c r="Q38" s="31"/>
       <c r="R38" s="31"/>
       <c r="S38" s="31" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="T38" s="31"/>
     </row>
     <row r="39" spans="17:20">
       <c r="Q39" s="28"/>
       <c r="T39" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40" spans="17:20">
       <c r="Q40" s="31"/>
       <c r="R40" s="31"/>
       <c r="S40" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="T40" s="31"/>
     </row>
     <row r="41" spans="17:20">
       <c r="Q41" s="28"/>
       <c r="T41" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -9852,7 +9852,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
       <c r="H1" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -9878,12 +9878,12 @@
         <v>15</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B3">
         <v>50</v>
@@ -9923,7 +9923,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E5" t="s">
         <v>99</v>
@@ -9935,12 +9935,12 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B6">
         <v>50</v>
@@ -9955,12 +9955,12 @@
         <v>99</v>
       </c>
       <c r="H6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E7" t="s">
         <v>99</v>
@@ -9971,7 +9971,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B8">
         <v>80</v>
@@ -9997,7 +9997,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E9" t="s">
         <v>78</v>
@@ -10008,7 +10008,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E10" t="s">
         <v>78</v>
@@ -10019,7 +10019,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B11" s="42"/>
       <c r="C11" s="42"/>
@@ -10027,7 +10027,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B12">
         <v>1000</v>
@@ -10048,13 +10048,13 @@
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J12" s="45"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F13">
         <v>25</v>
@@ -10062,22 +10062,22 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="42" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B19">
         <v>50</v>
@@ -10092,12 +10092,12 @@
         <v>99</v>
       </c>
       <c r="H19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B20">
         <v>50</v>
@@ -10112,7 +10112,7 @@
         <v>99</v>
       </c>
       <c r="H20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -10138,10 +10138,10 @@
   <sheetData>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
@@ -10155,7 +10155,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -10183,7 +10183,7 @@
         <v>86</v>
       </c>
       <c r="C5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -10192,45 +10192,45 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="B6" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C9" t="s">
         <v>99</v>
@@ -10238,7 +10238,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="B10" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3">
@@ -10301,7 +10301,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="R1" s="22"/>
       <c r="S1" s="22"/>
@@ -10313,7 +10313,7 @@
       <c r="Y1" s="24"/>
       <c r="Z1" s="52"/>
       <c r="AA1" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AB1" s="21"/>
       <c r="AC1" s="21"/>
@@ -10326,7 +10326,7 @@
     </row>
     <row r="2" spans="1:35" s="1" customFormat="1">
       <c r="C2" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E2" s="25"/>
       <c r="F2" s="25"/>
@@ -10367,7 +10367,7 @@
       <c r="AC2" s="21"/>
       <c r="AD2" s="49"/>
       <c r="AE2" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AF2" s="4"/>
       <c r="AG2" s="4"/>
@@ -10382,7 +10382,7 @@
         <v>48</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E3" s="25" t="s">
         <v>57</v>
@@ -10437,7 +10437,7 @@
       </c>
       <c r="V3" s="55"/>
       <c r="W3" s="23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="X3" s="24" t="s">
         <v>26</v>
@@ -10457,7 +10457,7 @@
       </c>
       <c r="AD3" s="49"/>
       <c r="AE3" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AF3" s="4" t="s">
         <v>75</v>
@@ -10475,7 +10475,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>80</v>
@@ -10502,7 +10502,7 @@
         <v>5</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M4" s="15" t="s">
         <v>83</v>
@@ -10520,10 +10520,10 @@
         <v>1</v>
       </c>
       <c r="R4" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="S4" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="T4" s="18"/>
       <c r="U4" s="18"/>
@@ -10565,7 +10565,7 @@
     </row>
     <row r="6" spans="1:35" s="15" customFormat="1">
       <c r="C6" s="15" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E6" s="15">
         <v>0.9</v>
@@ -10577,13 +10577,13 @@
         <v>69</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="Q6" s="16" t="b">
         <v>1</v>
@@ -10604,7 +10604,7 @@
         <v>50</v>
       </c>
       <c r="Y6" s="19" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="Z6" s="53"/>
       <c r="AA6" s="16" t="b">
@@ -10637,7 +10637,7 @@
         <v>50</v>
       </c>
       <c r="Y7" s="19" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="Z7" s="53"/>
       <c r="AA7" s="16" t="b">
@@ -10671,7 +10671,7 @@
     </row>
     <row r="9" spans="1:35" s="15" customFormat="1">
       <c r="C9" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E9" s="15">
         <v>1</v>
@@ -10683,10 +10683,10 @@
         <v>69</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L9" s="15" t="s">
         <v>6</v>
@@ -10724,13 +10724,13 @@
       </c>
       <c r="AD9" s="50"/>
       <c r="AE9" s="15" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="AF9" s="15">
         <v>1</v>
       </c>
       <c r="AG9" s="15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AH9" s="15" t="s">
         <v>2</v>
@@ -10818,7 +10818,7 @@
         <v>28</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>80</v>
@@ -10830,7 +10830,7 @@
         <v>50</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H15" s="15" t="s">
         <v>80</v>
@@ -10857,45 +10857,45 @@
         <v>1</v>
       </c>
       <c r="R15" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="S15" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="T15" s="18"/>
       <c r="U15" s="18"/>
       <c r="V15" s="50"/>
       <c r="W15" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="X15" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Y15" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Z15" s="50"/>
       <c r="AA15" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AB15" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AC15" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AD15" s="50"/>
       <c r="AE15" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AF15" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AG15" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AH15" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AI15" s="47"/>
     </row>
@@ -10913,7 +10913,7 @@
         <v>54</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="Q16" s="16" t="b">
         <v>1</v>
@@ -10934,7 +10934,7 @@
         <v>50</v>
       </c>
       <c r="Y16" s="19" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="Z16" s="53"/>
       <c r="AA16" s="16" t="b">
@@ -10948,16 +10948,16 @@
       </c>
       <c r="AD16" s="50"/>
       <c r="AE16" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AF16" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AG16" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AH16" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AI16" s="47"/>
     </row>
@@ -10975,7 +10975,7 @@
         <v>50</v>
       </c>
       <c r="Y17" s="19" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="Z17" s="53"/>
       <c r="AA17" s="16" t="b">
@@ -10992,7 +10992,7 @@
     </row>
     <row r="18" spans="1:35" s="15" customFormat="1">
       <c r="C18" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E18" s="15">
         <v>1</v>
@@ -11004,7 +11004,7 @@
         <v>2</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="Q18" s="16" t="b">
         <v>1</v>
@@ -11104,7 +11104,7 @@
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E21" s="15">
         <v>1</v>
@@ -11116,36 +11116,36 @@
         <v>2</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="Q21" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="R21" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="S21" s="15" t="b">
         <v>1</v>
       </c>
       <c r="V21" s="47"/>
       <c r="W21" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="X21" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Y21" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Z21" s="47"/>
       <c r="AA21" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AB21" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AC21" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AD21" s="47"/>
       <c r="AE21"/>
@@ -11172,7 +11172,7 @@
     </row>
     <row r="23" spans="1:35" s="15" customFormat="1">
       <c r="C23" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E23" s="15">
         <v>0.9</v>
@@ -11184,13 +11184,13 @@
         <v>2</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L23" s="15" t="s">
         <v>6</v>
       </c>
       <c r="M23" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N23" s="15" t="s">
         <v>85</v>
@@ -11222,17 +11222,17 @@
         <v>50</v>
       </c>
       <c r="Y23" s="19" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="Z23" s="53"/>
       <c r="AA23" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AB23" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AC23" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AD23" s="50"/>
       <c r="AE23" s="16" t="s">
@@ -11242,7 +11242,7 @@
         <v>50</v>
       </c>
       <c r="AG23" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AI23" s="47"/>
     </row>
@@ -11260,17 +11260,17 @@
         <v>170</v>
       </c>
       <c r="Y24" s="19" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="Z24" s="53"/>
       <c r="AA24" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AB24" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AC24" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AD24" s="50"/>
       <c r="AE24" s="16" t="s">
@@ -11280,7 +11280,7 @@
         <v>50</v>
       </c>
       <c r="AG24" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AI24" s="47"/>
     </row>
@@ -11425,19 +11425,19 @@
   <sheetData>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>208</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>58</v>
@@ -11451,19 +11451,19 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C3" t="s">
         <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F3">
         <v>50</v>
@@ -11471,18 +11471,18 @@
     </row>
     <row r="4" spans="1:8">
       <c r="C4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="C5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -11494,7 +11494,7 @@
         <v>100000</v>
       </c>
       <c r="G5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -11536,7 +11536,7 @@
         <v>208</v>
       </c>
       <c r="E9" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F9">
         <v>3500</v>
@@ -11544,19 +11544,19 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>208</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>58</v>
@@ -11564,36 +11564,36 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C13" t="s">
         <v>80</v>
       </c>
       <c r="D13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E13" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F13">
         <v>50</v>
       </c>
       <c r="H13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="C14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E14" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F14">
         <v>36</v>
@@ -11615,13 +11615,13 @@
     </row>
     <row r="16" spans="1:8">
       <c r="C16" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D16">
         <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F16">
         <v>7000</v>
@@ -11669,226 +11669,226 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="B4" s="32" t="s">
         <v>212</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>213</v>
       </c>
       <c r="C4" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="B5" s="33" t="s">
         <v>212</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>213</v>
       </c>
       <c r="C5" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="B6" s="32" t="s">
         <v>212</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>213</v>
       </c>
       <c r="C6" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="B7" s="33" t="s">
         <v>212</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>213</v>
       </c>
       <c r="C7" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="B8" s="32" t="s">
         <v>212</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>213</v>
       </c>
       <c r="C8" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="B9" s="33" t="s">
         <v>212</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>213</v>
       </c>
       <c r="C9" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="B10" s="34" t="s">
         <v>212</v>
-      </c>
-      <c r="B10" s="34" t="s">
-        <v>213</v>
       </c>
       <c r="C10" s="34" t="e">
         <v>#REF!</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="B11" s="34" t="s">
         <v>212</v>
-      </c>
-      <c r="B11" s="34" t="s">
-        <v>213</v>
       </c>
       <c r="C11" s="34" t="e">
         <v>#REF!</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="B12" s="34" t="s">
         <v>212</v>
-      </c>
-      <c r="B12" s="34" t="s">
-        <v>213</v>
       </c>
       <c r="C12" s="34" t="e">
         <v>#REF!</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="B13" s="34" t="s">
         <v>212</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>213</v>
       </c>
       <c r="C13" s="34" t="e">
         <v>#REF!</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="B14" s="34" t="s">
         <v>212</v>
-      </c>
-      <c r="B14" s="34" t="s">
-        <v>213</v>
       </c>
       <c r="C14" s="34" t="e">
         <v>#REF!</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="B15" s="34" t="s">
         <v>212</v>
-      </c>
-      <c r="B15" s="34" t="s">
-        <v>213</v>
       </c>
       <c r="C15" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="32" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C16" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="B17" s="33" t="s">
         <v>227</v>
-      </c>
-      <c r="B17" s="33" t="s">
-        <v>228</v>
       </c>
       <c r="C17" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="B18" s="32" t="s">
         <v>227</v>
-      </c>
-      <c r="B18" s="32" t="s">
-        <v>228</v>
       </c>
       <c r="C18" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="32" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C19" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -11909,72 +11909,72 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="B22" s="32" t="s">
         <v>230</v>
-      </c>
-      <c r="B22" s="32" t="s">
-        <v>231</v>
       </c>
       <c r="C22" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="33" t="s">
+        <v>229</v>
+      </c>
+      <c r="B23" s="33" t="s">
         <v>230</v>
-      </c>
-      <c r="B23" s="33" t="s">
-        <v>231</v>
       </c>
       <c r="C23" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D23" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="B24" s="32" t="s">
         <v>230</v>
-      </c>
-      <c r="B24" s="32" t="s">
-        <v>231</v>
       </c>
       <c r="C24" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D24" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="33" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C25" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D25" s="33" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="32" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C26" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D26" s="32" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -11987,86 +11987,86 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="32" t="s">
+        <v>236</v>
+      </c>
+      <c r="B28" s="32" t="s">
         <v>237</v>
-      </c>
-      <c r="B28" s="32" t="s">
-        <v>238</v>
       </c>
       <c r="C28" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D28" s="32" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="33" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C29" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D29" s="33" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="32" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C30" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D30" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="33" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C31" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D31" s="33" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="32" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C32" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D32" s="32" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="33" t="s">
+        <v>241</v>
+      </c>
+      <c r="B33" s="33" t="s">
         <v>242</v>
-      </c>
-      <c r="B33" s="33" t="s">
-        <v>243</v>
       </c>
       <c r="C33" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D33" s="36" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -12079,72 +12079,72 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="33" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C35" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D35" s="33" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="B36" s="32" t="s">
         <v>244</v>
-      </c>
-      <c r="B36" s="32" t="s">
-        <v>245</v>
       </c>
       <c r="C36" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D36" s="32" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="33" t="s">
+        <v>243</v>
+      </c>
+      <c r="B37" s="33" t="s">
         <v>244</v>
-      </c>
-      <c r="B37" s="33" t="s">
-        <v>245</v>
       </c>
       <c r="C37" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D37" s="33" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B38" s="32" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C38" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D38" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="33" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B39" s="33" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C39" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D39" s="33" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -12165,16 +12165,16 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="32" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B42" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C42" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D42" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -12187,226 +12187,226 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="32" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B44" s="39" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C44" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D44" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="33" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B45" s="36" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C45" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D45" s="33" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="32" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B46" s="39" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C46" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D46" s="32" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B47" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C47" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D47" s="33" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="32" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B48" s="39" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C48" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D48" s="32" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="33" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B49" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C49" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D49" s="33" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="32" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B50" s="39" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C50" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D50" s="32" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="33" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B51" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C51" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D51" s="33" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="32" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B52" s="39" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C52" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D52" s="32" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="33" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B53" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C53" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D53" s="33" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="32" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B54" s="32" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C54" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D54" s="32" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="33" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B55" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C55" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D55" s="33" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="32" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B56" s="32" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C56" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D56" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="33" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B57" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C57" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D57" s="33" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="32" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B58" s="39" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C58" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D58" s="32" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="33" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B59" s="36" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C59" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D59" s="33" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -12419,86 +12419,86 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="33" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B61" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C61" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D61" s="33" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="32" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B62" s="39" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C62" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D62" s="32" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="33" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B63" s="33" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C63" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D63" s="33" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="32" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B64" s="32" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C64" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D64" s="32" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="33" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B65" s="33" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C65" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D65" s="33" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="32" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B66" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C66" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D66" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -12519,44 +12519,44 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="33" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B69" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C69" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D69" s="33" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="32" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B70" s="32" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C70" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D70" s="32" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="33" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B71" s="33" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C71" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D71" s="33" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
before changing condition to include pfdetails
</commit_message>
<xml_diff>
--- a/data/inputs/Asset Model - Demo.xlsx
+++ b/data/inputs/Asset Model - Demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtreseder\OneDrive - KPMG\Documents\3. Client\Essential Energy\Probability of Failure Model\pof\data\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1824" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D002E248-A21D-4931-B70D-336D0596AB94}"/>
+  <xr:revisionPtr revIDLastSave="1831" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{595A6006-CDB7-4FE1-A362-4D586C916F8F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -202,7 +202,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="333">
   <si>
     <t>Cause</t>
   </si>
@@ -3618,8 +3618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA0734F-FFBE-4DAF-BDE5-A12359370A0D}">
   <dimension ref="A1:AV84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="XFD1" sqref="AW1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>
@@ -3662,22 +3662,33 @@
     <col min="47" max="47" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" s="1" customFormat="1">
+    <row r="1" spans="1:48">
+      <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="C1" s="1"/>
       <c r="D1" s="95"/>
       <c r="E1" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
       <c r="H1" s="95"/>
       <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
       <c r="O1" s="95"/>
       <c r="P1" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
       <c r="S1" s="95"/>
       <c r="T1" s="25" t="s">
         <v>42</v>
@@ -3715,7 +3726,8 @@
       <c r="AU1" s="67"/>
       <c r="AV1" s="67"/>
     </row>
-    <row r="2" spans="1:48" s="1" customFormat="1">
+    <row r="2" spans="1:48">
+      <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>45</v>
       </c>
@@ -3728,6 +3740,8 @@
       <c r="E2" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
       <c r="H2" s="95"/>
       <c r="I2" s="1" t="s">
         <v>48</v>
@@ -3735,10 +3749,16 @@
       <c r="J2" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
       <c r="O2" s="95"/>
       <c r="P2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
       <c r="S2" s="95"/>
       <c r="T2" s="25" t="s">
         <v>50</v>
@@ -3786,7 +3806,7 @@
       <c r="AU2" s="67"/>
       <c r="AV2" s="67"/>
     </row>
-    <row r="3" spans="1:48" s="1" customFormat="1">
+    <row r="3" spans="1:48">
       <c r="A3" s="1" t="s">
         <v>55</v>
       </c>
@@ -3932,12 +3952,40 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:48" s="59" customFormat="1" ht="12" customHeight="1">
+    <row r="4" spans="1:48" ht="12" customHeight="1">
+      <c r="A4" s="59"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="96"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
       <c r="H4" s="96"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
       <c r="O4" s="96"/>
+      <c r="P4" s="59"/>
+      <c r="Q4" s="59"/>
+      <c r="R4" s="59"/>
       <c r="S4" s="96"/>
+      <c r="T4" s="59"/>
+      <c r="U4" s="59"/>
+      <c r="V4" s="59"/>
+      <c r="W4" s="59"/>
+      <c r="X4" s="59"/>
+      <c r="Y4" s="59"/>
+      <c r="Z4" s="59"/>
+      <c r="AA4" s="59"/>
+      <c r="AB4" s="59"/>
+      <c r="AC4" s="59"/>
       <c r="AD4" s="96"/>
+      <c r="AE4" s="59"/>
+      <c r="AF4" s="59"/>
+      <c r="AG4" s="59"/>
       <c r="AH4" s="61"/>
       <c r="AI4" s="61"/>
       <c r="AJ4" s="61"/>
@@ -3951,8 +3999,13 @@
       <c r="AR4" s="127"/>
       <c r="AS4" s="73"/>
       <c r="AT4" s="62"/>
-    </row>
-    <row r="5" spans="1:48" s="15" customFormat="1">
+      <c r="AU4" s="59"/>
+      <c r="AV4" s="59"/>
+    </row>
+    <row r="5" spans="1:48">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
       <c r="D5" s="97" t="s">
         <v>28</v>
       </c>
@@ -3992,6 +4045,8 @@
       <c r="P5" s="15" t="s">
         <v>38</v>
       </c>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
       <c r="S5" s="97"/>
       <c r="T5" s="15" t="s">
         <v>79</v>
@@ -4020,6 +4075,7 @@
       <c r="AB5" s="41">
         <v>5</v>
       </c>
+      <c r="AC5" s="15"/>
       <c r="AD5" s="97" t="s">
         <v>82</v>
       </c>
@@ -4058,7 +4114,10 @@
       <c r="AU5" s="18"/>
       <c r="AV5" s="18"/>
     </row>
-    <row r="6" spans="1:48" s="15" customFormat="1">
+    <row r="6" spans="1:48">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="97"/>
       <c r="E6" t="s">
         <v>38</v>
@@ -4072,16 +4131,39 @@
       <c r="H6" s="98">
         <v>0</v>
       </c>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
       <c r="O6" s="97"/>
       <c r="P6" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="S6" s="97"/>
+      <c r="Q6" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="R6" s="15">
+        <v>6</v>
+      </c>
+      <c r="S6" s="97">
+        <v>1</v>
+      </c>
+      <c r="T6" s="15"/>
       <c r="U6" s="45"/>
       <c r="V6" s="45"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
       <c r="AA6" s="41"/>
       <c r="AB6" s="41"/>
+      <c r="AC6" s="15"/>
       <c r="AD6" s="97"/>
+      <c r="AE6" s="15"/>
+      <c r="AF6" s="15"/>
+      <c r="AG6" s="15"/>
       <c r="AH6" s="18"/>
       <c r="AI6" s="18"/>
       <c r="AJ6" s="18"/>
@@ -4104,7 +4186,7 @@
       <c r="AU6" s="18"/>
       <c r="AV6" s="18"/>
     </row>
-    <row r="7" spans="1:48" s="47" customFormat="1">
+    <row r="7" spans="1:48">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
@@ -4162,7 +4244,10 @@
       <c r="AU7" s="69"/>
       <c r="AV7" s="69"/>
     </row>
-    <row r="8" spans="1:48" s="15" customFormat="1">
+    <row r="8" spans="1:48">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
       <c r="D8" s="97"/>
       <c r="E8" t="s">
         <v>87</v>
@@ -4176,7 +4261,16 @@
       <c r="H8" s="98">
         <v>1</v>
       </c>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
       <c r="O8" s="97"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
       <c r="S8" s="97"/>
       <c r="T8" s="15" t="s">
         <v>89</v>
@@ -4199,10 +4293,15 @@
       <c r="Z8" s="15" t="s">
         <v>92</v>
       </c>
+      <c r="AA8" s="15"/>
+      <c r="AB8" s="15"/>
       <c r="AC8" s="15" t="s">
         <v>93</v>
       </c>
       <c r="AD8" s="97"/>
+      <c r="AE8" s="15"/>
+      <c r="AF8" s="15"/>
+      <c r="AG8" s="15"/>
       <c r="AH8" s="16" t="b">
         <v>1</v>
       </c>
@@ -4245,7 +4344,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:48" s="15" customFormat="1">
+    <row r="9" spans="1:48">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="97"/>
       <c r="E9" s="15" t="s">
         <v>97</v>
@@ -4259,9 +4361,31 @@
       <c r="H9" s="97" t="b">
         <v>0</v>
       </c>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
       <c r="O9" s="97"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
       <c r="S9" s="97"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
+      <c r="AA9" s="15"/>
+      <c r="AB9" s="15"/>
+      <c r="AC9" s="15"/>
       <c r="AD9" s="97"/>
+      <c r="AE9" s="15"/>
+      <c r="AF9" s="15"/>
+      <c r="AG9" s="15"/>
       <c r="AH9" s="16"/>
       <c r="AI9" s="16"/>
       <c r="AJ9" s="16"/>
@@ -4281,8 +4405,10 @@
       <c r="AR9" s="111"/>
       <c r="AS9" s="76"/>
       <c r="AT9" s="19"/>
-    </row>
-    <row r="10" spans="1:48" s="47" customFormat="1">
+      <c r="AU9" s="15"/>
+      <c r="AV9" s="15"/>
+    </row>
+    <row r="10" spans="1:48">
       <c r="A10" s="15"/>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
@@ -4340,7 +4466,10 @@
       <c r="AU10" s="69"/>
       <c r="AV10" s="69"/>
     </row>
-    <row r="11" spans="1:48" s="15" customFormat="1">
+    <row r="11" spans="1:48">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
       <c r="D11" s="97"/>
       <c r="E11" s="15" t="s">
         <v>100</v>
@@ -4354,7 +4483,16 @@
       <c r="H11" s="97" t="b">
         <v>0</v>
       </c>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
       <c r="O11" s="97"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
       <c r="S11" s="97"/>
       <c r="T11" s="15" t="s">
         <v>101</v>
@@ -4377,10 +4515,15 @@
       <c r="Z11" s="15" t="s">
         <v>103</v>
       </c>
+      <c r="AA11" s="15"/>
+      <c r="AB11" s="15"/>
       <c r="AC11" s="15" t="s">
         <v>6</v>
       </c>
       <c r="AD11" s="97"/>
+      <c r="AE11" s="15"/>
+      <c r="AF11" s="15"/>
+      <c r="AG11" s="15"/>
       <c r="AH11" s="16" t="b">
         <v>1</v>
       </c>
@@ -4423,7 +4566,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:48" s="15" customFormat="1">
+    <row r="12" spans="1:48">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
       <c r="D12" s="97"/>
       <c r="E12" s="15" t="s">
         <v>104</v>
@@ -4437,9 +4583,35 @@
       <c r="H12" s="97" t="b">
         <v>0</v>
       </c>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
       <c r="O12" s="97"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
       <c r="S12" s="97"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
+      <c r="V12" s="15"/>
+      <c r="W12" s="15"/>
+      <c r="X12" s="15"/>
+      <c r="Y12" s="15"/>
+      <c r="Z12" s="15"/>
+      <c r="AA12" s="15"/>
+      <c r="AB12" s="15"/>
+      <c r="AC12" s="15"/>
       <c r="AD12" s="97"/>
+      <c r="AE12" s="15"/>
+      <c r="AF12" s="15"/>
+      <c r="AG12" s="15"/>
+      <c r="AH12" s="15"/>
+      <c r="AI12" s="15"/>
+      <c r="AJ12" s="15"/>
+      <c r="AK12" s="15"/>
       <c r="AL12" s="97"/>
       <c r="AM12" s="82" t="s">
         <v>38</v>
@@ -4455,6 +4627,8 @@
       <c r="AR12" s="111"/>
       <c r="AS12" s="76"/>
       <c r="AT12" s="19"/>
+      <c r="AU12" s="15"/>
+      <c r="AV12" s="15"/>
     </row>
     <row r="13" spans="1:48">
       <c r="A13" s="15"/>
@@ -4466,7 +4640,7 @@
       <c r="AN13" s="80"/>
       <c r="AO13" s="120"/>
     </row>
-    <row r="14" spans="1:48" s="47" customFormat="1">
+    <row r="14" spans="1:48">
       <c r="A14" s="15"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
@@ -4516,10 +4690,25 @@
       <c r="AU14" s="69"/>
       <c r="AV14" s="69"/>
     </row>
-    <row r="15" spans="1:48" s="15" customFormat="1">
+    <row r="15" spans="1:48">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
       <c r="D15" s="97"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
       <c r="H15" s="97"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
       <c r="O15" s="97"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
       <c r="S15" s="97"/>
       <c r="T15" s="15" t="s">
         <v>106</v>
@@ -4542,10 +4731,15 @@
       <c r="Z15" s="15" t="s">
         <v>103</v>
       </c>
+      <c r="AA15" s="15"/>
+      <c r="AB15" s="15"/>
       <c r="AC15" s="15" t="s">
         <v>6</v>
       </c>
       <c r="AD15" s="97"/>
+      <c r="AE15" s="15"/>
+      <c r="AF15" s="15"/>
+      <c r="AG15" s="15"/>
       <c r="AH15" s="16"/>
       <c r="AI15" s="16"/>
       <c r="AJ15" s="16" t="b">
@@ -4578,7 +4772,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:48" s="56" customFormat="1">
+    <row r="16" spans="1:48">
       <c r="A16" s="15"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
@@ -4587,9 +4781,31 @@
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
       <c r="H16" s="97"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="56"/>
+      <c r="M16" s="56"/>
+      <c r="N16" s="56"/>
       <c r="O16" s="103"/>
+      <c r="P16" s="56"/>
+      <c r="Q16" s="56"/>
+      <c r="R16" s="56"/>
       <c r="S16" s="103"/>
+      <c r="T16" s="56"/>
+      <c r="U16" s="56"/>
+      <c r="V16" s="56"/>
+      <c r="W16" s="56"/>
+      <c r="X16" s="56"/>
+      <c r="Y16" s="56"/>
+      <c r="Z16" s="56"/>
+      <c r="AA16" s="56"/>
+      <c r="AB16" s="56"/>
+      <c r="AC16" s="56"/>
       <c r="AD16" s="103"/>
+      <c r="AE16" s="56"/>
+      <c r="AF16" s="56"/>
+      <c r="AG16" s="56"/>
       <c r="AH16" s="57"/>
       <c r="AI16" s="57"/>
       <c r="AJ16" s="57"/>
@@ -4603,9 +4819,17 @@
       <c r="AR16" s="113"/>
       <c r="AS16" s="78"/>
       <c r="AT16" s="58"/>
-    </row>
-    <row r="17" spans="1:48" s="15" customFormat="1">
+      <c r="AU16" s="56"/>
+      <c r="AV16" s="56"/>
+    </row>
+    <row r="17" spans="1:48">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
       <c r="D17" s="97"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
       <c r="H17" s="97"/>
       <c r="I17" s="15" t="s">
         <v>107</v>
@@ -4631,6 +4855,8 @@
       <c r="P17" s="15" t="s">
         <v>38</v>
       </c>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
       <c r="S17" s="97"/>
       <c r="T17" s="15" t="s">
         <v>79</v>
@@ -4650,12 +4876,14 @@
       <c r="Y17" s="15" t="s">
         <v>80</v>
       </c>
+      <c r="Z17" s="15"/>
       <c r="AA17" s="15">
         <v>20</v>
       </c>
       <c r="AB17" s="15">
         <v>5</v>
       </c>
+      <c r="AC17" s="15"/>
       <c r="AD17" s="97" t="s">
         <v>82</v>
       </c>
@@ -4686,11 +4914,24 @@
       <c r="AU17" s="18"/>
       <c r="AV17" s="18"/>
     </row>
-    <row r="18" spans="1:48" s="15" customFormat="1">
+    <row r="18" spans="1:48">
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
       <c r="D18" s="97"/>
-      <c r="F18"/>
+      <c r="E18" s="15"/>
+      <c r="G18" s="15"/>
       <c r="H18" s="97"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
       <c r="O18" s="97"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
       <c r="S18" s="97"/>
       <c r="T18" s="69"/>
       <c r="U18" s="69"/>
@@ -4722,11 +4963,24 @@
       <c r="AU18" s="69"/>
       <c r="AV18" s="69"/>
     </row>
-    <row r="19" spans="1:48" s="15" customFormat="1">
+    <row r="19" spans="1:48">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
       <c r="D19" s="97"/>
-      <c r="F19"/>
+      <c r="E19" s="15"/>
+      <c r="G19" s="15"/>
       <c r="H19" s="97"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
       <c r="O19" s="97"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
       <c r="S19" s="97"/>
       <c r="T19" s="15" t="s">
         <v>101</v>
@@ -4749,10 +5003,15 @@
       <c r="Z19" s="15" t="s">
         <v>103</v>
       </c>
+      <c r="AA19" s="15"/>
+      <c r="AB19" s="15"/>
       <c r="AC19" s="15" t="s">
         <v>6</v>
       </c>
       <c r="AD19" s="97"/>
+      <c r="AE19" s="15"/>
+      <c r="AF19" s="15"/>
+      <c r="AG19" s="15"/>
       <c r="AH19" s="16" t="b">
         <v>1</v>
       </c>
@@ -4795,15 +5054,41 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:48" s="15" customFormat="1">
+    <row r="20" spans="1:48">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
       <c r="D20" s="97"/>
-      <c r="E20"/>
-      <c r="F20"/>
-      <c r="G20"/>
       <c r="H20" s="97"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
       <c r="O20" s="97"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
       <c r="S20" s="97"/>
+      <c r="T20" s="15"/>
+      <c r="U20" s="15"/>
+      <c r="V20" s="15"/>
+      <c r="W20" s="15"/>
+      <c r="X20" s="15"/>
+      <c r="Y20" s="15"/>
+      <c r="Z20" s="15"/>
+      <c r="AA20" s="15"/>
+      <c r="AB20" s="15"/>
+      <c r="AC20" s="15"/>
       <c r="AD20" s="97"/>
+      <c r="AE20" s="15"/>
+      <c r="AF20" s="15"/>
+      <c r="AG20" s="15"/>
+      <c r="AH20" s="15"/>
+      <c r="AI20" s="15"/>
+      <c r="AJ20" s="15"/>
+      <c r="AK20" s="15"/>
       <c r="AL20" s="97"/>
       <c r="AM20" s="84" t="s">
         <v>38</v>
@@ -4819,44 +5104,12 @@
       <c r="AR20" s="111"/>
       <c r="AS20" s="76"/>
       <c r="AT20" s="19"/>
-    </row>
-    <row r="21" spans="1:48" s="15" customFormat="1">
-      <c r="C21"/>
-      <c r="D21" s="98"/>
-      <c r="E21"/>
-      <c r="F21"/>
-      <c r="G21"/>
-      <c r="H21" s="98"/>
-      <c r="I21"/>
-      <c r="J21"/>
-      <c r="K21"/>
-      <c r="L21"/>
-      <c r="M21"/>
-      <c r="N21"/>
-      <c r="O21" s="98"/>
-      <c r="P21"/>
-      <c r="Q21"/>
-      <c r="R21"/>
-      <c r="S21" s="98"/>
-      <c r="T21"/>
-      <c r="U21"/>
-      <c r="V21"/>
-      <c r="W21"/>
-      <c r="X21"/>
-      <c r="Y21"/>
-      <c r="Z21"/>
-      <c r="AA21"/>
-      <c r="AB21"/>
-      <c r="AC21"/>
-      <c r="AD21" s="98"/>
-      <c r="AE21"/>
-      <c r="AF21"/>
-      <c r="AG21"/>
-      <c r="AH21" s="17"/>
-      <c r="AI21" s="17"/>
-      <c r="AJ21" s="17"/>
-      <c r="AK21" s="17"/>
-      <c r="AL21" s="112"/>
+      <c r="AU20" s="15"/>
+      <c r="AV20" s="15"/>
+    </row>
+    <row r="21" spans="1:48">
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
       <c r="AM21" s="84" t="s">
         <v>37</v>
       </c>
@@ -4866,32 +5119,10 @@
       <c r="AO21" s="123">
         <v>3</v>
       </c>
-      <c r="AP21" s="17"/>
-      <c r="AQ21" s="17"/>
-      <c r="AR21" s="112"/>
-      <c r="AS21" s="77"/>
-      <c r="AT21" s="20"/>
-      <c r="AU21"/>
-      <c r="AV21"/>
-    </row>
-    <row r="22" spans="1:48" s="15" customFormat="1">
-      <c r="C22"/>
-      <c r="D22" s="98"/>
-      <c r="E22"/>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22" s="98"/>
-      <c r="I22"/>
-      <c r="J22"/>
-      <c r="K22"/>
-      <c r="L22"/>
-      <c r="M22"/>
-      <c r="N22"/>
-      <c r="O22" s="98"/>
-      <c r="P22"/>
-      <c r="Q22"/>
-      <c r="R22"/>
-      <c r="S22" s="98"/>
+    </row>
+    <row r="22" spans="1:48">
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
       <c r="T22" s="69"/>
       <c r="U22" s="69"/>
       <c r="V22" s="69"/>
@@ -4922,21 +5153,12 @@
       <c r="AU22" s="69"/>
       <c r="AV22" s="69"/>
     </row>
-    <row r="23" spans="1:48" s="15" customFormat="1">
-      <c r="C23"/>
-      <c r="D23" s="98"/>
-      <c r="H23" s="98"/>
-      <c r="I23"/>
-      <c r="J23"/>
-      <c r="K23"/>
-      <c r="L23"/>
-      <c r="M23"/>
-      <c r="N23"/>
-      <c r="O23" s="98"/>
-      <c r="P23"/>
-      <c r="Q23"/>
-      <c r="R23"/>
-      <c r="S23" s="98"/>
+    <row r="23" spans="1:48">
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
       <c r="T23" s="15" t="s">
         <v>106</v>
       </c>
@@ -4958,10 +5180,15 @@
       <c r="Z23" s="15" t="s">
         <v>103</v>
       </c>
+      <c r="AA23" s="15"/>
+      <c r="AB23" s="15"/>
       <c r="AC23" s="15" t="s">
         <v>6</v>
       </c>
       <c r="AD23" s="97"/>
+      <c r="AE23" s="15"/>
+      <c r="AF23" s="15"/>
+      <c r="AG23" s="15"/>
       <c r="AH23" s="16"/>
       <c r="AI23" s="16"/>
       <c r="AJ23" s="16" t="b">
@@ -4994,7 +5221,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:48" s="56" customFormat="1">
+    <row r="24" spans="1:48">
       <c r="A24" s="15"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -5003,9 +5230,31 @@
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
       <c r="H24" s="97"/>
+      <c r="I24" s="56"/>
+      <c r="J24" s="56"/>
+      <c r="K24" s="56"/>
+      <c r="L24" s="56"/>
+      <c r="M24" s="56"/>
+      <c r="N24" s="56"/>
       <c r="O24" s="103"/>
+      <c r="P24" s="56"/>
+      <c r="Q24" s="56"/>
+      <c r="R24" s="56"/>
       <c r="S24" s="103"/>
+      <c r="T24" s="56"/>
+      <c r="U24" s="56"/>
+      <c r="V24" s="56"/>
+      <c r="W24" s="56"/>
+      <c r="X24" s="56"/>
+      <c r="Y24" s="56"/>
+      <c r="Z24" s="56"/>
+      <c r="AA24" s="56"/>
+      <c r="AB24" s="56"/>
+      <c r="AC24" s="56"/>
       <c r="AD24" s="103"/>
+      <c r="AE24" s="56"/>
+      <c r="AF24" s="56"/>
+      <c r="AG24" s="56"/>
       <c r="AH24" s="57"/>
       <c r="AI24" s="57"/>
       <c r="AJ24" s="57"/>
@@ -5019,9 +5268,17 @@
       <c r="AR24" s="113"/>
       <c r="AS24" s="78"/>
       <c r="AT24" s="58"/>
-    </row>
-    <row r="25" spans="1:48" s="15" customFormat="1">
+      <c r="AU24" s="56"/>
+      <c r="AV24" s="56"/>
+    </row>
+    <row r="25" spans="1:48">
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
       <c r="D25" s="97"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
       <c r="H25" s="97"/>
       <c r="I25" s="15" t="s">
         <v>108</v>
@@ -5047,6 +5304,8 @@
       <c r="P25" s="15" t="s">
         <v>32</v>
       </c>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="15"/>
       <c r="S25" s="97"/>
       <c r="T25" s="15" t="s">
         <v>79</v>
@@ -5075,6 +5334,7 @@
       <c r="AB25" s="15">
         <v>5</v>
       </c>
+      <c r="AC25" s="15"/>
       <c r="AD25" s="97" t="s">
         <v>82</v>
       </c>
@@ -5105,11 +5365,24 @@
       <c r="AU25" s="18"/>
       <c r="AV25" s="18"/>
     </row>
-    <row r="26" spans="1:48" s="15" customFormat="1">
+    <row r="26" spans="1:48">
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
       <c r="D26" s="97"/>
-      <c r="F26"/>
+      <c r="E26" s="15"/>
+      <c r="G26" s="15"/>
       <c r="H26" s="97"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
       <c r="O26" s="97"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="15"/>
       <c r="S26" s="97"/>
       <c r="T26" s="69"/>
       <c r="U26" s="69"/>
@@ -5141,11 +5414,24 @@
       <c r="AU26" s="69"/>
       <c r="AV26" s="69"/>
     </row>
-    <row r="27" spans="1:48" s="15" customFormat="1">
+    <row r="27" spans="1:48">
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
       <c r="D27" s="97"/>
-      <c r="F27"/>
+      <c r="E27" s="15"/>
+      <c r="G27" s="15"/>
       <c r="H27" s="97"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
       <c r="O27" s="97"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
+      <c r="R27" s="15"/>
       <c r="S27" s="97"/>
       <c r="T27" s="15" t="s">
         <v>109</v>
@@ -5168,7 +5454,13 @@
       <c r="Z27" s="15" t="s">
         <v>81</v>
       </c>
+      <c r="AA27" s="15"/>
+      <c r="AB27" s="15"/>
+      <c r="AC27" s="15"/>
       <c r="AD27" s="97"/>
+      <c r="AE27" s="15"/>
+      <c r="AF27" s="15"/>
+      <c r="AG27" s="15"/>
       <c r="AH27" s="16" t="b">
         <v>1</v>
       </c>
@@ -5203,13 +5495,39 @@
       <c r="AU27" s="18"/>
       <c r="AV27" s="18"/>
     </row>
-    <row r="28" spans="1:48" s="15" customFormat="1">
+    <row r="28" spans="1:48">
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
       <c r="D28" s="97"/>
-      <c r="F28"/>
+      <c r="E28" s="15"/>
+      <c r="G28" s="15"/>
       <c r="H28" s="97"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
       <c r="O28" s="97"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
       <c r="S28" s="97"/>
+      <c r="T28" s="15"/>
+      <c r="U28" s="15"/>
+      <c r="V28" s="15"/>
+      <c r="W28" s="15"/>
+      <c r="X28" s="15"/>
+      <c r="Y28" s="15"/>
+      <c r="Z28" s="15"/>
+      <c r="AA28" s="15"/>
+      <c r="AB28" s="15"/>
+      <c r="AC28" s="15"/>
       <c r="AD28" s="97"/>
+      <c r="AE28" s="15"/>
+      <c r="AF28" s="15"/>
+      <c r="AG28" s="15"/>
       <c r="AH28" s="16"/>
       <c r="AI28" s="16"/>
       <c r="AJ28" s="16"/>
@@ -5229,12 +5547,27 @@
       <c r="AR28" s="111"/>
       <c r="AS28" s="76"/>
       <c r="AT28" s="19"/>
-    </row>
-    <row r="29" spans="1:48" s="15" customFormat="1">
+      <c r="AU28" s="15"/>
+      <c r="AV28" s="15"/>
+    </row>
+    <row r="29" spans="1:48">
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
       <c r="D29" s="97"/>
-      <c r="F29"/>
+      <c r="E29" s="15"/>
+      <c r="G29" s="15"/>
       <c r="H29" s="97"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
       <c r="O29" s="97"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="15"/>
+      <c r="R29" s="15"/>
       <c r="S29" s="97"/>
       <c r="T29" s="69"/>
       <c r="U29" s="69"/>
@@ -5266,11 +5599,24 @@
       <c r="AU29" s="69"/>
       <c r="AV29" s="69"/>
     </row>
-    <row r="30" spans="1:48" s="15" customFormat="1">
+    <row r="30" spans="1:48">
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
       <c r="D30" s="97"/>
-      <c r="F30"/>
+      <c r="E30" s="15"/>
+      <c r="G30" s="15"/>
       <c r="H30" s="97"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
       <c r="O30" s="97"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="15"/>
       <c r="S30" s="97"/>
       <c r="T30" s="15" t="s">
         <v>101</v>
@@ -5293,10 +5639,15 @@
       <c r="Z30" s="15" t="s">
         <v>103</v>
       </c>
+      <c r="AA30" s="15"/>
+      <c r="AB30" s="15"/>
       <c r="AC30" s="15" t="s">
         <v>6</v>
       </c>
       <c r="AD30" s="97"/>
+      <c r="AE30" s="15"/>
+      <c r="AF30" s="15"/>
+      <c r="AG30" s="15"/>
       <c r="AH30" s="16" t="b">
         <v>1</v>
       </c>
@@ -5339,15 +5690,41 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:48" s="15" customFormat="1">
+    <row r="31" spans="1:48">
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
       <c r="D31" s="97"/>
-      <c r="E31"/>
-      <c r="F31"/>
-      <c r="G31"/>
       <c r="H31" s="97"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
       <c r="O31" s="97"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="15"/>
       <c r="S31" s="97"/>
+      <c r="T31" s="15"/>
+      <c r="U31" s="15"/>
+      <c r="V31" s="15"/>
+      <c r="W31" s="15"/>
+      <c r="X31" s="15"/>
+      <c r="Y31" s="15"/>
+      <c r="Z31" s="15"/>
+      <c r="AA31" s="15"/>
+      <c r="AB31" s="15"/>
+      <c r="AC31" s="15"/>
       <c r="AD31" s="97"/>
+      <c r="AE31" s="15"/>
+      <c r="AF31" s="15"/>
+      <c r="AG31" s="15"/>
+      <c r="AH31" s="15"/>
+      <c r="AI31" s="15"/>
+      <c r="AJ31" s="15"/>
+      <c r="AK31" s="15"/>
       <c r="AL31" s="97"/>
       <c r="AM31" s="84" t="s">
         <v>38</v>
@@ -5363,44 +5740,12 @@
       <c r="AR31" s="111"/>
       <c r="AS31" s="76"/>
       <c r="AT31" s="19"/>
-    </row>
-    <row r="32" spans="1:48" s="15" customFormat="1">
-      <c r="C32"/>
-      <c r="D32" s="98"/>
-      <c r="E32"/>
-      <c r="F32"/>
-      <c r="G32"/>
-      <c r="H32" s="98"/>
-      <c r="I32"/>
-      <c r="J32"/>
-      <c r="K32"/>
-      <c r="L32"/>
-      <c r="M32"/>
-      <c r="N32"/>
-      <c r="O32" s="98"/>
-      <c r="P32"/>
-      <c r="Q32"/>
-      <c r="R32"/>
-      <c r="S32" s="98"/>
-      <c r="T32"/>
-      <c r="U32"/>
-      <c r="V32"/>
-      <c r="W32"/>
-      <c r="X32"/>
-      <c r="Y32"/>
-      <c r="Z32"/>
-      <c r="AA32"/>
-      <c r="AB32"/>
-      <c r="AC32"/>
-      <c r="AD32" s="98"/>
-      <c r="AE32"/>
-      <c r="AF32"/>
-      <c r="AG32"/>
-      <c r="AH32" s="17"/>
-      <c r="AI32" s="17"/>
-      <c r="AJ32" s="17"/>
-      <c r="AK32" s="17"/>
-      <c r="AL32" s="112"/>
+      <c r="AU31" s="15"/>
+      <c r="AV31" s="15"/>
+    </row>
+    <row r="32" spans="1:48">
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
       <c r="AM32" s="84" t="s">
         <v>37</v>
       </c>
@@ -5410,32 +5755,10 @@
       <c r="AO32" s="123">
         <v>3</v>
       </c>
-      <c r="AP32" s="17"/>
-      <c r="AQ32" s="17"/>
-      <c r="AR32" s="112"/>
-      <c r="AS32" s="77"/>
-      <c r="AT32" s="20"/>
-      <c r="AU32"/>
-      <c r="AV32"/>
-    </row>
-    <row r="33" spans="1:48" s="15" customFormat="1">
-      <c r="C33"/>
-      <c r="D33" s="98"/>
-      <c r="E33"/>
-      <c r="F33"/>
-      <c r="G33"/>
-      <c r="H33" s="98"/>
-      <c r="I33"/>
-      <c r="J33"/>
-      <c r="K33"/>
-      <c r="L33"/>
-      <c r="M33"/>
-      <c r="N33"/>
-      <c r="O33" s="98"/>
-      <c r="P33"/>
-      <c r="Q33"/>
-      <c r="R33"/>
-      <c r="S33" s="98"/>
+    </row>
+    <row r="33" spans="1:48">
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
       <c r="T33" s="69"/>
       <c r="U33" s="69"/>
       <c r="V33" s="69"/>
@@ -5466,21 +5789,12 @@
       <c r="AU33" s="69"/>
       <c r="AV33" s="69"/>
     </row>
-    <row r="34" spans="1:48" s="15" customFormat="1">
-      <c r="C34"/>
-      <c r="D34" s="98"/>
-      <c r="H34" s="98"/>
-      <c r="I34"/>
-      <c r="J34"/>
-      <c r="K34"/>
-      <c r="L34"/>
-      <c r="M34"/>
-      <c r="N34"/>
-      <c r="O34" s="98"/>
-      <c r="P34"/>
-      <c r="Q34"/>
-      <c r="R34"/>
-      <c r="S34" s="98"/>
+    <row r="34" spans="1:48">
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
       <c r="T34" s="15" t="s">
         <v>106</v>
       </c>
@@ -5502,10 +5816,15 @@
       <c r="Z34" s="15" t="s">
         <v>103</v>
       </c>
+      <c r="AA34" s="15"/>
+      <c r="AB34" s="15"/>
       <c r="AC34" s="15" t="s">
         <v>6</v>
       </c>
       <c r="AD34" s="97"/>
+      <c r="AE34" s="15"/>
+      <c r="AF34" s="15"/>
+      <c r="AG34" s="15"/>
       <c r="AH34" s="16"/>
       <c r="AI34" s="16"/>
       <c r="AJ34" s="16" t="b">
@@ -5538,7 +5857,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:48" s="56" customFormat="1">
+    <row r="35" spans="1:48">
       <c r="A35" s="15"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -5547,9 +5866,31 @@
       <c r="F35" s="15"/>
       <c r="G35" s="15"/>
       <c r="H35" s="97"/>
+      <c r="I35" s="56"/>
+      <c r="J35" s="56"/>
+      <c r="K35" s="56"/>
+      <c r="L35" s="56"/>
+      <c r="M35" s="56"/>
+      <c r="N35" s="56"/>
       <c r="O35" s="103"/>
+      <c r="P35" s="56"/>
+      <c r="Q35" s="56"/>
+      <c r="R35" s="56"/>
       <c r="S35" s="103"/>
+      <c r="T35" s="56"/>
+      <c r="U35" s="56"/>
+      <c r="V35" s="56"/>
+      <c r="W35" s="56"/>
+      <c r="X35" s="56"/>
+      <c r="Y35" s="56"/>
+      <c r="Z35" s="56"/>
+      <c r="AA35" s="56"/>
+      <c r="AB35" s="56"/>
+      <c r="AC35" s="56"/>
       <c r="AD35" s="103"/>
+      <c r="AE35" s="56"/>
+      <c r="AF35" s="56"/>
+      <c r="AG35" s="56"/>
       <c r="AH35" s="57"/>
       <c r="AI35" s="57"/>
       <c r="AJ35" s="57"/>
@@ -5563,9 +5904,17 @@
       <c r="AR35" s="113"/>
       <c r="AS35" s="78"/>
       <c r="AT35" s="58"/>
-    </row>
-    <row r="36" spans="1:48" s="15" customFormat="1">
+      <c r="AU35" s="56"/>
+      <c r="AV35" s="56"/>
+    </row>
+    <row r="36" spans="1:48">
+      <c r="A36" s="15"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
       <c r="D36" s="97"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
       <c r="H36" s="97"/>
       <c r="I36" s="15" t="s">
         <v>110</v>
@@ -5613,9 +5962,15 @@
       <c r="Z36" s="15" t="s">
         <v>81</v>
       </c>
+      <c r="AA36" s="15"/>
+      <c r="AB36" s="15"/>
+      <c r="AC36" s="15"/>
       <c r="AD36" s="97" t="s">
         <v>111</v>
       </c>
+      <c r="AE36" s="15"/>
+      <c r="AF36" s="15"/>
+      <c r="AG36" s="15"/>
       <c r="AH36" s="18" t="b">
         <v>1</v>
       </c>
@@ -5637,11 +5992,28 @@
       <c r="AR36" s="107"/>
       <c r="AS36" s="76"/>
       <c r="AT36" s="19"/>
-    </row>
-    <row r="37" spans="1:48" s="15" customFormat="1">
+      <c r="AU36" s="15"/>
+      <c r="AV36" s="15"/>
+    </row>
+    <row r="37" spans="1:48">
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
       <c r="D37" s="97"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
       <c r="H37" s="97"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
       <c r="O37" s="97"/>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="15"/>
+      <c r="R37" s="15"/>
       <c r="S37" s="97"/>
       <c r="T37" s="69"/>
       <c r="U37" s="69"/>
@@ -5673,10 +6045,25 @@
       <c r="AU37" s="69"/>
       <c r="AV37" s="69"/>
     </row>
-    <row r="38" spans="1:48" s="15" customFormat="1">
+    <row r="38" spans="1:48">
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
       <c r="D38" s="97"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
       <c r="H38" s="97"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
       <c r="O38" s="97"/>
+      <c r="P38" s="15"/>
+      <c r="Q38" s="15"/>
+      <c r="R38" s="15"/>
       <c r="S38" s="97"/>
       <c r="T38" s="15" t="s">
         <v>79</v>
@@ -5696,12 +6083,14 @@
       <c r="Y38" s="15" t="s">
         <v>80</v>
       </c>
+      <c r="Z38" s="15"/>
       <c r="AA38" s="15">
         <v>20</v>
       </c>
       <c r="AB38" s="15">
         <v>5</v>
       </c>
+      <c r="AC38" s="15"/>
       <c r="AD38" s="97" t="s">
         <v>82</v>
       </c>
@@ -5738,10 +6127,25 @@
       <c r="AU38" s="18"/>
       <c r="AV38" s="18"/>
     </row>
-    <row r="39" spans="1:48" s="15" customFormat="1">
+    <row r="39" spans="1:48">
+      <c r="A39" s="15"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
       <c r="D39" s="97"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
       <c r="H39" s="97"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="15"/>
+      <c r="L39" s="15"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="15"/>
       <c r="O39" s="97"/>
+      <c r="P39" s="15"/>
+      <c r="Q39" s="15"/>
+      <c r="R39" s="15"/>
       <c r="S39" s="97"/>
       <c r="T39" s="69"/>
       <c r="U39" s="69"/>
@@ -5773,24 +6177,9 @@
       <c r="AU39" s="69"/>
       <c r="AV39" s="69"/>
     </row>
-    <row r="40" spans="1:48" s="15" customFormat="1">
-      <c r="C40"/>
-      <c r="D40" s="98"/>
-      <c r="E40"/>
-      <c r="F40"/>
-      <c r="G40"/>
-      <c r="H40" s="98"/>
-      <c r="I40"/>
-      <c r="J40"/>
-      <c r="K40"/>
-      <c r="L40"/>
-      <c r="M40"/>
-      <c r="N40"/>
-      <c r="O40" s="98"/>
-      <c r="P40"/>
-      <c r="Q40"/>
-      <c r="R40"/>
-      <c r="S40" s="98"/>
+    <row r="40" spans="1:48">
+      <c r="A40" s="15"/>
+      <c r="B40" s="15"/>
       <c r="T40" s="15" t="s">
         <v>106</v>
       </c>
@@ -5812,10 +6201,15 @@
       <c r="Z40" s="15" t="s">
         <v>103</v>
       </c>
+      <c r="AA40" s="15"/>
+      <c r="AB40" s="15"/>
       <c r="AC40" s="15" t="s">
         <v>6</v>
       </c>
       <c r="AD40" s="97"/>
+      <c r="AE40" s="15"/>
+      <c r="AF40" s="15"/>
+      <c r="AG40" s="15"/>
       <c r="AH40" s="16"/>
       <c r="AI40" s="16"/>
       <c r="AJ40" s="16" t="b">
@@ -5848,7 +6242,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:48" s="56" customFormat="1">
+    <row r="41" spans="1:48">
       <c r="A41" s="15"/>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
@@ -5857,9 +6251,31 @@
       <c r="F41" s="15"/>
       <c r="G41" s="15"/>
       <c r="H41" s="97"/>
+      <c r="I41" s="56"/>
+      <c r="J41" s="56"/>
+      <c r="K41" s="56"/>
+      <c r="L41" s="56"/>
+      <c r="M41" s="56"/>
+      <c r="N41" s="56"/>
       <c r="O41" s="103"/>
+      <c r="P41" s="56"/>
+      <c r="Q41" s="56"/>
+      <c r="R41" s="56"/>
       <c r="S41" s="103"/>
+      <c r="T41" s="56"/>
+      <c r="U41" s="56"/>
+      <c r="V41" s="56"/>
+      <c r="W41" s="56"/>
+      <c r="X41" s="56"/>
+      <c r="Y41" s="56"/>
+      <c r="Z41" s="56"/>
+      <c r="AA41" s="56"/>
+      <c r="AB41" s="56"/>
+      <c r="AC41" s="56"/>
       <c r="AD41" s="103"/>
+      <c r="AE41" s="56"/>
+      <c r="AF41" s="56"/>
+      <c r="AG41" s="56"/>
       <c r="AH41" s="57"/>
       <c r="AI41" s="57"/>
       <c r="AJ41" s="57"/>
@@ -5873,9 +6289,17 @@
       <c r="AR41" s="113"/>
       <c r="AS41" s="78"/>
       <c r="AT41" s="58"/>
-    </row>
-    <row r="42" spans="1:48" s="15" customFormat="1">
+      <c r="AU41" s="56"/>
+      <c r="AV41" s="56"/>
+    </row>
+    <row r="42" spans="1:48">
+      <c r="A42" s="15"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
       <c r="D42" s="97"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
       <c r="H42" s="97"/>
       <c r="I42" s="15" t="s">
         <v>99</v>
@@ -5898,6 +6322,9 @@
       <c r="O42" s="99">
         <v>1</v>
       </c>
+      <c r="P42" s="15"/>
+      <c r="Q42" s="15"/>
+      <c r="R42" s="15"/>
       <c r="S42" s="97"/>
       <c r="T42" s="15" t="s">
         <v>79</v>
@@ -5920,9 +6347,15 @@
       <c r="Z42" s="15" t="s">
         <v>81</v>
       </c>
+      <c r="AA42" s="15"/>
+      <c r="AB42" s="15"/>
+      <c r="AC42" s="15"/>
       <c r="AD42" s="97" t="s">
         <v>111</v>
       </c>
+      <c r="AE42" s="15"/>
+      <c r="AF42" s="15"/>
+      <c r="AG42" s="15"/>
       <c r="AH42" s="18" t="b">
         <v>1</v>
       </c>
@@ -5950,11 +6383,28 @@
       </c>
       <c r="AS42" s="76"/>
       <c r="AT42" s="19"/>
-    </row>
-    <row r="43" spans="1:48" s="15" customFormat="1">
+      <c r="AU42" s="15"/>
+      <c r="AV42" s="15"/>
+    </row>
+    <row r="43" spans="1:48">
+      <c r="A43" s="15"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="15"/>
       <c r="D43" s="97"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
       <c r="H43" s="97"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="15"/>
       <c r="O43" s="97"/>
+      <c r="P43" s="15"/>
+      <c r="Q43" s="15"/>
+      <c r="R43" s="15"/>
       <c r="S43" s="97"/>
       <c r="T43" s="69"/>
       <c r="U43" s="69"/>
@@ -5986,10 +6436,25 @@
       <c r="AU43" s="69"/>
       <c r="AV43" s="69"/>
     </row>
-    <row r="44" spans="1:48" s="15" customFormat="1">
+    <row r="44" spans="1:48">
+      <c r="A44" s="15"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="15"/>
       <c r="D44" s="97"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
       <c r="H44" s="97"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="15"/>
       <c r="O44" s="97"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="15"/>
+      <c r="R44" s="15"/>
       <c r="S44" s="97"/>
       <c r="T44" s="45" t="s">
         <v>101</v>
@@ -6012,10 +6477,15 @@
       <c r="Z44" s="15" t="s">
         <v>103</v>
       </c>
+      <c r="AA44" s="15"/>
+      <c r="AB44" s="15"/>
       <c r="AC44" s="15" t="s">
         <v>6</v>
       </c>
       <c r="AD44" s="97"/>
+      <c r="AE44" s="15"/>
+      <c r="AF44" s="15"/>
+      <c r="AG44" s="15"/>
       <c r="AH44" s="16" t="b">
         <v>1</v>
       </c>
@@ -6058,12 +6528,44 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:48" s="15" customFormat="1">
+    <row r="45" spans="1:48">
+      <c r="A45" s="15"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
       <c r="D45" s="97"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
       <c r="H45" s="97"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="15"/>
+      <c r="K45" s="15"/>
+      <c r="L45" s="15"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="15"/>
       <c r="O45" s="97"/>
+      <c r="P45" s="15"/>
+      <c r="Q45" s="15"/>
+      <c r="R45" s="15"/>
       <c r="S45" s="97"/>
+      <c r="T45" s="15"/>
+      <c r="U45" s="15"/>
+      <c r="V45" s="15"/>
+      <c r="W45" s="15"/>
+      <c r="X45" s="15"/>
+      <c r="Y45" s="15"/>
+      <c r="Z45" s="15"/>
+      <c r="AA45" s="15"/>
+      <c r="AB45" s="15"/>
+      <c r="AC45" s="15"/>
       <c r="AD45" s="97"/>
+      <c r="AE45" s="15"/>
+      <c r="AF45" s="15"/>
+      <c r="AG45" s="15"/>
+      <c r="AH45" s="15"/>
+      <c r="AI45" s="15"/>
+      <c r="AJ45" s="15"/>
+      <c r="AK45" s="15"/>
       <c r="AL45" s="97"/>
       <c r="AM45" s="82" t="s">
         <v>38</v>
@@ -6079,44 +6581,12 @@
       <c r="AR45" s="111"/>
       <c r="AS45" s="76"/>
       <c r="AT45" s="19"/>
-    </row>
-    <row r="46" spans="1:48" s="15" customFormat="1">
-      <c r="C46"/>
-      <c r="D46" s="98"/>
-      <c r="E46"/>
-      <c r="F46"/>
-      <c r="G46"/>
-      <c r="H46" s="98"/>
-      <c r="I46"/>
-      <c r="J46"/>
-      <c r="K46"/>
-      <c r="L46"/>
-      <c r="M46"/>
-      <c r="N46"/>
-      <c r="O46" s="98"/>
-      <c r="P46"/>
-      <c r="Q46"/>
-      <c r="R46"/>
-      <c r="S46" s="98"/>
-      <c r="T46"/>
-      <c r="U46"/>
-      <c r="V46"/>
-      <c r="W46"/>
-      <c r="X46"/>
-      <c r="Y46"/>
-      <c r="Z46"/>
-      <c r="AA46"/>
-      <c r="AB46"/>
-      <c r="AC46"/>
-      <c r="AD46" s="98"/>
-      <c r="AE46"/>
-      <c r="AF46"/>
-      <c r="AG46"/>
-      <c r="AH46" s="17"/>
-      <c r="AI46" s="17"/>
-      <c r="AJ46" s="17"/>
-      <c r="AK46" s="17"/>
-      <c r="AL46" s="112"/>
+      <c r="AU45" s="15"/>
+      <c r="AV45" s="15"/>
+    </row>
+    <row r="46" spans="1:48">
+      <c r="A46" s="15"/>
+      <c r="B46" s="15"/>
       <c r="AM46" s="82" t="s">
         <v>37</v>
       </c>
@@ -6126,32 +6596,10 @@
       <c r="AO46" s="120">
         <v>3</v>
       </c>
-      <c r="AP46" s="17"/>
-      <c r="AQ46" s="17"/>
-      <c r="AR46" s="112"/>
-      <c r="AS46" s="77"/>
-      <c r="AT46" s="20"/>
-      <c r="AU46"/>
-      <c r="AV46"/>
-    </row>
-    <row r="47" spans="1:48" s="15" customFormat="1">
-      <c r="C47"/>
-      <c r="D47" s="98"/>
-      <c r="E47"/>
-      <c r="F47"/>
-      <c r="G47"/>
-      <c r="H47" s="98"/>
-      <c r="I47"/>
-      <c r="J47"/>
-      <c r="K47"/>
-      <c r="L47"/>
-      <c r="M47"/>
-      <c r="N47"/>
-      <c r="O47" s="98"/>
-      <c r="P47"/>
-      <c r="Q47"/>
-      <c r="R47"/>
-      <c r="S47" s="98"/>
+    </row>
+    <row r="47" spans="1:48">
+      <c r="A47" s="15"/>
+      <c r="B47" s="15"/>
       <c r="T47" s="69"/>
       <c r="U47" s="69"/>
       <c r="V47" s="69"/>
@@ -6182,24 +6630,9 @@
       <c r="AU47" s="69"/>
       <c r="AV47" s="69"/>
     </row>
-    <row r="48" spans="1:48" s="15" customFormat="1">
-      <c r="C48"/>
-      <c r="D48" s="98"/>
-      <c r="E48"/>
-      <c r="F48"/>
-      <c r="G48"/>
-      <c r="H48" s="98"/>
-      <c r="I48"/>
-      <c r="J48"/>
-      <c r="K48"/>
-      <c r="L48"/>
-      <c r="M48"/>
-      <c r="N48"/>
-      <c r="O48" s="98"/>
-      <c r="P48"/>
-      <c r="Q48"/>
-      <c r="R48"/>
-      <c r="S48" s="98"/>
+    <row r="48" spans="1:48">
+      <c r="A48" s="15"/>
+      <c r="B48" s="15"/>
       <c r="T48" s="15" t="s">
         <v>106</v>
       </c>
@@ -6221,10 +6654,15 @@
       <c r="Z48" s="15" t="s">
         <v>103</v>
       </c>
+      <c r="AA48" s="15"/>
+      <c r="AB48" s="15"/>
       <c r="AC48" s="15" t="s">
         <v>6</v>
       </c>
       <c r="AD48" s="97"/>
+      <c r="AE48" s="15"/>
+      <c r="AF48" s="15"/>
+      <c r="AG48" s="15"/>
       <c r="AH48" s="16"/>
       <c r="AI48" s="16"/>
       <c r="AJ48" s="16" t="b">
@@ -6257,7 +6695,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:48" s="56" customFormat="1">
+    <row r="49" spans="1:48">
       <c r="A49" s="15"/>
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
@@ -6266,9 +6704,31 @@
       <c r="F49" s="15"/>
       <c r="G49" s="15"/>
       <c r="H49" s="97"/>
+      <c r="I49" s="56"/>
+      <c r="J49" s="56"/>
+      <c r="K49" s="56"/>
+      <c r="L49" s="56"/>
+      <c r="M49" s="56"/>
+      <c r="N49" s="56"/>
       <c r="O49" s="103"/>
+      <c r="P49" s="56"/>
+      <c r="Q49" s="56"/>
+      <c r="R49" s="56"/>
       <c r="S49" s="103"/>
+      <c r="T49" s="56"/>
+      <c r="U49" s="56"/>
+      <c r="V49" s="56"/>
+      <c r="W49" s="56"/>
+      <c r="X49" s="56"/>
+      <c r="Y49" s="56"/>
+      <c r="Z49" s="56"/>
+      <c r="AA49" s="56"/>
+      <c r="AB49" s="56"/>
+      <c r="AC49" s="56"/>
       <c r="AD49" s="103"/>
+      <c r="AE49" s="56"/>
+      <c r="AF49" s="56"/>
+      <c r="AG49" s="56"/>
       <c r="AH49" s="57"/>
       <c r="AI49" s="57"/>
       <c r="AJ49" s="57"/>
@@ -6282,9 +6742,17 @@
       <c r="AR49" s="113"/>
       <c r="AS49" s="78"/>
       <c r="AT49" s="58"/>
-    </row>
-    <row r="50" spans="1:48" s="15" customFormat="1">
+      <c r="AU49" s="56"/>
+      <c r="AV49" s="56"/>
+    </row>
+    <row r="50" spans="1:48">
+      <c r="A50" s="15"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
       <c r="D50" s="97"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
       <c r="H50" s="97"/>
       <c r="I50" s="15" t="s">
         <v>113</v>
@@ -6307,6 +6775,9 @@
       <c r="O50" s="99">
         <v>1</v>
       </c>
+      <c r="P50" s="15"/>
+      <c r="Q50" s="15"/>
+      <c r="R50" s="15"/>
       <c r="S50" s="97"/>
       <c r="T50" s="15" t="s">
         <v>79</v>
@@ -6329,9 +6800,15 @@
       <c r="Z50" s="15" t="s">
         <v>81</v>
       </c>
+      <c r="AA50" s="15"/>
+      <c r="AB50" s="15"/>
+      <c r="AC50" s="15"/>
       <c r="AD50" s="97" t="s">
         <v>111</v>
       </c>
+      <c r="AE50" s="15"/>
+      <c r="AF50" s="15"/>
+      <c r="AG50" s="15"/>
       <c r="AH50" s="18" t="b">
         <v>1</v>
       </c>
@@ -6359,11 +6836,28 @@
       </c>
       <c r="AS50" s="76"/>
       <c r="AT50" s="19"/>
-    </row>
-    <row r="51" spans="1:48" s="15" customFormat="1">
+      <c r="AU50" s="15"/>
+      <c r="AV50" s="15"/>
+    </row>
+    <row r="51" spans="1:48">
+      <c r="A51" s="15"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="15"/>
       <c r="D51" s="97"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
       <c r="H51" s="97"/>
+      <c r="I51" s="15"/>
+      <c r="J51" s="15"/>
+      <c r="K51" s="15"/>
+      <c r="L51" s="15"/>
+      <c r="M51" s="15"/>
+      <c r="N51" s="15"/>
       <c r="O51" s="97"/>
+      <c r="P51" s="15"/>
+      <c r="Q51" s="15"/>
+      <c r="R51" s="15"/>
       <c r="S51" s="97"/>
       <c r="T51" s="69"/>
       <c r="U51" s="69"/>
@@ -6395,24 +6889,9 @@
       <c r="AU51" s="69"/>
       <c r="AV51" s="69"/>
     </row>
-    <row r="52" spans="1:48" s="15" customFormat="1">
-      <c r="C52"/>
-      <c r="D52" s="98"/>
-      <c r="E52"/>
-      <c r="F52"/>
-      <c r="G52"/>
-      <c r="H52" s="98"/>
-      <c r="I52"/>
-      <c r="J52"/>
-      <c r="K52"/>
-      <c r="L52"/>
-      <c r="M52"/>
-      <c r="N52"/>
-      <c r="O52" s="98"/>
-      <c r="P52"/>
-      <c r="Q52"/>
-      <c r="R52"/>
-      <c r="S52" s="98"/>
+    <row r="52" spans="1:48">
+      <c r="A52" s="15"/>
+      <c r="B52" s="15"/>
       <c r="T52" s="15" t="s">
         <v>106</v>
       </c>
@@ -6434,10 +6913,15 @@
       <c r="Z52" s="15" t="s">
         <v>103</v>
       </c>
+      <c r="AA52" s="15"/>
+      <c r="AB52" s="15"/>
       <c r="AC52" s="15" t="s">
         <v>6</v>
       </c>
       <c r="AD52" s="97"/>
+      <c r="AE52" s="15"/>
+      <c r="AF52" s="15"/>
+      <c r="AG52" s="15"/>
       <c r="AH52" s="16"/>
       <c r="AI52" s="16"/>
       <c r="AJ52" s="16" t="b">
@@ -6470,7 +6954,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:48" s="56" customFormat="1">
+    <row r="53" spans="1:48">
       <c r="A53" s="15"/>
       <c r="B53" s="15"/>
       <c r="C53" s="15"/>
@@ -6479,9 +6963,31 @@
       <c r="F53" s="15"/>
       <c r="G53" s="15"/>
       <c r="H53" s="97"/>
+      <c r="I53" s="56"/>
+      <c r="J53" s="56"/>
+      <c r="K53" s="56"/>
+      <c r="L53" s="56"/>
+      <c r="M53" s="56"/>
+      <c r="N53" s="56"/>
       <c r="O53" s="103"/>
+      <c r="P53" s="56"/>
+      <c r="Q53" s="56"/>
+      <c r="R53" s="56"/>
       <c r="S53" s="103"/>
+      <c r="T53" s="56"/>
+      <c r="U53" s="56"/>
+      <c r="V53" s="56"/>
+      <c r="W53" s="56"/>
+      <c r="X53" s="56"/>
+      <c r="Y53" s="56"/>
+      <c r="Z53" s="56"/>
+      <c r="AA53" s="56"/>
+      <c r="AB53" s="56"/>
+      <c r="AC53" s="56"/>
       <c r="AD53" s="103"/>
+      <c r="AE53" s="56"/>
+      <c r="AF53" s="56"/>
+      <c r="AG53" s="56"/>
       <c r="AH53" s="57"/>
       <c r="AI53" s="57"/>
       <c r="AJ53" s="57"/>
@@ -6495,9 +7001,17 @@
       <c r="AR53" s="113"/>
       <c r="AS53" s="78"/>
       <c r="AT53" s="58"/>
-    </row>
-    <row r="54" spans="1:48" s="15" customFormat="1">
+      <c r="AU53" s="56"/>
+      <c r="AV53" s="56"/>
+    </row>
+    <row r="54" spans="1:48">
+      <c r="A54" s="15"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
       <c r="D54" s="97"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
       <c r="H54" s="97"/>
       <c r="I54" s="15" t="s">
         <v>114</v>
@@ -6523,6 +7037,8 @@
       <c r="P54" s="15" t="s">
         <v>32</v>
       </c>
+      <c r="Q54" s="15"/>
+      <c r="R54" s="15"/>
       <c r="S54" s="97"/>
       <c r="T54" s="15" t="s">
         <v>79</v>
@@ -6542,9 +7058,16 @@
       <c r="Y54" s="15" t="s">
         <v>80</v>
       </c>
+      <c r="Z54" s="15"/>
+      <c r="AA54" s="15"/>
+      <c r="AB54" s="15"/>
+      <c r="AC54" s="15"/>
       <c r="AD54" s="97" t="s">
         <v>82</v>
       </c>
+      <c r="AE54" s="15"/>
+      <c r="AF54" s="15"/>
+      <c r="AG54" s="15"/>
       <c r="AH54" s="18" t="b">
         <v>1</v>
       </c>
@@ -6572,14 +7095,30 @@
       </c>
       <c r="AS54" s="76"/>
       <c r="AT54" s="19"/>
-    </row>
-    <row r="55" spans="1:48" s="15" customFormat="1">
+      <c r="AU54" s="15"/>
+      <c r="AV54" s="15"/>
+    </row>
+    <row r="55" spans="1:48">
+      <c r="A55" s="15"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
       <c r="D55" s="97"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
       <c r="H55" s="97"/>
+      <c r="I55" s="15"/>
+      <c r="J55" s="15"/>
+      <c r="K55" s="15"/>
+      <c r="L55" s="15"/>
+      <c r="M55" s="15"/>
+      <c r="N55" s="15"/>
       <c r="O55" s="97"/>
       <c r="P55" s="15" t="s">
         <v>38</v>
       </c>
+      <c r="Q55" s="15"/>
+      <c r="R55" s="15"/>
       <c r="S55" s="97"/>
       <c r="T55" s="69"/>
       <c r="U55" s="69"/>
@@ -6611,10 +7150,25 @@
       <c r="AU55" s="69"/>
       <c r="AV55" s="69"/>
     </row>
-    <row r="56" spans="1:48" s="15" customFormat="1">
+    <row r="56" spans="1:48">
+      <c r="A56" s="15"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="15"/>
       <c r="D56" s="99"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="15"/>
       <c r="H56" s="97"/>
+      <c r="I56" s="15"/>
+      <c r="J56" s="15"/>
+      <c r="K56" s="15"/>
+      <c r="L56" s="15"/>
+      <c r="M56" s="15"/>
+      <c r="N56" s="15"/>
       <c r="O56" s="97"/>
+      <c r="P56" s="15"/>
+      <c r="Q56" s="15"/>
+      <c r="R56" s="15"/>
       <c r="S56" s="97"/>
       <c r="T56" s="15" t="s">
         <v>101</v>
@@ -6637,10 +7191,15 @@
       <c r="Z56" s="15" t="s">
         <v>103</v>
       </c>
+      <c r="AA56" s="15"/>
+      <c r="AB56" s="15"/>
       <c r="AC56" s="15" t="s">
         <v>6</v>
       </c>
       <c r="AD56" s="97"/>
+      <c r="AE56" s="15"/>
+      <c r="AF56" s="15"/>
+      <c r="AG56" s="15"/>
       <c r="AH56" s="16" t="b">
         <v>1</v>
       </c>
@@ -6683,12 +7242,44 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:48" s="15" customFormat="1">
+    <row r="57" spans="1:48">
+      <c r="A57" s="15"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="15"/>
       <c r="D57" s="97"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15"/>
       <c r="H57" s="97"/>
+      <c r="I57" s="15"/>
+      <c r="J57" s="15"/>
+      <c r="K57" s="15"/>
+      <c r="L57" s="15"/>
+      <c r="M57" s="15"/>
+      <c r="N57" s="15"/>
       <c r="O57" s="97"/>
+      <c r="P57" s="15"/>
+      <c r="Q57" s="15"/>
+      <c r="R57" s="15"/>
       <c r="S57" s="97"/>
+      <c r="T57" s="15"/>
+      <c r="U57" s="15"/>
+      <c r="V57" s="15"/>
+      <c r="W57" s="15"/>
+      <c r="X57" s="15"/>
+      <c r="Y57" s="15"/>
+      <c r="Z57" s="15"/>
+      <c r="AA57" s="15"/>
+      <c r="AB57" s="15"/>
+      <c r="AC57" s="15"/>
       <c r="AD57" s="97"/>
+      <c r="AE57" s="15"/>
+      <c r="AF57" s="15"/>
+      <c r="AG57" s="15"/>
+      <c r="AH57" s="15"/>
+      <c r="AI57" s="15"/>
+      <c r="AJ57" s="15"/>
+      <c r="AK57" s="15"/>
       <c r="AL57" s="97"/>
       <c r="AM57" s="84" t="s">
         <v>38</v>
@@ -6704,44 +7295,12 @@
       <c r="AR57" s="111"/>
       <c r="AS57" s="76"/>
       <c r="AT57" s="19"/>
-    </row>
-    <row r="58" spans="1:48" s="15" customFormat="1">
-      <c r="C58"/>
-      <c r="D58" s="98"/>
-      <c r="E58"/>
-      <c r="F58"/>
-      <c r="G58"/>
-      <c r="H58" s="98"/>
-      <c r="I58"/>
-      <c r="J58"/>
-      <c r="K58"/>
-      <c r="L58"/>
-      <c r="M58"/>
-      <c r="N58"/>
-      <c r="O58" s="98"/>
-      <c r="P58"/>
-      <c r="Q58"/>
-      <c r="R58"/>
-      <c r="S58" s="98"/>
-      <c r="T58"/>
-      <c r="U58"/>
-      <c r="V58"/>
-      <c r="W58"/>
-      <c r="X58"/>
-      <c r="Y58"/>
-      <c r="Z58"/>
-      <c r="AA58"/>
-      <c r="AB58"/>
-      <c r="AC58"/>
-      <c r="AD58" s="98"/>
-      <c r="AE58"/>
-      <c r="AF58"/>
-      <c r="AG58"/>
-      <c r="AH58" s="17"/>
-      <c r="AI58" s="17"/>
-      <c r="AJ58" s="17"/>
-      <c r="AK58" s="17"/>
-      <c r="AL58" s="112"/>
+      <c r="AU57" s="15"/>
+      <c r="AV57" s="15"/>
+    </row>
+    <row r="58" spans="1:48">
+      <c r="A58" s="15"/>
+      <c r="B58" s="15"/>
       <c r="AM58" s="84" t="s">
         <v>37</v>
       </c>
@@ -6751,32 +7310,10 @@
       <c r="AO58" s="123">
         <v>3</v>
       </c>
-      <c r="AP58" s="17"/>
-      <c r="AQ58" s="17"/>
-      <c r="AR58" s="112"/>
-      <c r="AS58" s="77"/>
-      <c r="AT58" s="20"/>
-      <c r="AU58"/>
-      <c r="AV58"/>
-    </row>
-    <row r="59" spans="1:48" s="15" customFormat="1">
-      <c r="C59"/>
-      <c r="D59" s="98"/>
-      <c r="E59"/>
-      <c r="F59"/>
-      <c r="G59"/>
-      <c r="H59" s="98"/>
-      <c r="I59"/>
-      <c r="J59"/>
-      <c r="K59"/>
-      <c r="L59"/>
-      <c r="M59"/>
-      <c r="N59"/>
-      <c r="O59" s="98"/>
-      <c r="P59"/>
-      <c r="Q59"/>
-      <c r="R59"/>
-      <c r="S59" s="98"/>
+    </row>
+    <row r="59" spans="1:48">
+      <c r="A59" s="15"/>
+      <c r="B59" s="15"/>
       <c r="T59" s="69"/>
       <c r="U59" s="69"/>
       <c r="V59" s="69"/>
@@ -6807,24 +7344,9 @@
       <c r="AU59" s="69"/>
       <c r="AV59" s="69"/>
     </row>
-    <row r="60" spans="1:48" s="15" customFormat="1">
-      <c r="C60"/>
-      <c r="D60" s="98"/>
-      <c r="E60"/>
-      <c r="F60"/>
-      <c r="G60"/>
-      <c r="H60" s="98"/>
-      <c r="I60"/>
-      <c r="J60"/>
-      <c r="K60"/>
-      <c r="L60"/>
-      <c r="M60"/>
-      <c r="N60"/>
-      <c r="O60" s="98"/>
-      <c r="P60"/>
-      <c r="Q60"/>
-      <c r="R60"/>
-      <c r="S60" s="98"/>
+    <row r="60" spans="1:48">
+      <c r="A60" s="15"/>
+      <c r="B60" s="15"/>
       <c r="T60" s="15" t="s">
         <v>106</v>
       </c>
@@ -6846,10 +7368,15 @@
       <c r="Z60" s="15" t="s">
         <v>103</v>
       </c>
+      <c r="AA60" s="15"/>
+      <c r="AB60" s="15"/>
       <c r="AC60" s="15" t="s">
         <v>6</v>
       </c>
       <c r="AD60" s="97"/>
+      <c r="AE60" s="15"/>
+      <c r="AF60" s="15"/>
+      <c r="AG60" s="15"/>
       <c r="AH60" s="16"/>
       <c r="AI60" s="16"/>
       <c r="AJ60" s="16" t="b">
@@ -6882,12 +7409,40 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:48" s="59" customFormat="1" ht="12" customHeight="1">
+    <row r="61" spans="1:48" ht="12" customHeight="1">
+      <c r="A61" s="59"/>
+      <c r="B61" s="59"/>
+      <c r="C61" s="59"/>
       <c r="D61" s="96"/>
+      <c r="E61" s="59"/>
+      <c r="F61" s="59"/>
+      <c r="G61" s="59"/>
       <c r="H61" s="96"/>
+      <c r="I61" s="59"/>
+      <c r="J61" s="59"/>
+      <c r="K61" s="59"/>
+      <c r="L61" s="59"/>
+      <c r="M61" s="59"/>
+      <c r="N61" s="59"/>
       <c r="O61" s="96"/>
+      <c r="P61" s="59"/>
+      <c r="Q61" s="59"/>
+      <c r="R61" s="59"/>
       <c r="S61" s="96"/>
+      <c r="T61" s="59"/>
+      <c r="U61" s="59"/>
+      <c r="V61" s="59"/>
+      <c r="W61" s="59"/>
+      <c r="X61" s="59"/>
+      <c r="Y61" s="59"/>
+      <c r="Z61" s="59"/>
+      <c r="AA61" s="59"/>
+      <c r="AB61" s="59"/>
+      <c r="AC61" s="59"/>
       <c r="AD61" s="96"/>
+      <c r="AE61" s="59"/>
+      <c r="AF61" s="59"/>
+      <c r="AG61" s="59"/>
       <c r="AH61" s="61"/>
       <c r="AI61" s="61"/>
       <c r="AJ61" s="61"/>
@@ -6901,8 +7456,12 @@
       <c r="AR61" s="127"/>
       <c r="AS61" s="73"/>
       <c r="AT61" s="62"/>
-    </row>
-    <row r="62" spans="1:48" s="15" customFormat="1">
+      <c r="AU61" s="59"/>
+      <c r="AV61" s="59"/>
+    </row>
+    <row r="62" spans="1:48">
+      <c r="A62" s="15"/>
+      <c r="B62" s="15"/>
       <c r="C62" s="41"/>
       <c r="D62" s="99" t="s">
         <v>115</v>
@@ -6943,6 +7502,8 @@
       <c r="P62" s="15" t="s">
         <v>104</v>
       </c>
+      <c r="Q62" s="15"/>
+      <c r="R62" s="15"/>
       <c r="S62" s="97"/>
       <c r="T62" s="15" t="s">
         <v>79</v>
@@ -6971,6 +7532,7 @@
       <c r="AB62" s="15">
         <v>5</v>
       </c>
+      <c r="AC62" s="15"/>
       <c r="AD62" s="97" t="s">
         <v>82</v>
       </c>
@@ -7003,7 +7565,7 @@
       <c r="AU62" s="18"/>
       <c r="AV62" s="18"/>
     </row>
-    <row r="63" spans="1:48" s="47" customFormat="1">
+    <row r="63" spans="1:48">
       <c r="A63" s="15"/>
       <c r="B63" s="15"/>
       <c r="C63" s="41"/>
@@ -7053,10 +7615,25 @@
       <c r="AU63" s="69"/>
       <c r="AV63" s="69"/>
     </row>
-    <row r="64" spans="1:48" s="15" customFormat="1">
+    <row r="64" spans="1:48">
+      <c r="A64" s="15"/>
+      <c r="B64" s="15"/>
+      <c r="C64" s="15"/>
       <c r="D64" s="97"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15"/>
       <c r="H64" s="97"/>
+      <c r="I64" s="15"/>
+      <c r="J64" s="15"/>
+      <c r="K64" s="15"/>
+      <c r="L64" s="15"/>
+      <c r="M64" s="15"/>
+      <c r="N64" s="15"/>
       <c r="O64" s="97"/>
+      <c r="P64" s="15"/>
+      <c r="Q64" s="15"/>
+      <c r="R64" s="15"/>
       <c r="S64" s="97"/>
       <c r="T64" s="45" t="s">
         <v>101</v>
@@ -7079,10 +7656,15 @@
       <c r="Z64" s="15" t="s">
         <v>103</v>
       </c>
+      <c r="AA64" s="15"/>
+      <c r="AB64" s="15"/>
       <c r="AC64" s="15" t="s">
         <v>6</v>
       </c>
       <c r="AD64" s="97"/>
+      <c r="AE64" s="15"/>
+      <c r="AF64" s="15"/>
+      <c r="AG64" s="15"/>
       <c r="AH64" s="16" t="b">
         <v>1</v>
       </c>
@@ -7125,13 +7707,44 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:48" s="15" customFormat="1">
+    <row r="65" spans="1:48">
+      <c r="A65" s="15"/>
+      <c r="B65" s="15"/>
+      <c r="C65" s="15"/>
       <c r="D65" s="97"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15"/>
       <c r="H65" s="97"/>
+      <c r="I65" s="15"/>
+      <c r="J65" s="15"/>
+      <c r="K65" s="15"/>
+      <c r="L65" s="15"/>
+      <c r="M65" s="15"/>
+      <c r="N65" s="15"/>
       <c r="O65" s="97"/>
+      <c r="P65" s="15"/>
+      <c r="Q65" s="15"/>
+      <c r="R65" s="15"/>
       <c r="S65" s="97"/>
       <c r="T65" s="45"/>
+      <c r="U65" s="15"/>
+      <c r="V65" s="15"/>
+      <c r="W65" s="15"/>
+      <c r="X65" s="15"/>
+      <c r="Y65" s="15"/>
+      <c r="Z65" s="15"/>
+      <c r="AA65" s="15"/>
+      <c r="AB65" s="15"/>
+      <c r="AC65" s="15"/>
       <c r="AD65" s="97"/>
+      <c r="AE65" s="15"/>
+      <c r="AF65" s="15"/>
+      <c r="AG65" s="15"/>
+      <c r="AH65" s="15"/>
+      <c r="AI65" s="15"/>
+      <c r="AJ65" s="15"/>
+      <c r="AK65" s="15"/>
       <c r="AL65" s="97"/>
       <c r="AM65" s="84" t="s">
         <v>38</v>
@@ -7147,6 +7760,8 @@
       <c r="AR65" s="111"/>
       <c r="AS65" s="76"/>
       <c r="AT65" s="19"/>
+      <c r="AU65" s="15"/>
+      <c r="AV65" s="15"/>
     </row>
     <row r="66" spans="1:48">
       <c r="A66" s="15"/>
@@ -7162,7 +7777,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:48" s="47" customFormat="1">
+    <row r="67" spans="1:48">
       <c r="A67" s="15"/>
       <c r="B67" s="15"/>
       <c r="C67" s="15"/>
@@ -7212,10 +7827,25 @@
       <c r="AU67" s="69"/>
       <c r="AV67" s="69"/>
     </row>
-    <row r="68" spans="1:48" s="15" customFormat="1">
+    <row r="68" spans="1:48">
+      <c r="A68" s="15"/>
+      <c r="B68" s="15"/>
+      <c r="C68" s="15"/>
       <c r="D68" s="97"/>
+      <c r="E68" s="15"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="15"/>
       <c r="H68" s="97"/>
+      <c r="I68" s="15"/>
+      <c r="J68" s="15"/>
+      <c r="K68" s="15"/>
+      <c r="L68" s="15"/>
+      <c r="M68" s="15"/>
+      <c r="N68" s="15"/>
       <c r="O68" s="97"/>
+      <c r="P68" s="15"/>
+      <c r="Q68" s="15"/>
+      <c r="R68" s="15"/>
       <c r="S68" s="97"/>
       <c r="T68" s="15" t="s">
         <v>106</v>
@@ -7238,10 +7868,15 @@
       <c r="Z68" s="15" t="s">
         <v>103</v>
       </c>
+      <c r="AA68" s="15"/>
+      <c r="AB68" s="15"/>
       <c r="AC68" s="15" t="s">
         <v>6</v>
       </c>
       <c r="AD68" s="97"/>
+      <c r="AE68" s="15"/>
+      <c r="AF68" s="15"/>
+      <c r="AG68" s="15"/>
       <c r="AH68" s="16"/>
       <c r="AI68" s="16"/>
       <c r="AJ68" s="16" t="b">
@@ -7274,12 +7909,40 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:48" s="59" customFormat="1" ht="12" customHeight="1">
+    <row r="69" spans="1:48" ht="12" customHeight="1">
+      <c r="A69" s="59"/>
+      <c r="B69" s="59"/>
+      <c r="C69" s="59"/>
       <c r="D69" s="96"/>
+      <c r="E69" s="59"/>
+      <c r="F69" s="59"/>
+      <c r="G69" s="59"/>
       <c r="H69" s="96"/>
+      <c r="I69" s="59"/>
+      <c r="J69" s="59"/>
+      <c r="K69" s="59"/>
+      <c r="L69" s="59"/>
+      <c r="M69" s="59"/>
+      <c r="N69" s="59"/>
       <c r="O69" s="96"/>
+      <c r="P69" s="59"/>
+      <c r="Q69" s="59"/>
+      <c r="R69" s="59"/>
       <c r="S69" s="96"/>
+      <c r="T69" s="59"/>
+      <c r="U69" s="59"/>
+      <c r="V69" s="59"/>
+      <c r="W69" s="59"/>
+      <c r="X69" s="59"/>
+      <c r="Y69" s="59"/>
+      <c r="Z69" s="59"/>
+      <c r="AA69" s="59"/>
+      <c r="AB69" s="59"/>
+      <c r="AC69" s="59"/>
       <c r="AD69" s="96"/>
+      <c r="AE69" s="59"/>
+      <c r="AF69" s="59"/>
+      <c r="AG69" s="59"/>
       <c r="AH69" s="61"/>
       <c r="AI69" s="61"/>
       <c r="AJ69" s="61"/>
@@ -7293,8 +7956,12 @@
       <c r="AR69" s="127"/>
       <c r="AS69" s="73"/>
       <c r="AT69" s="62"/>
-    </row>
-    <row r="70" spans="1:48" s="15" customFormat="1">
+      <c r="AU69" s="59"/>
+      <c r="AV69" s="59"/>
+    </row>
+    <row r="70" spans="1:48">
+      <c r="A70" s="15"/>
+      <c r="B70" s="15"/>
       <c r="C70" s="41"/>
       <c r="D70" s="99" t="s">
         <v>118</v>
@@ -7335,6 +8002,8 @@
       <c r="P70" s="15" t="s">
         <v>38</v>
       </c>
+      <c r="Q70" s="15"/>
+      <c r="R70" s="15"/>
       <c r="S70" s="97"/>
       <c r="T70" s="15" t="s">
         <v>79</v>
@@ -7363,6 +8032,7 @@
       <c r="AB70" s="15">
         <v>5</v>
       </c>
+      <c r="AC70" s="15"/>
       <c r="AD70" s="97" t="s">
         <v>82</v>
       </c>
@@ -7395,7 +8065,7 @@
       <c r="AU70" s="18"/>
       <c r="AV70" s="18"/>
     </row>
-    <row r="71" spans="1:48" s="47" customFormat="1">
+    <row r="71" spans="1:48">
       <c r="A71" s="15"/>
       <c r="B71" s="15"/>
       <c r="C71" s="41"/>
@@ -7447,10 +8117,25 @@
       <c r="AU71" s="69"/>
       <c r="AV71" s="69"/>
     </row>
-    <row r="72" spans="1:48" s="15" customFormat="1">
+    <row r="72" spans="1:48">
+      <c r="A72" s="15"/>
+      <c r="B72" s="15"/>
+      <c r="C72" s="15"/>
       <c r="D72" s="97"/>
+      <c r="E72" s="15"/>
+      <c r="F72" s="15"/>
+      <c r="G72" s="15"/>
       <c r="H72" s="97"/>
+      <c r="I72" s="15"/>
+      <c r="J72" s="15"/>
+      <c r="K72" s="15"/>
+      <c r="L72" s="15"/>
+      <c r="M72" s="15"/>
+      <c r="N72" s="15"/>
       <c r="O72" s="97"/>
+      <c r="P72" s="15"/>
+      <c r="Q72" s="15"/>
+      <c r="R72" s="15"/>
       <c r="S72" s="97"/>
       <c r="T72" s="45" t="s">
         <v>120</v>
@@ -7473,10 +8158,15 @@
       <c r="Z72" s="15" t="s">
         <v>103</v>
       </c>
+      <c r="AA72" s="15"/>
+      <c r="AB72" s="15"/>
       <c r="AC72" s="15" t="s">
         <v>6</v>
       </c>
       <c r="AD72" s="97"/>
+      <c r="AE72" s="15"/>
+      <c r="AF72" s="15"/>
+      <c r="AG72" s="15"/>
       <c r="AH72" s="16" t="b">
         <v>1</v>
       </c>
@@ -7519,13 +8209,44 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:48" s="15" customFormat="1">
+    <row r="73" spans="1:48">
+      <c r="A73" s="15"/>
+      <c r="B73" s="15"/>
+      <c r="C73" s="15"/>
       <c r="D73" s="97"/>
+      <c r="E73" s="15"/>
+      <c r="F73" s="15"/>
+      <c r="G73" s="15"/>
       <c r="H73" s="97"/>
+      <c r="I73" s="15"/>
+      <c r="J73" s="15"/>
+      <c r="K73" s="15"/>
+      <c r="L73" s="15"/>
+      <c r="M73" s="15"/>
+      <c r="N73" s="15"/>
       <c r="O73" s="97"/>
+      <c r="P73" s="15"/>
+      <c r="Q73" s="15"/>
+      <c r="R73" s="15"/>
       <c r="S73" s="97"/>
       <c r="T73" s="45"/>
+      <c r="U73" s="15"/>
+      <c r="V73" s="15"/>
+      <c r="W73" s="15"/>
+      <c r="X73" s="15"/>
+      <c r="Y73" s="15"/>
+      <c r="Z73" s="15"/>
+      <c r="AA73" s="15"/>
+      <c r="AB73" s="15"/>
+      <c r="AC73" s="15"/>
       <c r="AD73" s="97"/>
+      <c r="AE73" s="15"/>
+      <c r="AF73" s="15"/>
+      <c r="AG73" s="15"/>
+      <c r="AH73" s="15"/>
+      <c r="AI73" s="15"/>
+      <c r="AJ73" s="15"/>
+      <c r="AK73" s="15"/>
       <c r="AL73" s="97"/>
       <c r="AM73" s="82" t="s">
         <v>38</v>
@@ -7541,6 +8262,8 @@
       <c r="AR73" s="111"/>
       <c r="AS73" s="76"/>
       <c r="AT73" s="19"/>
+      <c r="AU73" s="15"/>
+      <c r="AV73" s="15"/>
     </row>
     <row r="74" spans="1:48">
       <c r="A74" s="15"/>
@@ -7556,7 +8279,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:48" s="47" customFormat="1">
+    <row r="75" spans="1:48">
       <c r="A75" s="15"/>
       <c r="B75" s="15"/>
       <c r="C75" s="15"/>
@@ -7606,10 +8329,25 @@
       <c r="AU75" s="69"/>
       <c r="AV75" s="69"/>
     </row>
-    <row r="76" spans="1:48" s="15" customFormat="1">
+    <row r="76" spans="1:48">
+      <c r="A76" s="15"/>
+      <c r="B76" s="15"/>
+      <c r="C76" s="15"/>
       <c r="D76" s="97"/>
+      <c r="E76" s="15"/>
+      <c r="F76" s="15"/>
+      <c r="G76" s="15"/>
       <c r="H76" s="97"/>
+      <c r="I76" s="15"/>
+      <c r="J76" s="15"/>
+      <c r="K76" s="15"/>
+      <c r="L76" s="15"/>
+      <c r="M76" s="15"/>
+      <c r="N76" s="15"/>
       <c r="O76" s="97"/>
+      <c r="P76" s="15"/>
+      <c r="Q76" s="15"/>
+      <c r="R76" s="15"/>
       <c r="S76" s="97"/>
       <c r="T76" s="45" t="s">
         <v>121</v>
@@ -7632,10 +8370,15 @@
       <c r="Z76" s="15" t="s">
         <v>103</v>
       </c>
+      <c r="AA76" s="15"/>
+      <c r="AB76" s="15"/>
       <c r="AC76" s="15" t="s">
         <v>6</v>
       </c>
       <c r="AD76" s="97"/>
+      <c r="AE76" s="15"/>
+      <c r="AF76" s="15"/>
+      <c r="AG76" s="15"/>
       <c r="AH76" s="16"/>
       <c r="AI76" s="16"/>
       <c r="AJ76" s="16" t="b">
@@ -7668,12 +8411,40 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:48" s="63" customFormat="1">
+    <row r="77" spans="1:48">
+      <c r="A77" s="63"/>
+      <c r="B77" s="63"/>
+      <c r="C77" s="63"/>
       <c r="D77" s="100"/>
+      <c r="E77" s="63"/>
+      <c r="F77" s="63"/>
+      <c r="G77" s="63"/>
       <c r="H77" s="100"/>
+      <c r="I77" s="63"/>
+      <c r="J77" s="63"/>
+      <c r="K77" s="63"/>
+      <c r="L77" s="63"/>
+      <c r="M77" s="63"/>
+      <c r="N77" s="63"/>
       <c r="O77" s="100"/>
+      <c r="P77" s="63"/>
+      <c r="Q77" s="63"/>
+      <c r="R77" s="63"/>
       <c r="S77" s="100"/>
+      <c r="T77" s="63"/>
+      <c r="U77" s="63"/>
+      <c r="V77" s="63"/>
+      <c r="W77" s="63"/>
+      <c r="X77" s="63"/>
+      <c r="Y77" s="63"/>
+      <c r="Z77" s="63"/>
+      <c r="AA77" s="63"/>
+      <c r="AB77" s="63"/>
+      <c r="AC77" s="63"/>
       <c r="AD77" s="100"/>
+      <c r="AE77" s="63"/>
+      <c r="AF77" s="63"/>
+      <c r="AG77" s="63"/>
       <c r="AH77" s="64"/>
       <c r="AI77" s="64"/>
       <c r="AJ77" s="64"/>
@@ -7687,14 +8458,21 @@
       <c r="AR77" s="114"/>
       <c r="AS77" s="79"/>
       <c r="AT77" s="65"/>
-    </row>
-    <row r="78" spans="1:48" s="15" customFormat="1">
+      <c r="AU77" s="63"/>
+      <c r="AV77" s="63"/>
+    </row>
+    <row r="78" spans="1:48">
+      <c r="A78" s="15"/>
+      <c r="B78" s="15"/>
+      <c r="C78" s="15"/>
       <c r="D78" s="97" t="s">
         <v>122</v>
       </c>
       <c r="E78" s="15" t="s">
         <v>123</v>
       </c>
+      <c r="F78" s="15"/>
+      <c r="G78" s="15"/>
       <c r="H78" s="97"/>
       <c r="I78" s="15" t="s">
         <v>124</v>
@@ -7720,6 +8498,8 @@
       <c r="P78" s="15" t="s">
         <v>125</v>
       </c>
+      <c r="Q78" s="15"/>
+      <c r="R78" s="15"/>
       <c r="S78" s="97"/>
       <c r="T78" s="15" t="s">
         <v>126</v>
@@ -7739,6 +8519,9 @@
       <c r="Y78" s="15" t="s">
         <v>91</v>
       </c>
+      <c r="Z78" s="15"/>
+      <c r="AA78" s="15"/>
+      <c r="AB78" s="15"/>
       <c r="AC78" s="15" t="s">
         <v>6</v>
       </c>
@@ -7788,16 +8571,44 @@
       <c r="AU78" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="79" spans="1:48" s="15" customFormat="1">
+      <c r="AV78" s="15"/>
+    </row>
+    <row r="79" spans="1:48">
+      <c r="A79" s="15"/>
+      <c r="B79" s="15"/>
+      <c r="C79" s="15"/>
       <c r="D79" s="97"/>
       <c r="E79" s="15" t="s">
         <v>129</v>
       </c>
+      <c r="F79" s="15"/>
+      <c r="G79" s="15"/>
       <c r="H79" s="97"/>
+      <c r="I79" s="15"/>
+      <c r="J79" s="15"/>
+      <c r="K79" s="15"/>
+      <c r="L79" s="15"/>
+      <c r="M79" s="15"/>
+      <c r="N79" s="15"/>
       <c r="O79" s="97"/>
+      <c r="P79" s="15"/>
+      <c r="Q79" s="15"/>
+      <c r="R79" s="15"/>
       <c r="S79" s="97"/>
+      <c r="T79" s="15"/>
+      <c r="U79" s="15"/>
+      <c r="V79" s="15"/>
+      <c r="W79" s="15"/>
+      <c r="X79" s="15"/>
+      <c r="Y79" s="15"/>
+      <c r="Z79" s="15"/>
+      <c r="AA79" s="15"/>
+      <c r="AB79" s="15"/>
+      <c r="AC79" s="15"/>
       <c r="AD79" s="97"/>
+      <c r="AE79" s="15"/>
+      <c r="AF79" s="15"/>
+      <c r="AG79" s="15"/>
       <c r="AH79" s="16"/>
       <c r="AI79" s="16"/>
       <c r="AJ79" s="16"/>
@@ -7824,6 +8635,7 @@
       <c r="AU79" s="16" t="s">
         <v>128</v>
       </c>
+      <c r="AV79" s="15"/>
     </row>
     <row r="84" spans="2:8">
       <c r="B84" s="1"/>
@@ -7835,7 +8647,7 @@
       <c r="H84" s="95"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="AM13 B7:B13 Z17:AD17 X16:X17 U16:W16 C23:D23 E22:G23 B71:B74 B16:B23 C18:D20 E17:G19 C7:D12 E6:H12 B35:G39 C63:H64 H36:I36 B50:I50 B54:I54 B43:O44 B42:I42 C25:I25 B70:I70 B62:I62 T42:Y42 T22:AL22 T39:AL39 T18:AL18 T59:AL59 T47:AL47 T43:AL43 T33:AL33 T29:AL29 T75:AL75 T71:AL71 T37:AL37 T67:AL67 AH17:AO17 AA36:AR36 AA50:AR50 AE54:AR54 AA42:AR42 AH27:AO28 AH25:AO25 AM23:AR23 AM19:AR20 AM40:AR40 AM52:AR52 AM60:AR60 AO56:AR57 AM48:AR48 AO44:AR45 AM34:AR34 AM30:AR31 AM38:AR38 AP22:AV22 AP39:AR39 AP17:AV18 AP51:AV51 AP59:AV59 AP55:AV55 AP47:AV47 AP43:AV43 AP33:AV33 AP25:AV29 AP37:AR37 AS37:AV39 AW17:XFD60 Y16:XFD16 AP5:XFD10 W80:XFD81 Y24:AV24 AM11:XFD12 AM15:XFD15 AP14:XFD14 AM72:XFD73 AP71:XFD71 AM76:XFD76 AP75:XFD75 AM64:XFD65 AP63:XFD63 AM68:XFD68 AP67:XFD67 H23:S23 H18:S20 H37:S39 I12:S12 B40:S40 B52:S52 B56:S60 B45:S48 C71:S73 B75:S76 C65:S65 B67:S68 H34:S34 H29:S31 P36:Y36 I10:AL11 B80:U81 C16:T17 B15:V15 C24:W24 H28:AG28 H27:Y27 I64:AG64 B14:AL14 H26:AL26 I63:AL63 B5:AO6 I8:AO9 B77:XFD79 H35:AV35 B49:AV49 B53:AV53 B41:AV41 P70:XFD70 P62:XFD62 P25:T25 P42:S43 B51:AL51 P50:Y50 B55:AL55 P54:AC54 I7:AL7">
+  <conditionalFormatting sqref="AM13 B7:B13 Z17:AD17 X16:X17 U16:W16 C23:D23 E22:G23 B71:B74 B16:B23 C18:D20 E17:G19 C7:D12 E6:H12 B35:G39 C63:H64 H36:I36 B50:I50 B54:I54 B43:O44 B42:I42 C25:I25 B70:I70 B62:I62 T42:Y42 T22:AL22 T39:AL39 T18:AL18 T59:AL59 T47:AL47 T43:AL43 T33:AL33 T29:AL29 T75:AL75 T71:AL71 T37:AL37 T67:AL67 AH17:AO17 AA36:AR36 AA50:AR50 AE54:AR54 AA42:AR42 AH27:AO28 AH25:AO25 AM23:AR23 AM19:AR20 AM40:AR40 AM52:AR52 AM60:AR60 AO56:AR57 AM48:AR48 AO44:AR45 AM34:AR34 AM30:AR31 AM38:AR38 AP22:AV22 AP39:AR39 AP17:AV18 AP51:AV51 AP59:AV59 AP55:AV55 AP47:AV47 AP43:AV43 AP33:AV33 AP25:AV29 AP37:AR37 AS37:AV39 Y16:AV16 AP5:AV10 W80:AV81 Y24:AV24 AM11:AV12 AM15:AV15 AP14:AV14 AM72:AV73 AP71:AV71 AM76:AV76 AP75:AV75 AM64:AV65 AP63:AV63 AM68:AV68 AP67:AV67 H23:S23 H18:S20 H37:S39 I12:S12 B40:S40 B52:S52 B56:S60 B45:S48 C71:S73 B75:S76 C65:S65 B67:S68 H34:S34 H29:S31 P36:Y36 I10:AL11 B80:U81 C16:T17 B15:V15 C24:W24 H28:AG28 H27:Y27 I64:AG64 B14:AL14 H26:AL26 I63:AL63 B5:AO6 I8:AO9 B77:AV79 H35:AV35 B49:AV49 B53:AV53 B41:AV41 P70:AV70 P62:AV62 P25:T25 P42:S43 B51:AL51 P50:Y50 B55:AL55 P54:AC54 I7:AL7">
     <cfRule type="cellIs" dxfId="90" priority="181" operator="equal">
       <formula>"nil"</formula>
     </cfRule>

</xml_diff>

<commit_message>
update to load and from_dict
</commit_message>
<xml_diff>
--- a/data/inputs/Asset Model - Demo.xlsx
+++ b/data/inputs/Asset Model - Demo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23322"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23405"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtreseder\OneDrive - KPMG\Documents\3. Client\Essential Energy\Probability of Failure Model\pof\data\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1872" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D4EE982C-507A-4AF4-89EE-C153CA58DE85}"/>
+  <xr:revisionPtr revIDLastSave="1895" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DFA4ED6F-BE31-4191-9B3F-31B94F53D031}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3584,7 +3584,7 @@
   <dimension ref="A1:AV84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>
@@ -4116,7 +4116,7 @@
         <v>78</v>
       </c>
       <c r="R6" s="15">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="S6" s="97">
         <v>1</v>
@@ -5282,7 +5282,7 @@
         <v>78</v>
       </c>
       <c r="R25" s="15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S25" s="97">
         <v>1</v>

</xml_diff>

<commit_message>
minor changes to timeline
</commit_message>
<xml_diff>
--- a/data/inputs/Asset Model - Demo.xlsx
+++ b/data/inputs/Asset Model - Demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtreseder\OneDrive - KPMG\Documents\3. Client\Essential Energy\Probability of Failure Model\pof\data\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1929" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{86E64C97-298C-4791-B94E-5395CFEA7FF9}"/>
+  <xr:revisionPtr revIDLastSave="1931" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{26EB1D61-E1B4-4298-A7F6-16EE6AC67CAE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,6 +50,7 @@
     <author>tc={EDC7C1E7-87D8-4DCB-A596-9C8067A50A9A}</author>
     <author>tc={C397EB22-6AC0-4AF2-9D5D-CDA1CF4C3832}</author>
     <author>tc={3FC98A93-1BD2-46CA-8439-5A569DD9E38A}</author>
+    <author>tc={A36EDA56-9BB8-4481-8541-35CA7263BBE2}</author>
     <author>tc={214FAD6C-C7E5-485F-8706-D09B002BBC46}</author>
     <author>tc={87DFEB67-927C-442C-956F-66557C9248F0}</author>
     <author>tc={3531B4B9-52F1-48E1-BD1D-58D8097B8528}</author>
@@ -89,7 +90,15 @@
     250 mm</t>
       </text>
     </comment>
-    <comment ref="AM8" authorId="3" shapeId="0" xr:uid="{214FAD6C-C7E5-485F-8706-D09B002BBC46}">
+    <comment ref="E8" authorId="3" shapeId="0" xr:uid="{A36EDA56-9BB8-4481-8541-35CA7263BBE2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Removed to solve timeline error when method wasn't actuall called anywhere</t>
+      </text>
+    </comment>
+    <comment ref="AM8" authorId="4" shapeId="0" xr:uid="{214FAD6C-C7E5-485F-8706-D09B002BBC46}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -97,7 +106,7 @@
     Confirm with Peter Couch / Greg Toms</t>
       </text>
     </comment>
-    <comment ref="AM13" authorId="4" shapeId="0" xr:uid="{87DFEB67-927C-442C-956F-66557C9248F0}">
+    <comment ref="AM13" authorId="5" shapeId="0" xr:uid="{87DFEB67-927C-442C-956F-66557C9248F0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -105,7 +114,7 @@
     add safety factor back</t>
       </text>
     </comment>
-    <comment ref="T44" authorId="5" shapeId="0" xr:uid="{3531B4B9-52F1-48E1-BD1D-58D8097B8528}">
+    <comment ref="T44" authorId="6" shapeId="0" xr:uid="{3531B4B9-52F1-48E1-BD1D-58D8097B8528}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -115,7 +124,7 @@
     probs delete</t>
       </text>
     </comment>
-    <comment ref="D56" authorId="6" shapeId="0" xr:uid="{2C545A15-58BF-4325-853E-F01A6E2CD754}">
+    <comment ref="D56" authorId="7" shapeId="0" xr:uid="{2C545A15-58BF-4325-853E-F01A6E2CD754}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -123,7 +132,7 @@
     Change task type to planned / reactive / risk?</t>
       </text>
     </comment>
-    <comment ref="D62" authorId="7" shapeId="0" xr:uid="{B6F30610-5DE2-43DC-8686-4075E019810F}">
+    <comment ref="D62" authorId="8" shapeId="0" xr:uid="{B6F30610-5DE2-43DC-8686-4075E019810F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -131,7 +140,7 @@
     How do we deal with failures that accelerate other failure modes?</t>
       </text>
     </comment>
-    <comment ref="I62" authorId="8" shapeId="0" xr:uid="{F6470554-740D-4816-85E3-E23C5729D666}">
+    <comment ref="I62" authorId="9" shapeId="0" xr:uid="{F6470554-740D-4816-85E3-E23C5729D666}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -139,7 +148,7 @@
     Break it out later</t>
       </text>
     </comment>
-    <comment ref="Z62" authorId="9" shapeId="0" xr:uid="{9FFAA4E9-09CD-479C-BFE9-ED94809A5C81}">
+    <comment ref="Z62" authorId="10" shapeId="0" xr:uid="{9FFAA4E9-09CD-479C-BFE9-ED94809A5C81}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -148,7 +157,7 @@
 Add an additional task?</t>
       </text>
     </comment>
-    <comment ref="T64" authorId="10" shapeId="0" xr:uid="{BE62B33B-1180-42C8-AE27-EADC70606D7B}">
+    <comment ref="T64" authorId="11" shapeId="0" xr:uid="{BE62B33B-1180-42C8-AE27-EADC70606D7B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -156,7 +165,7 @@
     Make this a repair task</t>
       </text>
     </comment>
-    <comment ref="D70" authorId="11" shapeId="0" xr:uid="{C4841757-EFF4-403A-A229-DD7AF8BE79E4}">
+    <comment ref="D70" authorId="12" shapeId="0" xr:uid="{C4841757-EFF4-403A-A229-DD7AF8BE79E4}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -164,7 +173,7 @@
     How do we deal with failures that accelerate other failure modes?</t>
       </text>
     </comment>
-    <comment ref="Z70" authorId="12" shapeId="0" xr:uid="{1E2E6910-FDBF-4DAD-9ACF-D9553B573D8C}">
+    <comment ref="Z70" authorId="13" shapeId="0" xr:uid="{1E2E6910-FDBF-4DAD-9ACF-D9553B573D8C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -173,7 +182,7 @@
 Add an additional task?</t>
       </text>
     </comment>
-    <comment ref="T72" authorId="13" shapeId="0" xr:uid="{65DC17AD-63E9-433B-A662-056382EECC79}">
+    <comment ref="T72" authorId="14" shapeId="0" xr:uid="{65DC17AD-63E9-433B-A662-056382EECC79}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -181,7 +190,7 @@
     Make this a repair task</t>
       </text>
     </comment>
-    <comment ref="E78" authorId="14" shapeId="0" xr:uid="{2A9F7F02-73AD-487F-89D9-8F1E4E03126C}">
+    <comment ref="E78" authorId="15" shapeId="0" xr:uid="{2A9F7F02-73AD-487F-89D9-8F1E4E03126C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -189,7 +198,7 @@
     fix method to allow multiple indicators for one component</t>
       </text>
     </comment>
-    <comment ref="I78" authorId="15" shapeId="0" xr:uid="{D0C67513-5DB5-4D3F-8187-F19DE320258E}">
+    <comment ref="I78" authorId="16" shapeId="0" xr:uid="{D0C67513-5DB5-4D3F-8187-F19DE320258E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -202,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="331">
   <si>
     <t>Cause</t>
   </si>
@@ -462,310 +471,310 @@
     <t>ssf_calc</t>
   </si>
   <si>
+    <t>termite_powder</t>
+  </si>
+  <si>
+    <t>repair</t>
+  </si>
+  <si>
+    <t>ConditionTask</t>
+  </si>
+  <si>
+    <t>grp</t>
+  </si>
+  <si>
+    <t>fm</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>reduction_factor</t>
+  </si>
+  <si>
+    <t>lightning_damage</t>
+  </si>
+  <si>
+    <t>step</t>
+  </si>
+  <si>
+    <t>fire_damage</t>
+  </si>
+  <si>
+    <t>impact_damage</t>
+  </si>
+  <si>
+    <t>CAT3/4 replacement</t>
+  </si>
+  <si>
+    <t>replace</t>
+  </si>
+  <si>
+    <t>as_good_as_new</t>
+  </si>
+  <si>
+    <t>lean_angle</t>
+  </si>
+  <si>
+    <t>CAT1/2 replacement</t>
+  </si>
+  <si>
+    <t>fungal decay _ external</t>
+  </si>
+  <si>
+    <t>fungal decay _ internal</t>
+  </si>
+  <si>
+    <t>pole_saver_rod</t>
+  </si>
+  <si>
+    <t>lightning</t>
+  </si>
+  <si>
+    <t>assisted_failures</t>
+  </si>
+  <si>
+    <t>impact</t>
+  </si>
+  <si>
+    <t>weathering</t>
+  </si>
+  <si>
+    <t>pole footing</t>
+  </si>
+  <si>
+    <t>leaning</t>
+  </si>
+  <si>
+    <t>any reason</t>
+  </si>
+  <si>
+    <t>pole_cap</t>
+  </si>
+  <si>
+    <t>missing</t>
+  </si>
+  <si>
+    <t>Pole cap replacement</t>
+  </si>
+  <si>
+    <t>Pole replacement</t>
+  </si>
+  <si>
+    <t>crossarm</t>
+  </si>
+  <si>
+    <t>cross_sectional_area</t>
+  </si>
+  <si>
+    <t>Fix_this_error</t>
+  </si>
+  <si>
+    <t>add_no_condition_method</t>
+  </si>
+  <si>
+    <t>strut</t>
+  </si>
+  <si>
+    <t>modify</t>
+  </si>
+  <si>
+    <t>addition</t>
+  </si>
+  <si>
+    <t>crack_length</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>Sub System</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Maintainable Item</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>Pole</t>
+  </si>
+  <si>
+    <t>Pole Stay</t>
+  </si>
+  <si>
+    <t>Pole Cap</t>
+  </si>
+  <si>
+    <t>Pole Footing</t>
+  </si>
+  <si>
+    <t>pole (common)</t>
+  </si>
+  <si>
+    <t>pole (timber)</t>
+  </si>
+  <si>
+    <t>pole (concrete)</t>
+  </si>
+  <si>
+    <t>pole (steel)</t>
+  </si>
+  <si>
+    <t>pole (composite)</t>
+  </si>
+  <si>
+    <t>pole fixtures</t>
+  </si>
+  <si>
+    <t>attachments</t>
+  </si>
+  <si>
+    <t>pole cap</t>
+  </si>
+  <si>
+    <t>steps</t>
+  </si>
+  <si>
+    <t>pole stay</t>
+  </si>
+  <si>
+    <t>pole attachment</t>
+  </si>
+  <si>
+    <t>top attachment point</t>
+  </si>
+  <si>
+    <t>thimble</t>
+  </si>
+  <si>
+    <t>wire</t>
+  </si>
+  <si>
+    <t>dead end</t>
+  </si>
+  <si>
+    <t>insulator</t>
+  </si>
+  <si>
+    <t>batten</t>
+  </si>
+  <si>
+    <t>sight guard</t>
+  </si>
+  <si>
+    <t>anchor rod</t>
+  </si>
+  <si>
+    <t>footing</t>
+  </si>
+  <si>
+    <t>pole modification</t>
+  </si>
+  <si>
+    <t>reinforcement</t>
+  </si>
+  <si>
+    <t>nail</t>
+  </si>
+  <si>
+    <t>acroprop</t>
+  </si>
+  <si>
+    <t>pole accessories</t>
+  </si>
+  <si>
+    <t>fauna protection</t>
+  </si>
+  <si>
+    <t>stay protection</t>
+  </si>
+  <si>
+    <t>cattle guard post</t>
+  </si>
+  <si>
+    <t>Indicators</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>[pole] {broken} due to (termites)</t>
+  </si>
+  <si>
+    <t>[pole] {broken} due to (lightning)</t>
+  </si>
+  <si>
+    <t>nil</t>
+  </si>
+  <si>
+    <t>[pole] {broken} due to (impact)</t>
+  </si>
+  <si>
+    <t>[pole] {broken} due to (fire damage)</t>
+  </si>
+  <si>
+    <t>[pole] {broken} due to (fungal decay - internal)</t>
+  </si>
+  <si>
+    <t>[pole] {broken} due to (fungal decay - external)</t>
+  </si>
+  <si>
+    <t>[pole] {broken} due to (weathering)</t>
+  </si>
+  <si>
+    <t>[pole foundation] due to (unknown)</t>
+  </si>
+  <si>
+    <t>[pole cap] due to (unknown)</t>
+  </si>
+  <si>
+    <t>pole_cap_present</t>
+  </si>
+  <si>
+    <t>[pole stay] due to (unknown)</t>
+  </si>
+  <si>
+    <t>[pole stay] due to (impact)</t>
+  </si>
+  <si>
+    <t>[pole stay] due to (corrosion)</t>
+  </si>
+  <si>
+    <t>[pole stay] due to (bed log)</t>
+  </si>
+  <si>
+    <t>[pole top equipment] due to {cracking}</t>
+  </si>
+  <si>
+    <t>cracking_present</t>
+  </si>
+  <si>
+    <t>simple_safety_factor</t>
+  </si>
+  <si>
+    <t>sf</t>
+  </si>
+  <si>
+    <t>ssf</t>
+  </si>
+  <si>
     <t>actual_safety_factor</t>
   </si>
   <si>
     <t>dsf_calc</t>
-  </si>
-  <si>
-    <t>termite_powder</t>
-  </si>
-  <si>
-    <t>repair</t>
-  </si>
-  <si>
-    <t>ConditionTask</t>
-  </si>
-  <si>
-    <t>grp</t>
-  </si>
-  <si>
-    <t>fm</t>
-  </si>
-  <si>
-    <t>max</t>
-  </si>
-  <si>
-    <t>all</t>
-  </si>
-  <si>
-    <t>reduction_factor</t>
-  </si>
-  <si>
-    <t>lightning_damage</t>
-  </si>
-  <si>
-    <t>step</t>
-  </si>
-  <si>
-    <t>fire_damage</t>
-  </si>
-  <si>
-    <t>impact_damage</t>
-  </si>
-  <si>
-    <t>CAT3/4 replacement</t>
-  </si>
-  <si>
-    <t>replace</t>
-  </si>
-  <si>
-    <t>as_good_as_new</t>
-  </si>
-  <si>
-    <t>lean_angle</t>
-  </si>
-  <si>
-    <t>CAT1/2 replacement</t>
-  </si>
-  <si>
-    <t>fungal decay _ external</t>
-  </si>
-  <si>
-    <t>fungal decay _ internal</t>
-  </si>
-  <si>
-    <t>pole_saver_rod</t>
-  </si>
-  <si>
-    <t>lightning</t>
-  </si>
-  <si>
-    <t>assisted_failures</t>
-  </si>
-  <si>
-    <t>impact</t>
-  </si>
-  <si>
-    <t>weathering</t>
-  </si>
-  <si>
-    <t>pole footing</t>
-  </si>
-  <si>
-    <t>leaning</t>
-  </si>
-  <si>
-    <t>any reason</t>
-  </si>
-  <si>
-    <t>pole_cap</t>
-  </si>
-  <si>
-    <t>missing</t>
-  </si>
-  <si>
-    <t>Pole cap replacement</t>
-  </si>
-  <si>
-    <t>Pole replacement</t>
-  </si>
-  <si>
-    <t>crossarm</t>
-  </si>
-  <si>
-    <t>cross_sectional_area</t>
-  </si>
-  <si>
-    <t>Fix_this_error</t>
-  </si>
-  <si>
-    <t>add_no_condition_method</t>
-  </si>
-  <si>
-    <t>strut</t>
-  </si>
-  <si>
-    <t>modify</t>
-  </si>
-  <si>
-    <t>addition</t>
-  </si>
-  <si>
-    <t>crack_length</t>
-  </si>
-  <si>
-    <t>System</t>
-  </si>
-  <si>
-    <t>Sub System</t>
-  </si>
-  <si>
-    <t>Module</t>
-  </si>
-  <si>
-    <t>Maintainable Item</t>
-  </si>
-  <si>
-    <t>Component</t>
-  </si>
-  <si>
-    <t>Material</t>
-  </si>
-  <si>
-    <t>Treatment</t>
-  </si>
-  <si>
-    <t>Pole</t>
-  </si>
-  <si>
-    <t>Pole Stay</t>
-  </si>
-  <si>
-    <t>Pole Cap</t>
-  </si>
-  <si>
-    <t>Pole Footing</t>
-  </si>
-  <si>
-    <t>pole (common)</t>
-  </si>
-  <si>
-    <t>pole (timber)</t>
-  </si>
-  <si>
-    <t>pole (concrete)</t>
-  </si>
-  <si>
-    <t>pole (steel)</t>
-  </si>
-  <si>
-    <t>pole (composite)</t>
-  </si>
-  <si>
-    <t>pole fixtures</t>
-  </si>
-  <si>
-    <t>attachments</t>
-  </si>
-  <si>
-    <t>pole cap</t>
-  </si>
-  <si>
-    <t>steps</t>
-  </si>
-  <si>
-    <t>pole stay</t>
-  </si>
-  <si>
-    <t>pole attachment</t>
-  </si>
-  <si>
-    <t>top attachment point</t>
-  </si>
-  <si>
-    <t>thimble</t>
-  </si>
-  <si>
-    <t>wire</t>
-  </si>
-  <si>
-    <t>dead end</t>
-  </si>
-  <si>
-    <t>insulator</t>
-  </si>
-  <si>
-    <t>batten</t>
-  </si>
-  <si>
-    <t>sight guard</t>
-  </si>
-  <si>
-    <t>anchor rod</t>
-  </si>
-  <si>
-    <t>footing</t>
-  </si>
-  <si>
-    <t>pole modification</t>
-  </si>
-  <si>
-    <t>reinforcement</t>
-  </si>
-  <si>
-    <t>nail</t>
-  </si>
-  <si>
-    <t>acroprop</t>
-  </si>
-  <si>
-    <t>pole accessories</t>
-  </si>
-  <si>
-    <t>fauna protection</t>
-  </si>
-  <si>
-    <t>stay protection</t>
-  </si>
-  <si>
-    <t>cattle guard post</t>
-  </si>
-  <si>
-    <t>Indicators</t>
-  </si>
-  <si>
-    <t>Condition</t>
-  </si>
-  <si>
-    <t>[pole] {broken} due to (termites)</t>
-  </si>
-  <si>
-    <t>[pole] {broken} due to (lightning)</t>
-  </si>
-  <si>
-    <t>nil</t>
-  </si>
-  <si>
-    <t>[pole] {broken} due to (impact)</t>
-  </si>
-  <si>
-    <t>[pole] {broken} due to (fire damage)</t>
-  </si>
-  <si>
-    <t>[pole] {broken} due to (fungal decay - internal)</t>
-  </si>
-  <si>
-    <t>[pole] {broken} due to (fungal decay - external)</t>
-  </si>
-  <si>
-    <t>[pole] {broken} due to (weathering)</t>
-  </si>
-  <si>
-    <t>[pole foundation] due to (unknown)</t>
-  </si>
-  <si>
-    <t>[pole cap] due to (unknown)</t>
-  </si>
-  <si>
-    <t>pole_cap_present</t>
-  </si>
-  <si>
-    <t>[pole stay] due to (unknown)</t>
-  </si>
-  <si>
-    <t>[pole stay] due to (impact)</t>
-  </si>
-  <si>
-    <t>[pole stay] due to (corrosion)</t>
-  </si>
-  <si>
-    <t>[pole stay] due to (bed log)</t>
-  </si>
-  <si>
-    <t>[pole top equipment] due to {cracking}</t>
-  </si>
-  <si>
-    <t>cracking_present</t>
-  </si>
-  <si>
-    <t>simple_safety_factor</t>
-  </si>
-  <si>
-    <t>sf</t>
-  </si>
-  <si>
-    <t>ssf</t>
   </si>
   <si>
     <t>asf</t>
@@ -2623,6 +2632,9 @@
   <threadedComment ref="G6" dT="2020-09-09T03:31:13.87" personId="{382B0E3D-8CF3-4AD9-8A08-175DF2A62319}" id="{3FC98A93-1BD2-46CA-8439-5A569DD9E38A}">
     <text>250 mm</text>
   </threadedComment>
+  <threadedComment ref="E8" dT="2020-10-11T23:14:06.89" personId="{382B0E3D-8CF3-4AD9-8A08-175DF2A62319}" id="{A36EDA56-9BB8-4481-8541-35CA7263BBE2}">
+    <text>Removed to solve timeline error when method wasn't actuall called anywhere</text>
+  </threadedComment>
   <threadedComment ref="AM8" dT="2020-09-09T03:33:43.87" personId="{382B0E3D-8CF3-4AD9-8A08-175DF2A62319}" id="{214FAD6C-C7E5-485F-8706-D09B002BBC46}">
     <text>Confirm with Peter Couch / Greg Toms</text>
   </threadedComment>
@@ -2768,7 +2780,7 @@
         <v>273</v>
       </c>
       <c r="Q13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="S13" t="s">
         <v>274</v>
@@ -2779,7 +2791,7 @@
         <v>275</v>
       </c>
       <c r="O14" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="Q14" t="s">
         <v>276</v>
@@ -2802,7 +2814,7 @@
         <v>281</v>
       </c>
       <c r="S15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:19">
@@ -2810,7 +2822,7 @@
         <v>282</v>
       </c>
       <c r="Q16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="S16" t="s">
         <v>283</v>
@@ -2853,19 +2865,19 @@
         <v>79</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="O31" s="1" t="s">
         <v>291</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="S31" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:19">
@@ -2876,10 +2888,10 @@
         <v>24</v>
       </c>
       <c r="R32" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="S32" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" spans="2:19">
@@ -2924,7 +2936,7 @@
         <v>292</v>
       </c>
       <c r="R35" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="S35">
         <v>1</v>
@@ -2957,7 +2969,7 @@
         <v>287</v>
       </c>
       <c r="E38" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K38" t="s">
         <v>2</v>
@@ -2971,7 +2983,7 @@
         <v>294</v>
       </c>
       <c r="J39" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="2:19">
@@ -2999,13 +3011,13 @@
         <v>296</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>297</v>
@@ -3060,7 +3072,7 @@
         <v>301</v>
       </c>
       <c r="E60" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -3075,7 +3087,7 @@
     </row>
     <row r="65" spans="1:3">
       <c r="B65" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C65" s="15" t="s">
         <v>304</v>
@@ -3591,8 +3603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA0734F-FFBE-4DAF-BDE5-A12359370A0D}">
   <dimension ref="A1:AV84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AM38" sqref="AM38"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>
@@ -4223,18 +4235,8 @@
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="97"/>
-      <c r="E8" t="s">
-        <v>86</v>
-      </c>
-      <c r="F8" t="s">
-        <v>87</v>
-      </c>
-      <c r="G8" s="42">
-        <v>6</v>
-      </c>
-      <c r="H8" s="138">
-        <v>1</v>
-      </c>
+      <c r="G8" s="42"/>
+      <c r="H8" s="138"/>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
@@ -4247,7 +4249,7 @@
       <c r="R8" s="15"/>
       <c r="S8" s="97"/>
       <c r="T8" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="U8" s="42">
         <v>0.9</v>
@@ -4259,18 +4261,18 @@
         <v>2</v>
       </c>
       <c r="X8" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y8" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z8" s="15" t="s">
         <v>89</v>
-      </c>
-      <c r="Y8" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z8" s="15" t="s">
-        <v>91</v>
       </c>
       <c r="AA8" s="15"/>
       <c r="AB8" s="15"/>
       <c r="AC8" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AD8" s="97"/>
       <c r="AE8" s="15"/>
@@ -4294,25 +4296,25 @@
         <v>50</v>
       </c>
       <c r="AO8" s="118" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP8" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR8" s="110" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS8" s="91" t="s">
+        <v>92</v>
+      </c>
+      <c r="AT8" s="93">
+        <v>0</v>
+      </c>
+      <c r="AU8" s="18" t="s">
         <v>93</v>
-      </c>
-      <c r="AP8" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ8" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="AR8" s="110" t="b">
-        <v>0</v>
-      </c>
-      <c r="AS8" s="91" t="s">
-        <v>94</v>
-      </c>
-      <c r="AT8" s="93">
-        <v>0</v>
-      </c>
-      <c r="AU8" s="18" t="s">
-        <v>95</v>
       </c>
       <c r="AV8" s="18" t="s">
         <v>2</v>
@@ -4324,10 +4326,10 @@
       <c r="C9" s="15"/>
       <c r="D9" s="97"/>
       <c r="E9" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G9" s="15" t="b">
         <v>1</v>
@@ -4372,7 +4374,7 @@
         <v>50</v>
       </c>
       <c r="AO9" s="118" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AP9" s="16"/>
       <c r="AQ9" s="16"/>
@@ -4388,10 +4390,10 @@
       <c r="C10" s="15"/>
       <c r="D10" s="97"/>
       <c r="E10" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G10" s="15" t="b">
         <v>1</v>
@@ -4446,10 +4448,10 @@
       <c r="C11" s="15"/>
       <c r="D11" s="97"/>
       <c r="E11" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G11" s="15" t="b">
         <v>1</v>
@@ -4469,7 +4471,7 @@
       <c r="R11" s="15"/>
       <c r="S11" s="97"/>
       <c r="T11" s="15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="U11" s="15">
         <v>1</v>
@@ -4481,13 +4483,13 @@
         <v>2</v>
       </c>
       <c r="X11" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Y11" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z11" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AA11" s="15"/>
       <c r="AB11" s="15"/>
@@ -4528,13 +4530,13 @@
         <v>0</v>
       </c>
       <c r="AS11" s="76" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AT11" s="19">
         <v>1</v>
       </c>
       <c r="AU11" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AV11" s="15" t="s">
         <v>2</v>
@@ -4546,10 +4548,10 @@
       <c r="C12" s="15"/>
       <c r="D12" s="97"/>
       <c r="E12" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G12" s="15" t="b">
         <v>1</v>
@@ -4683,7 +4685,7 @@
       <c r="R15" s="15"/>
       <c r="S15" s="97"/>
       <c r="T15" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="U15" s="15">
         <v>1</v>
@@ -4695,13 +4697,13 @@
         <v>2</v>
       </c>
       <c r="X15" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Y15" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z15" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AA15" s="15"/>
       <c r="AB15" s="15"/>
@@ -4732,13 +4734,13 @@
         <v>0</v>
       </c>
       <c r="AS15" s="76" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AT15" s="19">
         <v>1</v>
       </c>
       <c r="AU15" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AV15" s="15" t="s">
         <v>2</v>
@@ -4804,7 +4806,7 @@
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
       <c r="I17" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J17" s="45" t="s">
         <v>78</v>
@@ -4959,7 +4961,7 @@
       <c r="R19" s="15"/>
       <c r="S19" s="97"/>
       <c r="T19" s="15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="U19" s="15">
         <v>1</v>
@@ -4971,13 +4973,13 @@
         <v>2</v>
       </c>
       <c r="X19" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Y19" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z19" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AA19" s="15"/>
       <c r="AB19" s="15"/>
@@ -5018,13 +5020,13 @@
         <v>0</v>
       </c>
       <c r="AS19" s="76" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AT19" s="19">
         <v>1</v>
       </c>
       <c r="AU19" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AV19" s="15" t="s">
         <v>2</v>
@@ -5136,7 +5138,7 @@
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
       <c r="T23" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="U23" s="15">
         <v>1</v>
@@ -5148,13 +5150,13 @@
         <v>2</v>
       </c>
       <c r="X23" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Y23" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z23" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AA23" s="15"/>
       <c r="AB23" s="15"/>
@@ -5185,13 +5187,13 @@
         <v>0</v>
       </c>
       <c r="AS23" s="76" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AT23" s="19">
         <v>1</v>
       </c>
       <c r="AU23" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AV23" s="15" t="s">
         <v>2</v>
@@ -5257,7 +5259,7 @@
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
       <c r="I25" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J25" s="45" t="s">
         <v>78</v>
@@ -5414,7 +5416,7 @@
       <c r="R27" s="15"/>
       <c r="S27" s="97"/>
       <c r="T27" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="U27" s="45">
         <v>0.9</v>
@@ -5426,10 +5428,10 @@
         <v>2</v>
       </c>
       <c r="X27" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Y27" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z27" s="15" t="s">
         <v>81</v>
@@ -5459,7 +5461,7 @@
         <v>50</v>
       </c>
       <c r="AO27" s="123" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AP27" s="16" t="b">
         <v>0</v>
@@ -5520,7 +5522,7 @@
         <v>50</v>
       </c>
       <c r="AO28" s="123" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AP28" s="16"/>
       <c r="AQ28" s="16"/>
@@ -5599,7 +5601,7 @@
       <c r="R30" s="15"/>
       <c r="S30" s="97"/>
       <c r="T30" s="15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="U30" s="15">
         <v>1</v>
@@ -5611,13 +5613,13 @@
         <v>2</v>
       </c>
       <c r="X30" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Y30" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z30" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AA30" s="15"/>
       <c r="AB30" s="15"/>
@@ -5658,13 +5660,13 @@
         <v>0</v>
       </c>
       <c r="AS30" s="76" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AT30" s="19">
         <v>1</v>
       </c>
       <c r="AU30" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AV30" s="15" t="s">
         <v>2</v>
@@ -5776,7 +5778,7 @@
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
       <c r="T34" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="U34" s="15">
         <v>1</v>
@@ -5788,13 +5790,13 @@
         <v>2</v>
       </c>
       <c r="X34" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Y34" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z34" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AA34" s="15"/>
       <c r="AB34" s="15"/>
@@ -5825,13 +5827,13 @@
         <v>0</v>
       </c>
       <c r="AS34" s="76" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AT34" s="19">
         <v>1</v>
       </c>
       <c r="AU34" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AV34" s="15" t="s">
         <v>2</v>
@@ -5897,10 +5899,10 @@
       <c r="G36" s="15"/>
       <c r="H36" s="15"/>
       <c r="I36" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J36" s="41" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K36" s="41">
         <v>0</v>
@@ -5946,7 +5948,7 @@
       <c r="AB36" s="15"/>
       <c r="AC36" s="15"/>
       <c r="AD36" s="97" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AE36" s="15"/>
       <c r="AF36" s="15"/>
@@ -5959,7 +5961,7 @@
       <c r="AK36" s="18"/>
       <c r="AL36" s="108"/>
       <c r="AM36" s="84" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AN36" s="19" t="b">
         <v>1</v>
@@ -6091,7 +6093,7 @@
       <c r="AK38" s="18"/>
       <c r="AL38" s="108"/>
       <c r="AM38" s="84" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AN38" s="19" t="b">
         <v>1</v>
@@ -6161,7 +6163,7 @@
       <c r="A40" s="15"/>
       <c r="B40" s="15"/>
       <c r="T40" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="U40" s="15">
         <v>1</v>
@@ -6173,13 +6175,13 @@
         <v>2</v>
       </c>
       <c r="X40" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Y40" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z40" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AA40" s="15"/>
       <c r="AB40" s="15"/>
@@ -6210,13 +6212,13 @@
         <v>0</v>
       </c>
       <c r="AS40" s="76" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AT40" s="19">
         <v>1</v>
       </c>
       <c r="AU40" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AV40" s="15" t="s">
         <v>2</v>
@@ -6282,10 +6284,10 @@
       <c r="G42" s="15"/>
       <c r="H42" s="15"/>
       <c r="I42" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J42" s="41" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K42" s="41">
         <v>0</v>
@@ -6331,7 +6333,7 @@
       <c r="AB42" s="15"/>
       <c r="AC42" s="15"/>
       <c r="AD42" s="97" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AE42" s="15"/>
       <c r="AF42" s="15"/>
@@ -6344,7 +6346,7 @@
       <c r="AK42" s="18"/>
       <c r="AL42" s="108"/>
       <c r="AM42" s="84" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AN42" s="19" t="b">
         <v>1</v>
@@ -6437,7 +6439,7 @@
       <c r="R44" s="15"/>
       <c r="S44" s="97"/>
       <c r="T44" s="45" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="U44" s="15">
         <v>1</v>
@@ -6449,13 +6451,13 @@
         <v>2</v>
       </c>
       <c r="X44" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Y44" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z44" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AA44" s="15"/>
       <c r="AB44" s="15"/>
@@ -6496,13 +6498,13 @@
         <v>0</v>
       </c>
       <c r="AS44" s="76" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AT44" s="19">
         <v>1</v>
       </c>
       <c r="AU44" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AV44" s="15" t="s">
         <v>2</v>
@@ -6614,7 +6616,7 @@
       <c r="A48" s="15"/>
       <c r="B48" s="15"/>
       <c r="T48" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="U48" s="15">
         <v>1</v>
@@ -6626,13 +6628,13 @@
         <v>2</v>
       </c>
       <c r="X48" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Y48" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z48" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AA48" s="15"/>
       <c r="AB48" s="15"/>
@@ -6663,13 +6665,13 @@
         <v>0</v>
       </c>
       <c r="AS48" s="76" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AT48" s="19">
         <v>1</v>
       </c>
       <c r="AU48" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AV48" s="15" t="s">
         <v>2</v>
@@ -6735,10 +6737,10 @@
       <c r="G50" s="15"/>
       <c r="H50" s="15"/>
       <c r="I50" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J50" s="41" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K50" s="41">
         <v>0</v>
@@ -6784,7 +6786,7 @@
       <c r="AB50" s="15"/>
       <c r="AC50" s="15"/>
       <c r="AD50" s="97" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AE50" s="15"/>
       <c r="AF50" s="15"/>
@@ -6873,7 +6875,7 @@
       <c r="A52" s="15"/>
       <c r="B52" s="15"/>
       <c r="T52" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="U52" s="15">
         <v>1</v>
@@ -6885,13 +6887,13 @@
         <v>2</v>
       </c>
       <c r="X52" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Y52" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z52" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AA52" s="15"/>
       <c r="AB52" s="15"/>
@@ -6922,13 +6924,13 @@
         <v>0</v>
       </c>
       <c r="AS52" s="76" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AT52" s="19">
         <v>1</v>
       </c>
       <c r="AU52" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AV52" s="15" t="s">
         <v>2</v>
@@ -6994,7 +6996,7 @@
       <c r="G54" s="15"/>
       <c r="H54" s="15"/>
       <c r="I54" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J54" s="41" t="s">
         <v>78</v>
@@ -7163,7 +7165,7 @@
       <c r="R56" s="15"/>
       <c r="S56" s="97"/>
       <c r="T56" s="15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="U56" s="15">
         <v>1</v>
@@ -7175,13 +7177,13 @@
         <v>2</v>
       </c>
       <c r="X56" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Y56" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z56" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AA56" s="15"/>
       <c r="AB56" s="15"/>
@@ -7222,13 +7224,13 @@
         <v>0</v>
       </c>
       <c r="AS56" s="76" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AT56" s="19">
         <v>1</v>
       </c>
       <c r="AU56" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AV56" s="15" t="s">
         <v>2</v>
@@ -7340,7 +7342,7 @@
       <c r="A60" s="15"/>
       <c r="B60" s="15"/>
       <c r="T60" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="U60" s="15">
         <v>1</v>
@@ -7352,13 +7354,13 @@
         <v>2</v>
       </c>
       <c r="X60" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Y60" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z60" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AA60" s="15"/>
       <c r="AB60" s="15"/>
@@ -7389,13 +7391,13 @@
         <v>0</v>
       </c>
       <c r="AS60" s="76" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AT60" s="19">
         <v>1</v>
       </c>
       <c r="AU60" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AV60" s="15" t="s">
         <v>2</v>
@@ -7456,20 +7458,20 @@
       <c r="B62" s="15"/>
       <c r="C62" s="41"/>
       <c r="D62" s="99" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E62" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F62" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G62" s="15" t="b">
         <v>0</v>
       </c>
       <c r="H62" s="15"/>
       <c r="I62" s="42" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J62" s="41" t="s">
         <v>78</v>
@@ -7490,7 +7492,7 @@
         <v>10</v>
       </c>
       <c r="P62" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="Q62" s="15"/>
       <c r="R62" s="15"/>
@@ -7626,7 +7628,7 @@
       <c r="R64" s="15"/>
       <c r="S64" s="97"/>
       <c r="T64" s="45" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="U64" s="15">
         <v>1</v>
@@ -7638,13 +7640,13 @@
         <v>2</v>
       </c>
       <c r="X64" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Y64" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z64" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AA64" s="15"/>
       <c r="AB64" s="15"/>
@@ -7685,13 +7687,13 @@
         <v>0</v>
       </c>
       <c r="AS64" s="76" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AT64" s="19">
         <v>1</v>
       </c>
       <c r="AU64" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AV64" s="15" t="s">
         <v>2</v>
@@ -7838,7 +7840,7 @@
       <c r="R68" s="15"/>
       <c r="S68" s="97"/>
       <c r="T68" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="U68" s="15">
         <v>1</v>
@@ -7850,13 +7852,13 @@
         <v>69</v>
       </c>
       <c r="X68" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Y68" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z68" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AA68" s="15"/>
       <c r="AB68" s="15"/>
@@ -7887,13 +7889,13 @@
         <v>0</v>
       </c>
       <c r="AS68" s="76" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AT68" s="19">
         <v>1</v>
       </c>
       <c r="AU68" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AV68" s="15" t="s">
         <v>2</v>
@@ -7954,20 +7956,20 @@
       <c r="B70" s="15"/>
       <c r="C70" s="41"/>
       <c r="D70" s="99" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E70" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F70" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G70" s="15" t="b">
         <v>0</v>
       </c>
       <c r="H70" s="15"/>
       <c r="I70" s="15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J70" s="41" t="s">
         <v>78</v>
@@ -8126,7 +8128,7 @@
       <c r="R72" s="15"/>
       <c r="S72" s="97"/>
       <c r="T72" s="45" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="U72" s="15">
         <v>1</v>
@@ -8138,13 +8140,13 @@
         <v>2</v>
       </c>
       <c r="X72" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Y72" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z72" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AA72" s="15"/>
       <c r="AB72" s="15"/>
@@ -8185,13 +8187,13 @@
         <v>0</v>
       </c>
       <c r="AS72" s="76" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AT72" s="19">
         <v>1</v>
       </c>
       <c r="AU72" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AV72" s="15" t="s">
         <v>2</v>
@@ -8338,7 +8340,7 @@
       <c r="R76" s="15"/>
       <c r="S76" s="97"/>
       <c r="T76" s="45" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="U76" s="15">
         <v>1</v>
@@ -8350,13 +8352,13 @@
         <v>69</v>
       </c>
       <c r="X76" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Y76" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z76" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AA76" s="15"/>
       <c r="AB76" s="15"/>
@@ -8387,13 +8389,13 @@
         <v>0</v>
       </c>
       <c r="AS76" s="76" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AT76" s="19">
         <v>1</v>
       </c>
       <c r="AU76" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AV76" s="15" t="s">
         <v>2</v>
@@ -8454,16 +8456,16 @@
       <c r="B78" s="15"/>
       <c r="C78" s="15"/>
       <c r="D78" s="97" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E78" s="15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F78" s="15"/>
       <c r="G78" s="15"/>
       <c r="H78" s="15"/>
       <c r="I78" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J78" s="15" t="s">
         <v>78</v>
@@ -8484,13 +8486,13 @@
         <v>10</v>
       </c>
       <c r="P78" s="15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="Q78" s="15"/>
       <c r="R78" s="15"/>
       <c r="S78" s="97"/>
       <c r="T78" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="U78" s="15">
         <v>0.9</v>
@@ -8502,10 +8504,10 @@
         <v>2</v>
       </c>
       <c r="X78" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="Y78" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z78" s="15"/>
       <c r="AA78" s="15"/>
@@ -8514,7 +8516,7 @@
         <v>6</v>
       </c>
       <c r="AD78" s="97" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="AE78" s="15" t="s">
         <v>84</v>
@@ -8545,7 +8547,7 @@
         <v>50</v>
       </c>
       <c r="AO78" s="120" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AP78" s="16"/>
       <c r="AQ78" s="16"/>
@@ -8557,7 +8559,7 @@
         <v>50</v>
       </c>
       <c r="AU78" s="16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="AV78" s="15"/>
     </row>
@@ -8567,7 +8569,7 @@
       <c r="C79" s="15"/>
       <c r="D79" s="97"/>
       <c r="E79" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F79" s="15"/>
       <c r="G79" s="15"/>
@@ -8609,7 +8611,7 @@
         <v>170</v>
       </c>
       <c r="AO79" s="120" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AP79" s="16"/>
       <c r="AQ79" s="16"/>
@@ -8621,7 +8623,7 @@
         <v>50</v>
       </c>
       <c r="AU79" s="16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="AV79" s="15"/>
     </row>
@@ -9044,39 +9046,39 @@
     <row r="2" spans="1:20">
       <c r="J2" s="1"/>
       <c r="Q2" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="R2" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="S2" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="R2" s="27" t="s">
+      <c r="T2" s="27" t="s">
         <v>128</v>
-      </c>
-      <c r="S2" s="27" t="s">
-        <v>129</v>
-      </c>
-      <c r="T2" s="27" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" t="s">
         <v>131</v>
-      </c>
-      <c r="C3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D3" t="s">
-        <v>133</v>
       </c>
       <c r="Q3" s="28"/>
     </row>
     <row r="4" spans="1:20">
       <c r="B4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="Q4" s="29" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="R4" s="29"/>
       <c r="S4" s="29"/>
@@ -9084,7 +9086,7 @@
     </row>
     <row r="5" spans="1:20">
       <c r="B5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="Q5" s="29"/>
       <c r="R5" s="30" t="s">
@@ -9095,7 +9097,7 @@
     </row>
     <row r="6" spans="1:20">
       <c r="B6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="Q6" s="31"/>
       <c r="R6" s="31"/>
@@ -9106,72 +9108,72 @@
     </row>
     <row r="7" spans="1:20">
       <c r="B7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="T7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="T8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="T9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="T10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="T11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="Q12" s="31"/>
       <c r="R12" s="31"/>
       <c r="S12" s="31" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="T12" s="31"/>
     </row>
     <row r="13" spans="1:20">
       <c r="T13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="Q14" s="31"/>
       <c r="R14" s="31"/>
       <c r="S14" s="31" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="T14" s="31"/>
     </row>
     <row r="15" spans="1:20">
       <c r="T15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="T16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="17:20">
       <c r="T17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="17:20">
       <c r="Q18" s="29"/>
       <c r="R18" s="30" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="S18" s="29"/>
       <c r="T18" s="29"/>
@@ -9180,85 +9182,85 @@
       <c r="Q19" s="31"/>
       <c r="R19" s="31"/>
       <c r="S19" s="31" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="T19" s="31"/>
     </row>
     <row r="20" spans="17:20">
       <c r="T20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="17:20">
       <c r="Q21" s="28"/>
       <c r="S21" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="17:20">
       <c r="Q22" s="28"/>
       <c r="T22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="17:20">
       <c r="Q23" s="28"/>
       <c r="S23" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="17:20">
       <c r="Q24" s="28"/>
       <c r="T24" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="17:20">
       <c r="Q25" s="28"/>
       <c r="T25" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="17:20">
       <c r="Q26" s="28"/>
       <c r="S26" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="17:20">
       <c r="Q27" s="28"/>
       <c r="S27" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="17:20">
       <c r="Q28" s="28"/>
       <c r="T28" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="17:20">
       <c r="Q29" s="28"/>
       <c r="S29" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="17:20">
       <c r="Q30" s="28"/>
       <c r="T30" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="31" spans="17:20">
       <c r="Q31" s="28"/>
       <c r="T31" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="17:20">
       <c r="Q32" s="29"/>
       <c r="R32" s="30" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="S32" s="29"/>
       <c r="T32" s="29"/>
@@ -9267,34 +9269,34 @@
       <c r="Q33" s="31"/>
       <c r="R33" s="31"/>
       <c r="S33" s="31" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="T33" s="31"/>
     </row>
     <row r="34" spans="17:20">
       <c r="Q34" s="28"/>
       <c r="T34" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="17:20">
       <c r="Q35" s="31"/>
       <c r="R35" s="31"/>
       <c r="S35" s="31" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="T35" s="31"/>
     </row>
     <row r="36" spans="17:20">
       <c r="Q36" s="28"/>
       <c r="T36" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="17:20">
       <c r="Q37" s="29"/>
       <c r="R37" s="30" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="S37" s="29"/>
       <c r="T37" s="29"/>
@@ -9303,28 +9305,28 @@
       <c r="Q38" s="31"/>
       <c r="R38" s="31"/>
       <c r="S38" s="31" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="T38" s="31"/>
     </row>
     <row r="39" spans="17:20">
       <c r="Q39" s="28"/>
       <c r="T39" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="40" spans="17:20">
       <c r="Q40" s="31"/>
       <c r="R40" s="31"/>
       <c r="S40" s="31" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="T40" s="31"/>
     </row>
     <row r="41" spans="17:20">
       <c r="Q41" s="28"/>
       <c r="T41" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -9365,7 +9367,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
       <c r="H1" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -9391,12 +9393,12 @@
         <v>15</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B3">
         <v>50</v>
@@ -9436,10 +9438,10 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -9448,12 +9450,12 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B6">
         <v>50</v>
@@ -9465,18 +9467,18 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H7" t="s">
         <v>38</v>
@@ -9484,7 +9486,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B8">
         <v>80</v>
@@ -9510,7 +9512,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E9" t="s">
         <v>78</v>
@@ -9521,7 +9523,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E10" t="s">
         <v>78</v>
@@ -9532,7 +9534,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B11" s="42"/>
       <c r="C11" s="42"/>
@@ -9540,7 +9542,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B12">
         <v>1000</v>
@@ -9561,13 +9563,13 @@
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J12" s="45"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F13">
         <v>25</v>
@@ -9575,22 +9577,22 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="42" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B19">
         <v>50</v>
@@ -9602,15 +9604,15 @@
         <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H19" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B20">
         <v>50</v>
@@ -9622,10 +9624,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H20" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -9651,10 +9653,10 @@
   <sheetData>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
@@ -9668,7 +9670,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -9693,10 +9695,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="B5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -9705,15 +9707,15 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="B6" t="s">
-        <v>86</v>
+        <v>186</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>187</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -9727,7 +9729,7 @@
         <v>189</v>
       </c>
       <c r="B7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -9735,7 +9737,7 @@
         <v>190</v>
       </c>
       <c r="B8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -9743,10 +9745,10 @@
         <v>191</v>
       </c>
       <c r="B9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -9826,7 +9828,7 @@
       <c r="Y1" s="24"/>
       <c r="Z1" s="52"/>
       <c r="AA1" s="21" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AB1" s="21"/>
       <c r="AC1" s="21"/>
@@ -9880,7 +9882,7 @@
       <c r="AC2" s="21"/>
       <c r="AD2" s="49"/>
       <c r="AE2" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AF2" s="4"/>
       <c r="AG2" s="4"/>
@@ -10015,7 +10017,7 @@
         <v>5</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M4" s="15" t="s">
         <v>82</v>
@@ -10078,7 +10080,7 @@
     </row>
     <row r="6" spans="1:35" s="15" customFormat="1">
       <c r="C6" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E6" s="15">
         <v>0.9</v>
@@ -10090,13 +10092,13 @@
         <v>69</v>
       </c>
       <c r="H6" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="I6" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="I6" s="15" t="s">
-        <v>91</v>
-      </c>
       <c r="L6" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="Q6" s="16" t="b">
         <v>1</v>
@@ -10117,7 +10119,7 @@
         <v>50</v>
       </c>
       <c r="Y6" s="19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Z6" s="53"/>
       <c r="AA6" s="16" t="b">
@@ -10150,7 +10152,7 @@
         <v>50</v>
       </c>
       <c r="Y7" s="19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Z7" s="53"/>
       <c r="AA7" s="16" t="b">
@@ -10196,10 +10198,10 @@
         <v>69</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="L9" s="15" t="s">
         <v>6</v>
@@ -10237,13 +10239,13 @@
       </c>
       <c r="AD9" s="50"/>
       <c r="AE9" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AF9" s="15">
         <v>1</v>
       </c>
       <c r="AG9" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AH9" s="15" t="s">
         <v>2</v>
@@ -10379,42 +10381,42 @@
       <c r="U15" s="18"/>
       <c r="V15" s="50"/>
       <c r="W15" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="X15" s="18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Y15" s="18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Z15" s="50"/>
       <c r="AA15" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AB15" s="18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AC15" s="18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AD15" s="50"/>
       <c r="AE15" s="18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AF15" s="18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AG15" s="18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AH15" s="18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AI15" s="47"/>
     </row>
     <row r="16" spans="1:35" s="15" customFormat="1">
       <c r="C16" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E16" s="15">
         <v>0.9</v>
@@ -10426,7 +10428,7 @@
         <v>54</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Q16" s="16" t="b">
         <v>1</v>
@@ -10447,7 +10449,7 @@
         <v>50</v>
       </c>
       <c r="Y16" s="19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Z16" s="53"/>
       <c r="AA16" s="16" t="b">
@@ -10461,16 +10463,16 @@
       </c>
       <c r="AD16" s="50"/>
       <c r="AE16" s="18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AF16" s="18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AG16" s="18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AH16" s="18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AI16" s="47"/>
     </row>
@@ -10488,7 +10490,7 @@
         <v>50</v>
       </c>
       <c r="Y17" s="19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Z17" s="53"/>
       <c r="AA17" s="16" t="b">
@@ -10517,7 +10519,7 @@
         <v>2</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Q18" s="16" t="b">
         <v>1</v>
@@ -10629,7 +10631,7 @@
         <v>2</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Q21" s="15" t="s">
         <v>198</v>
@@ -10642,23 +10644,23 @@
       </c>
       <c r="V21" s="47"/>
       <c r="W21" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="X21" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Y21" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Z21" s="47"/>
       <c r="AA21" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AB21" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AC21" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AD21" s="47"/>
       <c r="AE21"/>
@@ -10685,7 +10687,7 @@
     </row>
     <row r="23" spans="1:35" s="15" customFormat="1">
       <c r="C23" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E23" s="15">
         <v>0.9</v>
@@ -10697,13 +10699,13 @@
         <v>2</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="L23" s="15" t="s">
         <v>6</v>
       </c>
       <c r="M23" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="N23" s="15" t="s">
         <v>84</v>
@@ -10735,17 +10737,17 @@
         <v>50</v>
       </c>
       <c r="Y23" s="19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Z23" s="53"/>
       <c r="AA23" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AB23" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AC23" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AD23" s="50"/>
       <c r="AE23" s="16" t="s">
@@ -10755,7 +10757,7 @@
         <v>50</v>
       </c>
       <c r="AG23" s="16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="AI23" s="47"/>
     </row>
@@ -10773,17 +10775,17 @@
         <v>170</v>
       </c>
       <c r="Y24" s="19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Z24" s="53"/>
       <c r="AA24" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AB24" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AC24" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AD24" s="50"/>
       <c r="AE24" s="16" t="s">
@@ -10793,7 +10795,7 @@
         <v>50</v>
       </c>
       <c r="AG24" s="16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="AI24" s="47"/>
     </row>
@@ -10938,7 +10940,7 @@
   <sheetData>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>204</v>
@@ -10964,10 +10966,10 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C3" t="s">
         <v>79</v>
@@ -10976,7 +10978,7 @@
         <v>208</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F3">
         <v>50</v>
@@ -10984,13 +10986,13 @@
     </row>
     <row r="4" spans="1:8">
       <c r="C4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D4" t="s">
         <v>208</v>
       </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -11049,7 +11051,7 @@
         <v>208</v>
       </c>
       <c r="E9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F9">
         <v>3500</v>
@@ -11057,7 +11059,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>204</v>
@@ -11077,10 +11079,10 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C13" t="s">
         <v>79</v>
@@ -11089,7 +11091,7 @@
         <v>208</v>
       </c>
       <c r="E13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F13">
         <v>50</v>
@@ -11100,13 +11102,13 @@
     </row>
     <row r="14" spans="1:8">
       <c r="C14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D14" t="s">
         <v>208</v>
       </c>
       <c r="E14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F14">
         <v>36</v>
@@ -11114,7 +11116,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="C15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -11128,13 +11130,13 @@
     </row>
     <row r="16" spans="1:8">
       <c r="C16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D16">
         <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F16">
         <v>7000</v>

</xml_diff>

<commit_message>
changes to indicator ec
</commit_message>
<xml_diff>
--- a/data/inputs/Asset Model - Demo.xlsx
+++ b/data/inputs/Asset Model - Demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtreseder\OneDrive - KPMG\Documents\3. Client\Essential Energy\Probability of Failure Model\pof\data\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1949" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B7286B10-D206-4ACE-911C-2D5093702859}"/>
+  <xr:revisionPtr revIDLastSave="1964" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2DF6B453-F960-457F-A376-03248CAF50C6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1196,7 +1196,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1286,8 +1286,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="22">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1411,6 +1418,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA6A6A6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -1457,7 +1470,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1720,6 +1733,21 @@
     <xf numFmtId="0" fontId="11" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="2" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -3559,8 +3587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA0734F-FFBE-4DAF-BDE5-A12359370A0D}">
   <dimension ref="A1:AV80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AO46" sqref="AO46"/>
+    <sheetView tabSelected="1" topLeftCell="S14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AQ39" sqref="AQ39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>
@@ -5887,9 +5915,11 @@
       <c r="AM36" s="84"/>
       <c r="AN36" s="19"/>
       <c r="AO36" s="120"/>
-      <c r="AP36" s="44"/>
-      <c r="AQ36" s="44"/>
-      <c r="AR36" s="106"/>
+      <c r="AP36" s="145"/>
+      <c r="AQ36" s="145" t="b">
+        <v>1</v>
+      </c>
+      <c r="AR36" s="146"/>
       <c r="AS36" s="76"/>
       <c r="AT36" s="19"/>
       <c r="AU36" s="15"/>
@@ -5935,12 +5965,12 @@
       <c r="AK37" s="70"/>
       <c r="AL37" s="109"/>
       <c r="AM37" s="83"/>
-      <c r="AN37" s="68"/>
-      <c r="AO37" s="117"/>
-      <c r="AP37" s="44"/>
-      <c r="AQ37" s="44"/>
-      <c r="AR37" s="106"/>
-      <c r="AS37" s="75"/>
+      <c r="AN37" s="140"/>
+      <c r="AO37" s="141"/>
+      <c r="AP37" s="142"/>
+      <c r="AQ37" s="142"/>
+      <c r="AR37" s="143"/>
+      <c r="AS37" s="144"/>
       <c r="AT37" s="71"/>
       <c r="AU37" s="69"/>
       <c r="AV37" s="69"/>
@@ -6013,9 +6043,11 @@
       <c r="AM38" s="84"/>
       <c r="AN38" s="19"/>
       <c r="AO38" s="120"/>
-      <c r="AP38" s="44"/>
-      <c r="AQ38" s="44"/>
-      <c r="AR38" s="106"/>
+      <c r="AP38" s="145"/>
+      <c r="AQ38" s="145" t="b">
+        <v>1</v>
+      </c>
+      <c r="AR38" s="146"/>
       <c r="AS38" s="74"/>
       <c r="AT38" s="93"/>
       <c r="AU38" s="18"/>

</xml_diff>

<commit_message>
t_initiate + 1 line 489
</commit_message>
<xml_diff>
--- a/data/inputs/Asset Model - Demo.xlsx
+++ b/data/inputs/Asset Model - Demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtreseder\OneDrive - KPMG\Documents\3. Client\Essential Energy\Probability of Failure Model\pof\data\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2055" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CD023BF1-A62D-425C-BEAB-B554A9A5ACCF}"/>
+  <xr:revisionPtr revIDLastSave="2058" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4901E195-3075-42E8-A283-6C44F9564FBB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3516,8 +3516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA0734F-FFBE-4DAF-BDE5-A12359370A0D}">
   <dimension ref="A1:AV80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z3" sqref="Z3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>

</xml_diff>

<commit_message>
dash locking concept working
</commit_message>
<xml_diff>
--- a/data/inputs/Asset Model - Demo.xlsx
+++ b/data/inputs/Asset Model - Demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtreseder\OneDrive - KPMG\Documents\3. Client\Essential Energy\Probability of Failure Model\pof\data\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2058" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4901E195-3075-42E8-A283-6C44F9564FBB}"/>
+  <xr:revisionPtr revIDLastSave="2062" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FD84132D-7C7C-48AA-B4FC-3E87A9F3210B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3517,7 +3517,10 @@
   <dimension ref="A1:AV80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>
@@ -5802,7 +5805,7 @@
         <v>1.5</v>
       </c>
       <c r="O36" s="132">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P36" s="94"/>
       <c r="Q36" s="41"/>
@@ -6183,7 +6186,7 @@
         <v>1.5</v>
       </c>
       <c r="O42" s="132">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P42" s="15"/>
       <c r="Q42" s="15"/>
@@ -6423,7 +6426,7 @@
         <v>1.5</v>
       </c>
       <c r="O46" s="132">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P46" s="15"/>
       <c r="Q46" s="15"/>

</xml_diff>